<commit_message>
Add OrgUnit description to xls
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4409" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4501" uniqueCount="986">
   <si>
     <t>DATA</t>
   </si>
@@ -3014,13 +3014,109 @@
   </si>
   <si>
     <t>GenerateViewCollection</t>
+  </si>
+  <si>
+    <t>ORG_ORGANIZATIONAL_UNIT</t>
+  </si>
+  <si>
+    <t>ORG_NUMBER</t>
+  </si>
+  <si>
+    <t>ABBR</t>
+  </si>
+  <si>
+    <t>LOCATION_ABBR</t>
+  </si>
+  <si>
+    <t>SYS_LOCATION_ID</t>
+  </si>
+  <si>
+    <t>ORG_TYPE_ID</t>
+  </si>
+  <si>
+    <t>EMAIL_FROM</t>
+  </si>
+  <si>
+    <t>EMAIL_TO</t>
+  </si>
+  <si>
+    <t>IS_EGDOK_PRINT_ALWAYS</t>
+  </si>
+  <si>
+    <t>OE-Nummer</t>
+  </si>
+  <si>
+    <t>Org Number</t>
+  </si>
+  <si>
+    <t>OE-Bezeichnung</t>
+  </si>
+  <si>
+    <t>OE-Kürzel</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Angabe, ob EGDok-Dokumente für diese OE auch bei negativem Ergebnis gedruckt werden können</t>
+  </si>
+  <si>
+    <t>Location abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OE-Typ </t>
+  </si>
+  <si>
+    <t>Org type</t>
+  </si>
+  <si>
+    <t>Email from</t>
+  </si>
+  <si>
+    <t>Email to</t>
+  </si>
+  <si>
+    <t>Email von</t>
+  </si>
+  <si>
+    <t>Email bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standortcode </t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>EGDok print always</t>
+  </si>
+  <si>
+    <t>Standortcode-Kürzel</t>
+  </si>
+  <si>
+    <t>SysLocation</t>
+  </si>
+  <si>
+    <t>OrgType</t>
+  </si>
+  <si>
+    <t>OrgAccountingArea</t>
+  </si>
+  <si>
+    <t>OrgAccountingArea,OrgType,SysLocation</t>
+  </si>
+  <si>
+    <t>Organisationseinheit</t>
+  </si>
+  <si>
+    <t>Organizational unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3053,6 +3149,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3115,7 +3219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3137,6 +3241,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3432,13 +3540,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T98"/>
+  <dimension ref="A1:T99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomRight" activeCell="N100" sqref="N100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6161,6 +6269,35 @@
         <v>147</v>
       </c>
     </row>
+    <row r="99" spans="1:14">
+      <c r="A99" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" t="s">
+        <v>954</v>
+      </c>
+      <c r="C99" t="s">
+        <v>152</v>
+      </c>
+      <c r="D99" t="s">
+        <v>160</v>
+      </c>
+      <c r="E99" t="s">
+        <v>785</v>
+      </c>
+      <c r="J99" t="s">
+        <v>983</v>
+      </c>
+      <c r="K99" t="s">
+        <v>984</v>
+      </c>
+      <c r="L99" t="s">
+        <v>985</v>
+      </c>
+      <c r="N99" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L98">
     <filterColumn colId="1"/>
@@ -6187,10 +6324,10 @@
   <dimension ref="A1:I554"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G467" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
+      <selection pane="bottomRight" activeCell="I478" sqref="I478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17495,7 +17632,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="465" spans="1:8">
+    <row r="465" spans="1:9">
       <c r="A465" t="s">
         <v>153</v>
       </c>
@@ -17518,7 +17655,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="466" spans="1:8">
+    <row r="466" spans="1:9">
       <c r="A466" t="s">
         <v>153</v>
       </c>
@@ -17544,7 +17681,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="467" spans="1:8">
+    <row r="467" spans="1:9">
       <c r="A467" t="s">
         <v>153</v>
       </c>
@@ -17570,7 +17707,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="468" spans="1:8">
+    <row r="468" spans="1:9">
       <c r="A468" t="s">
         <v>153</v>
       </c>
@@ -17593,7 +17730,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="469" spans="1:8">
+    <row r="469" spans="1:9">
       <c r="A469" t="s">
         <v>153</v>
       </c>
@@ -17619,7 +17756,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="470" spans="1:8">
+    <row r="470" spans="1:9">
       <c r="A470" t="s">
         <v>153</v>
       </c>
@@ -17645,7 +17782,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="471" spans="1:8">
+    <row r="471" spans="1:9">
       <c r="A471" t="s">
         <v>153</v>
       </c>
@@ -17671,7 +17808,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="472" spans="1:8">
+    <row r="472" spans="1:9">
       <c r="A472" t="s">
         <v>153</v>
       </c>
@@ -17694,7 +17831,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="473" spans="1:8">
+    <row r="473" spans="1:9">
       <c r="A473" t="s">
         <v>153</v>
       </c>
@@ -17715,6 +17852,279 @@
       </c>
       <c r="H473" s="7" t="s">
         <v>636</v>
+      </c>
+    </row>
+    <row r="474" spans="1:9" ht="15.75">
+      <c r="A474" t="s">
+        <v>153</v>
+      </c>
+      <c r="B474" t="s">
+        <v>954</v>
+      </c>
+      <c r="C474" t="s">
+        <v>955</v>
+      </c>
+      <c r="D474" t="s">
+        <v>147</v>
+      </c>
+      <c r="E474" t="s">
+        <v>147</v>
+      </c>
+      <c r="F474" t="s">
+        <v>147</v>
+      </c>
+      <c r="G474" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="H474" s="7" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="475" spans="1:9" ht="15.75">
+      <c r="A475" t="s">
+        <v>153</v>
+      </c>
+      <c r="B475" t="s">
+        <v>954</v>
+      </c>
+      <c r="C475" t="s">
+        <v>12</v>
+      </c>
+      <c r="D475" t="s">
+        <v>147</v>
+      </c>
+      <c r="G475" s="12" t="s">
+        <v>965</v>
+      </c>
+      <c r="H475" s="7" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9" ht="15.75">
+      <c r="A476" t="s">
+        <v>153</v>
+      </c>
+      <c r="B476" t="s">
+        <v>954</v>
+      </c>
+      <c r="C476" t="s">
+        <v>956</v>
+      </c>
+      <c r="D476" t="s">
+        <v>147</v>
+      </c>
+      <c r="G476" s="12" t="s">
+        <v>966</v>
+      </c>
+      <c r="H476" s="7" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9">
+      <c r="A477" t="s">
+        <v>153</v>
+      </c>
+      <c r="B477" t="s">
+        <v>954</v>
+      </c>
+      <c r="C477" t="s">
+        <v>957</v>
+      </c>
+      <c r="D477" t="s">
+        <v>147</v>
+      </c>
+      <c r="G477" s="7" t="s">
+        <v>979</v>
+      </c>
+      <c r="H477" s="7" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="478" spans="1:9" ht="15.75">
+      <c r="A478" t="s">
+        <v>153</v>
+      </c>
+      <c r="B478" t="s">
+        <v>954</v>
+      </c>
+      <c r="C478" t="s">
+        <v>958</v>
+      </c>
+      <c r="D478" t="s">
+        <v>147</v>
+      </c>
+      <c r="G478" s="12" t="s">
+        <v>976</v>
+      </c>
+      <c r="H478" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="I478" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="479" spans="1:9" ht="15.75">
+      <c r="A479" t="s">
+        <v>153</v>
+      </c>
+      <c r="B479" t="s">
+        <v>954</v>
+      </c>
+      <c r="C479" t="s">
+        <v>959</v>
+      </c>
+      <c r="D479" t="s">
+        <v>147</v>
+      </c>
+      <c r="F479" t="s">
+        <v>147</v>
+      </c>
+      <c r="G479" s="12" t="s">
+        <v>970</v>
+      </c>
+      <c r="H479" s="7" t="s">
+        <v>971</v>
+      </c>
+      <c r="I479" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="480" spans="1:9">
+      <c r="A480" t="s">
+        <v>153</v>
+      </c>
+      <c r="B480" t="s">
+        <v>954</v>
+      </c>
+      <c r="C480" t="s">
+        <v>960</v>
+      </c>
+      <c r="D480" t="s">
+        <v>147</v>
+      </c>
+      <c r="G480" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="H480" s="7" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="481" spans="1:9">
+      <c r="A481" t="s">
+        <v>153</v>
+      </c>
+      <c r="B481" t="s">
+        <v>954</v>
+      </c>
+      <c r="C481" t="s">
+        <v>961</v>
+      </c>
+      <c r="D481" t="s">
+        <v>147</v>
+      </c>
+      <c r="G481" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="H481" s="7" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9" ht="47.25">
+      <c r="A482" t="s">
+        <v>153</v>
+      </c>
+      <c r="B482" t="s">
+        <v>954</v>
+      </c>
+      <c r="C482" t="s">
+        <v>962</v>
+      </c>
+      <c r="D482" t="s">
+        <v>147</v>
+      </c>
+      <c r="F482" t="s">
+        <v>147</v>
+      </c>
+      <c r="G482" s="13" t="s">
+        <v>968</v>
+      </c>
+      <c r="H482" s="7" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9" ht="15.75">
+      <c r="A483" t="s">
+        <v>153</v>
+      </c>
+      <c r="B483" t="s">
+        <v>954</v>
+      </c>
+      <c r="C483" t="s">
+        <v>499</v>
+      </c>
+      <c r="D483" t="s">
+        <v>147</v>
+      </c>
+      <c r="G483" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="H483" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I483" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9">
+      <c r="A484" t="s">
+        <v>153</v>
+      </c>
+      <c r="B484" t="s">
+        <v>954</v>
+      </c>
+      <c r="C484" t="s">
+        <v>903</v>
+      </c>
+      <c r="D484" t="s">
+        <v>147</v>
+      </c>
+      <c r="E484" t="s">
+        <v>147</v>
+      </c>
+      <c r="F484" t="s">
+        <v>147</v>
+      </c>
+      <c r="G484" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H484" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9">
+      <c r="A485" t="s">
+        <v>153</v>
+      </c>
+      <c r="B485" t="s">
+        <v>954</v>
+      </c>
+      <c r="C485" t="s">
+        <v>904</v>
+      </c>
+      <c r="D485" t="s">
+        <v>147</v>
+      </c>
+      <c r="E485" t="s">
+        <v>147</v>
+      </c>
+      <c r="F485" t="s">
+        <v>147</v>
+      </c>
+      <c r="G485" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="H485" s="7" t="s">
+        <v>908</v>
       </c>
     </row>
     <row r="554" ht="16.5" customHeight="1"/>

</xml_diff>

<commit_message>
add relationships views for fe
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4521" uniqueCount="995">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4551" uniqueCount="1013">
   <si>
     <t>DATA</t>
   </si>
@@ -3137,6 +3137,60 @@
   </si>
   <si>
     <t>OrdFederalState</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/ExamConstraintExamClasses</t>
+  </si>
+  <si>
+    <t>examClasses</t>
+  </si>
+  <si>
+    <t>Klassen</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>OrdFederalState,ExamRecognitionType</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/ExamStationExamRecognitionTypes</t>
+  </si>
+  <si>
+    <t>examRecognitionTypes</t>
+  </si>
+  <si>
+    <t>Anerkennungen</t>
+  </si>
+  <si>
+    <t>Recognitions</t>
+  </si>
+  <si>
+    <t>examRecognitionType</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/ExamRecognitionTypeExamClasses</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/MeetingPointOrganizationalUnits</t>
+  </si>
+  <si>
+    <t>Org. units</t>
+  </si>
+  <si>
+    <t>organizationalUnits</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/HolidayOrdFederalStates</t>
+  </si>
+  <si>
+    <t>federalStates</t>
+  </si>
+  <si>
+    <t>Bundesländer</t>
+  </si>
+  <si>
+    <t>Federalstates</t>
   </si>
 </sst>
 </file>
@@ -3569,11 +3623,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="P14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3940,6 +3994,9 @@
       <c r="C11" t="s">
         <v>151</v>
       </c>
+      <c r="J11" t="s">
+        <v>991</v>
+      </c>
       <c r="K11" t="s">
         <v>114</v>
       </c>
@@ -3948,6 +4005,18 @@
       </c>
       <c r="N11" t="s">
         <v>147</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="P11" t="s">
+        <v>996</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>998</v>
       </c>
       <c r="S11" t="s">
         <v>789</v>
@@ -4015,6 +4084,9 @@
       <c r="C14" t="s">
         <v>151</v>
       </c>
+      <c r="J14" t="s">
+        <v>991</v>
+      </c>
       <c r="K14" t="s">
         <v>119</v>
       </c>
@@ -4024,8 +4096,23 @@
       <c r="N14" t="s">
         <v>147</v>
       </c>
+      <c r="O14" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="P14" t="s">
+        <v>996</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>998</v>
+      </c>
       <c r="S14" t="s">
         <v>789</v>
+      </c>
+      <c r="T14" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -4048,7 +4135,7 @@
         <v>43</v>
       </c>
       <c r="J15" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="K15" t="s">
         <v>121</v>
@@ -4094,7 +4181,7 @@
         <v>151</v>
       </c>
       <c r="J17" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="K17" t="s">
         <v>125</v>
@@ -4104,6 +4191,18 @@
       </c>
       <c r="N17" t="s">
         <v>147</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>1003</v>
       </c>
       <c r="S17" t="s">
         <v>934</v>
@@ -4148,6 +4247,9 @@
       <c r="C19" t="s">
         <v>151</v>
       </c>
+      <c r="J19" t="s">
+        <v>994</v>
+      </c>
       <c r="K19" t="s">
         <v>129</v>
       </c>
@@ -4156,6 +4258,18 @@
       </c>
       <c r="N19" t="s">
         <v>147</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>1012</v>
       </c>
       <c r="S19" t="s">
         <v>789</v>
@@ -4255,6 +4369,9 @@
       <c r="C23" t="s">
         <v>151</v>
       </c>
+      <c r="J23" t="s">
+        <v>988</v>
+      </c>
       <c r="K23" t="s">
         <v>137</v>
       </c>
@@ -4263,6 +4380,18 @@
       </c>
       <c r="N23" t="s">
         <v>147</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>213</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>1007</v>
       </c>
       <c r="S23" t="s">
         <v>789</v>
@@ -6392,11 +6521,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I554"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G96" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I115" sqref="I115"/>
+      <selection pane="bottomRight" activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7845,6 +7974,9 @@
       <c r="H59" s="7" t="s">
         <v>103</v>
       </c>
+      <c r="I59" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
@@ -7967,7 +8099,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="45">
+    <row r="65" spans="1:9" ht="45">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -7987,7 +8119,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="30">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -8007,7 +8139,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="30">
+    <row r="67" spans="1:9" ht="30">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -8027,7 +8159,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -8047,7 +8179,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -8073,7 +8205,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -8099,7 +8231,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -8125,7 +8257,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -8148,7 +8280,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -8174,7 +8306,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -8200,7 +8332,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="30">
+    <row r="75" spans="1:9" ht="30">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -8223,7 +8355,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -8248,8 +8380,11 @@
       <c r="H76" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -8275,7 +8410,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -8301,7 +8436,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -8324,7 +8459,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -8872,6 +9007,9 @@
       <c r="H103" s="7" t="s">
         <v>675</v>
       </c>
+      <c r="I103" t="s">
+        <v>1004</v>
+      </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
@@ -9071,6 +9209,9 @@
       <c r="H111" s="7" t="s">
         <v>720</v>
       </c>
+      <c r="I111" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
@@ -9606,6 +9747,9 @@
       </c>
       <c r="H133" s="7" t="s">
         <v>729</v>
+      </c>
+      <c r="I133" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="134" spans="1:9">

</xml_diff>

<commit_message>
splitting object for configuration and fe
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4551" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4688" uniqueCount="1062">
   <si>
     <t>DATA</t>
   </si>
@@ -3191,6 +3191,153 @@
   </si>
   <si>
     <t>Federalstates</t>
+  </si>
+  <si>
+    <t>INS_CORE_DATA_PRODUCT</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>PRODUCT_NUMBER</t>
+  </si>
+  <si>
+    <t>IS_NEXT_INSPECTION_PRODUCT</t>
+  </si>
+  <si>
+    <t>IS_PROVISION_COST_MAY_BE_CALCULATED</t>
+  </si>
+  <si>
+    <t>PRICE_REPORT_REQUIRED</t>
+  </si>
+  <si>
+    <t>INS_PRODUCT_TYPE_ID</t>
+  </si>
+  <si>
+    <t>INS_PRODUCT_MATERIAL_GROUP_ID</t>
+  </si>
+  <si>
+    <t>INS_PRODUCT_CLASS_ID</t>
+  </si>
+  <si>
+    <t>INS_CORE_DATA_PRODUCT_GROUP_ID</t>
+  </si>
+  <si>
+    <t>IS_INGENER</t>
+  </si>
+  <si>
+    <t>IS_PRODUCTIVE</t>
+  </si>
+  <si>
+    <t>IS_KM_GELD</t>
+  </si>
+  <si>
+    <t>IS_OTHER_MATERIAL</t>
+  </si>
+  <si>
+    <t>IS_TRIP</t>
+  </si>
+  <si>
+    <t>REUSAGE_TYPE</t>
+  </si>
+  <si>
+    <t>OLD_PRODUCT_NUMBER</t>
+  </si>
+  <si>
+    <t>Produktnummer</t>
+  </si>
+  <si>
+    <t>Product number</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt eine Nachprüfung ist</t>
+  </si>
+  <si>
+    <t>Is next inspection product</t>
+  </si>
+  <si>
+    <t>Angabe, ob für Produkt Gestellungskosten verrechnet werden können</t>
+  </si>
+  <si>
+    <t>Is provision cost may be calculated</t>
+  </si>
+  <si>
+    <t>Price report required</t>
+  </si>
+  <si>
+    <t>Zahlungsbericht erforderlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produkttyp </t>
+  </si>
+  <si>
+    <t>Gewichtsklasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objekttyp  </t>
+  </si>
+  <si>
+    <t>Materialgruppe</t>
+  </si>
+  <si>
+    <t>Material group</t>
+  </si>
+  <si>
+    <t>Produktklasse</t>
+  </si>
+  <si>
+    <t>Product class</t>
+  </si>
+  <si>
+    <t>Arbeitswert/Zeitdauer</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt eine Ingenieursleistung ist</t>
+  </si>
+  <si>
+    <t>Is ingeneur</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt eine Produktivleistung ist („0“ = Aufwandserfassung unproduktiv, „1“ = Produktiv (TP), „2“ = Aufwandserfassung produktiv)</t>
+  </si>
+  <si>
+    <t>Is productive</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt eine Kilometergeld-Leistung für den Verkauf an Kunden ist</t>
+  </si>
+  <si>
+    <t>Is KM Geld</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt eine besondere Leistung ist</t>
+  </si>
+  <si>
+    <t>Is other material</t>
+  </si>
+  <si>
+    <t>Produkt ist Reisezeitprodukt für Aufwandsrückmeldung</t>
+  </si>
+  <si>
+    <t>Is trip</t>
+  </si>
+  <si>
+    <t>Angabe, ob Produkt mehrfach in einem Auftrag erbracht werden kann („0“ = Anzahl immer 1, „1“ = Mehrfach ganzzahlig, „2“ = Mehrfach (&gt;0) mit 2 Nachkommastellen</t>
+  </si>
+  <si>
+    <t>Reusage type</t>
+  </si>
+  <si>
+    <t>Steuerkennzeichen</t>
+  </si>
+  <si>
+    <t>Alte VF97-Produktnummer</t>
+  </si>
+  <si>
+    <t>Old product number</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -3621,13 +3768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T99"/>
+  <dimension ref="A1:T100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R20" sqref="R20"/>
+      <selection pane="bottomRight" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5521,7 +5668,7 @@
         <v>767</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>1061</v>
       </c>
       <c r="F66" t="s">
         <v>147</v>
@@ -5547,7 +5694,7 @@
         <v>768</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>1061</v>
       </c>
       <c r="F67" t="s">
         <v>147</v>
@@ -5573,7 +5720,7 @@
         <v>766</v>
       </c>
       <c r="C68" t="s">
-        <v>151</v>
+        <v>1061</v>
       </c>
       <c r="F68" t="s">
         <v>147</v>
@@ -6237,7 +6384,7 @@
         <v>779</v>
       </c>
       <c r="C91" t="s">
-        <v>151</v>
+        <v>1061</v>
       </c>
       <c r="F91" t="s">
         <v>147</v>
@@ -6446,7 +6593,7 @@
         <v>778</v>
       </c>
       <c r="C98" t="s">
-        <v>151</v>
+        <v>1061</v>
       </c>
       <c r="F98" t="s">
         <v>147</v>
@@ -6493,6 +6640,32 @@
         <v>789</v>
       </c>
       <c r="T99" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
+      <c r="A100" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C100" t="s">
+        <v>152</v>
+      </c>
+      <c r="D100" t="s">
+        <v>160</v>
+      </c>
+      <c r="E100" t="s">
+        <v>225</v>
+      </c>
+      <c r="K100" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L100" t="s">
+        <v>225</v>
+      </c>
+      <c r="N100" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6522,10 +6695,10 @@
   <dimension ref="A1:I554"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D496" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I112" sqref="I112"/>
+      <selection pane="bottomRight" activeCell="H504" sqref="H504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18107,7 +18280,7 @@
       <c r="F474" t="s">
         <v>147</v>
       </c>
-      <c r="G474" s="12" t="s">
+      <c r="G474" s="13" t="s">
         <v>957</v>
       </c>
       <c r="H474" s="7" t="s">
@@ -18127,7 +18300,7 @@
       <c r="D475" t="s">
         <v>147</v>
       </c>
-      <c r="G475" s="12" t="s">
+      <c r="G475" s="13" t="s">
         <v>959</v>
       </c>
       <c r="H475" s="7" t="s">
@@ -18147,7 +18320,7 @@
       <c r="D476" t="s">
         <v>147</v>
       </c>
-      <c r="G476" s="12" t="s">
+      <c r="G476" s="13" t="s">
         <v>960</v>
       </c>
       <c r="H476" s="7" t="s">
@@ -18187,7 +18360,7 @@
       <c r="D478" t="s">
         <v>147</v>
       </c>
-      <c r="G478" s="12" t="s">
+      <c r="G478" s="13" t="s">
         <v>970</v>
       </c>
       <c r="H478" s="7" t="s">
@@ -18213,7 +18386,7 @@
       <c r="F479" t="s">
         <v>147</v>
       </c>
-      <c r="G479" s="12" t="s">
+      <c r="G479" s="13" t="s">
         <v>964</v>
       </c>
       <c r="H479" s="7" t="s">
@@ -18296,7 +18469,7 @@
       <c r="D483" t="s">
         <v>147</v>
       </c>
-      <c r="G483" s="12" t="s">
+      <c r="G483" s="13" t="s">
         <v>182</v>
       </c>
       <c r="H483" s="7" t="s">
@@ -18355,6 +18528,433 @@
         <v>905</v>
       </c>
       <c r="H485" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9" ht="15.75">
+      <c r="A486" t="s">
+        <v>153</v>
+      </c>
+      <c r="B486" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C486" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D486" t="s">
+        <v>147</v>
+      </c>
+      <c r="E486" t="s">
+        <v>147</v>
+      </c>
+      <c r="F486" t="s">
+        <v>147</v>
+      </c>
+      <c r="G486" s="13" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H486" s="7" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="487" spans="1:9" ht="31.5">
+      <c r="A487" t="s">
+        <v>153</v>
+      </c>
+      <c r="B487" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C487" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D487" t="s">
+        <v>147</v>
+      </c>
+      <c r="G487" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H487" s="7" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9" ht="47.25">
+      <c r="A488" t="s">
+        <v>153</v>
+      </c>
+      <c r="B488" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D488" t="s">
+        <v>147</v>
+      </c>
+      <c r="G488" s="13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H488" s="7" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9">
+      <c r="A489" t="s">
+        <v>153</v>
+      </c>
+      <c r="B489" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C489" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D489" t="s">
+        <v>147</v>
+      </c>
+      <c r="G489" s="7" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H489" s="7" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9" ht="15.75">
+      <c r="A490" t="s">
+        <v>153</v>
+      </c>
+      <c r="B490" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C490" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D490" t="s">
+        <v>147</v>
+      </c>
+      <c r="F490" t="s">
+        <v>147</v>
+      </c>
+      <c r="G490" s="12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="H490" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" ht="15.75">
+      <c r="A491" t="s">
+        <v>153</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C491" t="s">
+        <v>586</v>
+      </c>
+      <c r="D491" t="s">
+        <v>147</v>
+      </c>
+      <c r="G491" s="12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H491" s="7" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" ht="15.75">
+      <c r="A492" t="s">
+        <v>153</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C492" t="s">
+        <v>584</v>
+      </c>
+      <c r="D492" t="s">
+        <v>147</v>
+      </c>
+      <c r="G492" s="12" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H492" s="7" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9" ht="15.75">
+      <c r="A493" t="s">
+        <v>153</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D493" t="s">
+        <v>147</v>
+      </c>
+      <c r="G493" s="12" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H493" s="7" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9" ht="15.75">
+      <c r="A494" t="s">
+        <v>153</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D494" t="s">
+        <v>147</v>
+      </c>
+      <c r="G494" s="12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H494" s="7" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" ht="15.75">
+      <c r="A495" t="s">
+        <v>153</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D495" t="s">
+        <v>147</v>
+      </c>
+      <c r="G495" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H495" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" ht="30">
+      <c r="A496" t="s">
+        <v>153</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D496" t="s">
+        <v>147</v>
+      </c>
+      <c r="G496" s="7" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H496" s="7" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" ht="75">
+      <c r="A497" t="s">
+        <v>153</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D497" t="s">
+        <v>147</v>
+      </c>
+      <c r="G497" s="7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H497" s="7" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" ht="30">
+      <c r="A498" t="s">
+        <v>153</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D498" t="s">
+        <v>147</v>
+      </c>
+      <c r="G498" s="7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H498" s="7" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" ht="30">
+      <c r="A499" t="s">
+        <v>153</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D499" t="s">
+        <v>147</v>
+      </c>
+      <c r="G499" s="7" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H499" s="7" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" ht="30">
+      <c r="A500" t="s">
+        <v>153</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D500" t="s">
+        <v>147</v>
+      </c>
+      <c r="G500" s="7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H500" s="7" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" ht="75">
+      <c r="A501" t="s">
+        <v>153</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D501" t="s">
+        <v>147</v>
+      </c>
+      <c r="F501" t="s">
+        <v>147</v>
+      </c>
+      <c r="G501" s="7" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H501" s="7" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8">
+      <c r="A502" t="s">
+        <v>153</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C502" t="s">
+        <v>559</v>
+      </c>
+      <c r="D502" t="s">
+        <v>147</v>
+      </c>
+      <c r="G502" s="7" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H502" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8">
+      <c r="A503" t="s">
+        <v>153</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C503" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D503" t="s">
+        <v>147</v>
+      </c>
+      <c r="E503" t="s">
+        <v>147</v>
+      </c>
+      <c r="G503" s="7" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H503" s="7" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8">
+      <c r="A504" t="s">
+        <v>153</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C504" t="s">
+        <v>902</v>
+      </c>
+      <c r="D504" t="s">
+        <v>147</v>
+      </c>
+      <c r="E504" t="s">
+        <v>147</v>
+      </c>
+      <c r="F504" t="s">
+        <v>147</v>
+      </c>
+      <c r="G504" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H504" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8">
+      <c r="A505" t="s">
+        <v>153</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C505" t="s">
+        <v>903</v>
+      </c>
+      <c r="D505" t="s">
+        <v>147</v>
+      </c>
+      <c r="E505" t="s">
+        <v>147</v>
+      </c>
+      <c r="F505" t="s">
+        <v>147</v>
+      </c>
+      <c r="G505" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H505" s="7" t="s">
         <v>907</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add fe product, driver school and relationships
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4764" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5185" uniqueCount="1179">
   <si>
     <t>DATA</t>
   </si>
@@ -3386,6 +3386,309 @@
   </si>
   <si>
     <t>empEmployeeId</t>
+  </si>
+  <si>
+    <t>DRL_CORE_DATA_PRODUCT</t>
+  </si>
+  <si>
+    <t>DRL_CORE_DATA_PRODUCT_LOCALIZATION</t>
+  </si>
+  <si>
+    <t>DRL_CORE_DATA_PRODUCT_CLASS_BASIS_RSP</t>
+  </si>
+  <si>
+    <t>DRL_DRIVER_SCHOOL</t>
+  </si>
+  <si>
+    <t>DRL_DRIVER_SCHOOL_EXAM_RECOGNITION_TYPE_RSP</t>
+  </si>
+  <si>
+    <t>DRL_DRIVER_SCHOOL_INFO_RSP</t>
+  </si>
+  <si>
+    <t>DRL_COMMUNITY_PARTICIPANT</t>
+  </si>
+  <si>
+    <t>ExamClass,LegalBasis</t>
+  </si>
+  <si>
+    <t>SysLanguage,ExamClass,LegalBasis</t>
+  </si>
+  <si>
+    <t>FE-Produkt</t>
+  </si>
+  <si>
+    <t>FE-Product</t>
+  </si>
+  <si>
+    <t>Rechtsgrund/Klasse</t>
+  </si>
+  <si>
+    <t>Legal basis/class</t>
+  </si>
+  <si>
+    <t>Fahrschule</t>
+  </si>
+  <si>
+    <t>Driverschool</t>
+  </si>
+  <si>
+    <t>Fahrschule Information</t>
+  </si>
+  <si>
+    <t>Anerkennung der Fahrschule</t>
+  </si>
+  <si>
+    <t>Driverschool recognition</t>
+  </si>
+  <si>
+    <t>Mitglied der Fahrschulgemeinschaft</t>
+  </si>
+  <si>
+    <t>Community participant</t>
+  </si>
+  <si>
+    <t>localizations,classBasisRsp</t>
+  </si>
+  <si>
+    <t>Lokalisierung,Rechtsgrund/Klasse</t>
+  </si>
+  <si>
+    <t>Localization,Legalbasis/class</t>
+  </si>
+  <si>
+    <t>examRecognitions,driverSchoolInfo</t>
+  </si>
+  <si>
+    <t>Anerkennung,Information</t>
+  </si>
+  <si>
+    <t>Recognition/Info</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>Mitglieder</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>POINT_AMOUNT</t>
+  </si>
+  <si>
+    <t>MIN_AGE</t>
+  </si>
+  <si>
+    <t>MAX_AGE</t>
+  </si>
+  <si>
+    <t>EXAM_TYPE</t>
+  </si>
+  <si>
+    <t>PRIOR_TIME_IN_MONTHS</t>
+  </si>
+  <si>
+    <t>EXPIRATION_IN_MONTH</t>
+  </si>
+  <si>
+    <t>REPEAT_TIME_IN_DAYS</t>
+  </si>
+  <si>
+    <t>TRAINING_CERT_FLAG</t>
+  </si>
+  <si>
+    <t>RESULT_FLAG</t>
+  </si>
+  <si>
+    <t>MULTIPLY_FLAG</t>
+  </si>
+  <si>
+    <t>IS_MOFA_PRINT</t>
+  </si>
+  <si>
+    <t>IS_ADDITIONAL_PRODUCT</t>
+  </si>
+  <si>
+    <t>IS_PREPAYMENT_REQUIRED</t>
+  </si>
+  <si>
+    <t>FE_PRODUCT_NUMBER</t>
+  </si>
+  <si>
+    <t>REPEAT_TIME_IN_DAYS_REDUCED</t>
+  </si>
+  <si>
+    <t>Anzahl der Punkte des Produkts</t>
+  </si>
+  <si>
+    <t>Point amount</t>
+  </si>
+  <si>
+    <t>Mindestalter des Bewerbers</t>
+  </si>
+  <si>
+    <t>Min age</t>
+  </si>
+  <si>
+    <t>Max age</t>
+  </si>
+  <si>
+    <t>Höchstalter des Bewerbers</t>
+  </si>
+  <si>
+    <t>Prüfungsart</t>
+  </si>
+  <si>
+    <t>Vorzeitige Prüfung in Monaten</t>
+  </si>
+  <si>
+    <t>Verfallsfrist der Leistung in Monaten</t>
+  </si>
+  <si>
+    <t>Ausbildungsbescheinigung notwendig</t>
+  </si>
+  <si>
+    <t>Ergebnis notwendig</t>
+  </si>
+  <si>
+    <t>Leistung mehrfach möglich</t>
+  </si>
+  <si>
+    <t>Zusatzleistung</t>
+  </si>
+  <si>
+    <t>Mofaprüfbescheinigung</t>
+  </si>
+  <si>
+    <t>Vorzahlung erforderlich</t>
+  </si>
+  <si>
+    <t>Pflicht Produkt</t>
+  </si>
+  <si>
+    <t>FE-Produktnummer</t>
+  </si>
+  <si>
+    <t>Wiederholungsfrist in Tagen</t>
+  </si>
+  <si>
+    <t>abgekürzte Wiederholungsfrist in Tagen</t>
+  </si>
+  <si>
+    <t>Exam type</t>
+  </si>
+  <si>
+    <t>Prior time in month</t>
+  </si>
+  <si>
+    <t>Expiration in month</t>
+  </si>
+  <si>
+    <t>Repeat time in days</t>
+  </si>
+  <si>
+    <t>Training certificate required</t>
+  </si>
+  <si>
+    <t>Result required</t>
+  </si>
+  <si>
+    <t>Can be multiple</t>
+  </si>
+  <si>
+    <t>Is Mofa print product</t>
+  </si>
+  <si>
+    <t>Is additional product</t>
+  </si>
+  <si>
+    <t>Prepayment required</t>
+  </si>
+  <si>
+    <t>FE product number</t>
+  </si>
+  <si>
+    <t>Reduced repeat time in days</t>
+  </si>
+  <si>
+    <t>DRL_CORE_DATA_PRODUCT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasse </t>
+  </si>
+  <si>
+    <t>DRL_LEGAL_BASIS_ID</t>
+  </si>
+  <si>
+    <t>Legalbasis</t>
+  </si>
+  <si>
+    <t>DRIVER_SCHOOL_NUMBER</t>
+  </si>
+  <si>
+    <t>ORD_CUSTOMER_ID</t>
+  </si>
+  <si>
+    <t>Driverschool number</t>
+  </si>
+  <si>
+    <t>Kunde</t>
+  </si>
+  <si>
+    <t>Fahrschulnummer</t>
+  </si>
+  <si>
+    <t>DRL_SCHOOL_INFO_ID</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>DRL_DRIVER_SCHOOL_ID_PARTICIPANT</t>
+  </si>
+  <si>
+    <t>DRL_DRIVER_SCHOOL_ID_LEAD</t>
+  </si>
+  <si>
+    <t>führende Fahrschule</t>
+  </si>
+  <si>
+    <t>Driverschool lead</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Mitglied Fahrschule</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/DriverSchoolExamRecognitionTypes,DriverLicenceMasterData/DriverSchoolInfos</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/CoreDataProductLocalizations,DriverLicenceMasterData/CoreDataProductClassBases</t>
+  </si>
+  <si>
+    <t>coreDataProductId</t>
+  </si>
+  <si>
+    <t>driverSchoolId</t>
+  </si>
+  <si>
+    <t>driverSchoolIdLead</t>
+  </si>
+  <si>
+    <t>ExamRecognitionType,SchoolInfo</t>
+  </si>
+  <si>
+    <t>SchoolInfo</t>
+  </si>
+  <si>
+    <t>schoolInfo</t>
+  </si>
+  <si>
+    <t>DriverLicenceMasterData/CommunityParticipants</t>
   </si>
 </sst>
 </file>
@@ -3816,13 +4119,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T101"/>
+  <dimension ref="A1:T108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="I89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3979,6 +4282,18 @@
       <c r="N4" t="s">
         <v>147</v>
       </c>
+      <c r="O4" s="7" t="s">
+        <v>1178</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>1106</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="90">
       <c r="A5" t="s">
@@ -4669,6 +4984,9 @@
       <c r="S26" t="s">
         <v>789</v>
       </c>
+      <c r="T26" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
@@ -4692,6 +5010,9 @@
       <c r="S27" t="s">
         <v>680</v>
       </c>
+      <c r="T27" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" t="s">
@@ -6804,6 +7125,218 @@
       </c>
       <c r="L101" t="s">
         <v>1065</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" ht="30">
+      <c r="A102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C102" t="s">
+        <v>151</v>
+      </c>
+      <c r="J102" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K102" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L102" t="s">
+        <v>1088</v>
+      </c>
+      <c r="N102" t="s">
+        <v>147</v>
+      </c>
+      <c r="O102" s="7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="P102" t="s">
+        <v>1098</v>
+      </c>
+      <c r="Q102" s="7" t="s">
+        <v>1099</v>
+      </c>
+      <c r="R102" s="7" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C103" t="s">
+        <v>151</v>
+      </c>
+      <c r="G103" t="s">
+        <v>147</v>
+      </c>
+      <c r="H103" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I103" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J103" t="s">
+        <v>989</v>
+      </c>
+      <c r="K103" t="s">
+        <v>1064</v>
+      </c>
+      <c r="L103" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" ht="15.75">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C104" t="s">
+        <v>151</v>
+      </c>
+      <c r="G104" t="s">
+        <v>147</v>
+      </c>
+      <c r="H104" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I104" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J104" t="s">
+        <v>1085</v>
+      </c>
+      <c r="K104" s="12" t="s">
+        <v>1089</v>
+      </c>
+      <c r="L104" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" ht="30">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C105" t="s">
+        <v>151</v>
+      </c>
+      <c r="J105" t="s">
+        <v>1175</v>
+      </c>
+      <c r="K105" t="s">
+        <v>1091</v>
+      </c>
+      <c r="L105" t="s">
+        <v>1092</v>
+      </c>
+      <c r="N105" t="s">
+        <v>147</v>
+      </c>
+      <c r="O105" s="7" t="s">
+        <v>1170</v>
+      </c>
+      <c r="P105" t="s">
+        <v>1101</v>
+      </c>
+      <c r="Q105" s="7" t="s">
+        <v>1102</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
+      <c r="A106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C106" t="s">
+        <v>151</v>
+      </c>
+      <c r="G106" t="s">
+        <v>147</v>
+      </c>
+      <c r="H106" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I106" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J106" t="s">
+        <v>990</v>
+      </c>
+      <c r="K106" t="s">
+        <v>1094</v>
+      </c>
+      <c r="L106" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C107" t="s">
+        <v>151</v>
+      </c>
+      <c r="G107" t="s">
+        <v>147</v>
+      </c>
+      <c r="H107" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I107" t="s">
+        <v>1081</v>
+      </c>
+      <c r="J107" t="s">
+        <v>1176</v>
+      </c>
+      <c r="K107" t="s">
+        <v>1093</v>
+      </c>
+      <c r="L107" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
+      <c r="A108" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C108" t="s">
+        <v>151</v>
+      </c>
+      <c r="G108" t="s">
+        <v>147</v>
+      </c>
+      <c r="H108" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I108" t="s">
+        <v>42</v>
+      </c>
+      <c r="K108" t="s">
+        <v>1096</v>
+      </c>
+      <c r="L108" t="s">
+        <v>1097</v>
       </c>
     </row>
   </sheetData>
@@ -6829,13 +7362,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I554"/>
+  <dimension ref="A1:I558"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H499" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G542" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I507" sqref="I507"/>
+      <selection pane="bottomRight" activeCell="I553" sqref="I553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19248,7 +19781,1147 @@
         <v>907</v>
       </c>
     </row>
-    <row r="554" ht="16.5" customHeight="1"/>
+    <row r="512" spans="1:9">
+      <c r="A512" t="s">
+        <v>0</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C512" t="s">
+        <v>398</v>
+      </c>
+      <c r="D512" t="s">
+        <v>147</v>
+      </c>
+      <c r="F512" t="s">
+        <v>147</v>
+      </c>
+      <c r="G512" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H512" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8">
+      <c r="A513" t="s">
+        <v>0</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G513" s="7" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H513" s="7" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" ht="15.75">
+      <c r="A514" t="s">
+        <v>0</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C514" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D514" t="s">
+        <v>147</v>
+      </c>
+      <c r="F514" t="s">
+        <v>147</v>
+      </c>
+      <c r="G514" s="12" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H514" s="7" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" ht="15.75">
+      <c r="A515" t="s">
+        <v>0</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C515" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D515" t="s">
+        <v>147</v>
+      </c>
+      <c r="G515" s="12" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H515" s="7" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" ht="15.75">
+      <c r="A516" t="s">
+        <v>0</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C516" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D516" t="s">
+        <v>147</v>
+      </c>
+      <c r="F516" t="s">
+        <v>147</v>
+      </c>
+      <c r="G516" s="12" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H516" s="7" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" ht="15.75">
+      <c r="A517" t="s">
+        <v>0</v>
+      </c>
+      <c r="B517" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C517" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D517" t="s">
+        <v>147</v>
+      </c>
+      <c r="F517" t="s">
+        <v>147</v>
+      </c>
+      <c r="G517" s="12" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H517" s="7" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" ht="15.75">
+      <c r="A518" t="s">
+        <v>0</v>
+      </c>
+      <c r="B518" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C518" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D518" t="s">
+        <v>147</v>
+      </c>
+      <c r="F518" t="s">
+        <v>147</v>
+      </c>
+      <c r="G518" s="12" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H518" s="7" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" ht="15.75">
+      <c r="A519" t="s">
+        <v>0</v>
+      </c>
+      <c r="B519" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C519" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D519" t="s">
+        <v>147</v>
+      </c>
+      <c r="F519" t="s">
+        <v>147</v>
+      </c>
+      <c r="G519" s="12" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H519" s="7" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" ht="15.75">
+      <c r="A520" t="s">
+        <v>0</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C520" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D520" t="s">
+        <v>147</v>
+      </c>
+      <c r="G520" s="12" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H520" s="7" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" ht="15.75">
+      <c r="A521" t="s">
+        <v>0</v>
+      </c>
+      <c r="B521" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C521" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D521" t="s">
+        <v>147</v>
+      </c>
+      <c r="G521" s="12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H521" s="7" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" ht="15.75">
+      <c r="A522" t="s">
+        <v>0</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C522" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D522" t="s">
+        <v>147</v>
+      </c>
+      <c r="G522" s="12" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H522" s="7" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8">
+      <c r="A523" t="s">
+        <v>0</v>
+      </c>
+      <c r="B523" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D523" t="s">
+        <v>147</v>
+      </c>
+      <c r="G523" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H523" s="7" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8">
+      <c r="A524" t="s">
+        <v>0</v>
+      </c>
+      <c r="B524" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C524" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D524" t="s">
+        <v>147</v>
+      </c>
+      <c r="G524" s="7" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H524" s="7" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8">
+      <c r="A525" t="s">
+        <v>0</v>
+      </c>
+      <c r="B525" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C525" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D525" t="s">
+        <v>147</v>
+      </c>
+      <c r="G525" s="7" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H525" s="7" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8">
+      <c r="A526" t="s">
+        <v>0</v>
+      </c>
+      <c r="B526" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C526" t="s">
+        <v>576</v>
+      </c>
+      <c r="D526" t="s">
+        <v>147</v>
+      </c>
+      <c r="G526" s="7" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H526" s="7" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8">
+      <c r="A527" t="s">
+        <v>0</v>
+      </c>
+      <c r="B527" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C527" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D527" t="s">
+        <v>147</v>
+      </c>
+      <c r="E527" t="s">
+        <v>147</v>
+      </c>
+      <c r="F527" t="s">
+        <v>147</v>
+      </c>
+      <c r="G527" s="7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H527" s="7" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8">
+      <c r="A528" t="s">
+        <v>0</v>
+      </c>
+      <c r="B528" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C528" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D528" t="s">
+        <v>147</v>
+      </c>
+      <c r="F528" t="s">
+        <v>147</v>
+      </c>
+      <c r="G528" s="7" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H528" s="7" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="529" spans="1:9">
+      <c r="A529" t="s">
+        <v>0</v>
+      </c>
+      <c r="B529" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C529" t="s">
+        <v>902</v>
+      </c>
+      <c r="D529" t="s">
+        <v>147</v>
+      </c>
+      <c r="E529" t="s">
+        <v>147</v>
+      </c>
+      <c r="F529" t="s">
+        <v>147</v>
+      </c>
+      <c r="G529" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H529" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="530" spans="1:9">
+      <c r="A530" t="s">
+        <v>0</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C530" t="s">
+        <v>903</v>
+      </c>
+      <c r="D530" t="s">
+        <v>147</v>
+      </c>
+      <c r="E530" t="s">
+        <v>147</v>
+      </c>
+      <c r="F530" t="s">
+        <v>147</v>
+      </c>
+      <c r="G530" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H530" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="531" spans="1:9">
+      <c r="A531" t="s">
+        <v>0</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C531" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D531" t="s">
+        <v>147</v>
+      </c>
+      <c r="F531" t="s">
+        <v>147</v>
+      </c>
+      <c r="G531" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H531" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9">
+      <c r="A532" t="s">
+        <v>0</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C532" t="s">
+        <v>7</v>
+      </c>
+      <c r="D532" t="s">
+        <v>147</v>
+      </c>
+      <c r="E532" t="s">
+        <v>147</v>
+      </c>
+      <c r="F532" t="s">
+        <v>147</v>
+      </c>
+      <c r="G532" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="H532" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="I532" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9">
+      <c r="A533" t="s">
+        <v>0</v>
+      </c>
+      <c r="B533" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C533" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D533" t="s">
+        <v>147</v>
+      </c>
+      <c r="E533" t="s">
+        <v>147</v>
+      </c>
+      <c r="F533" t="s">
+        <v>147</v>
+      </c>
+      <c r="G533" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="H533" s="7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9">
+      <c r="A534" t="s">
+        <v>0</v>
+      </c>
+      <c r="B534" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C534" t="s">
+        <v>9</v>
+      </c>
+      <c r="D534" t="s">
+        <v>147</v>
+      </c>
+      <c r="E534" t="s">
+        <v>147</v>
+      </c>
+      <c r="G534" s="7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H534" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9">
+      <c r="A535" t="s">
+        <v>0</v>
+      </c>
+      <c r="B535" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C535" t="s">
+        <v>902</v>
+      </c>
+      <c r="D535" t="s">
+        <v>147</v>
+      </c>
+      <c r="E535" t="s">
+        <v>147</v>
+      </c>
+      <c r="F535" t="s">
+        <v>147</v>
+      </c>
+      <c r="G535" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H535" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9">
+      <c r="A536" t="s">
+        <v>0</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C536" t="s">
+        <v>903</v>
+      </c>
+      <c r="D536" t="s">
+        <v>147</v>
+      </c>
+      <c r="E536" t="s">
+        <v>147</v>
+      </c>
+      <c r="F536" t="s">
+        <v>147</v>
+      </c>
+      <c r="G536" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H536" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9" ht="15.75">
+      <c r="A537" t="s">
+        <v>0</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C537" t="s">
+        <v>11</v>
+      </c>
+      <c r="D537" t="s">
+        <v>147</v>
+      </c>
+      <c r="E537" t="s">
+        <v>147</v>
+      </c>
+      <c r="F537" t="s">
+        <v>147</v>
+      </c>
+      <c r="G537" s="12" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H537" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I537" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9">
+      <c r="A538" t="s">
+        <v>0</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C538" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D538" t="s">
+        <v>147</v>
+      </c>
+      <c r="F538" t="s">
+        <v>147</v>
+      </c>
+      <c r="G538" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H538" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9">
+      <c r="A539" t="s">
+        <v>0</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C539" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D539" t="s">
+        <v>147</v>
+      </c>
+      <c r="E539" t="s">
+        <v>147</v>
+      </c>
+      <c r="F539" t="s">
+        <v>147</v>
+      </c>
+      <c r="G539" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H539" s="7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="I539" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9">
+      <c r="A540" t="s">
+        <v>0</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C540" t="s">
+        <v>41</v>
+      </c>
+      <c r="D540" t="s">
+        <v>147</v>
+      </c>
+      <c r="E540" t="s">
+        <v>147</v>
+      </c>
+      <c r="F540" t="s">
+        <v>147</v>
+      </c>
+      <c r="G540" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="H540" s="7" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9">
+      <c r="A541" t="s">
+        <v>0</v>
+      </c>
+      <c r="B541" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C541" t="s">
+        <v>902</v>
+      </c>
+      <c r="D541" t="s">
+        <v>147</v>
+      </c>
+      <c r="E541" t="s">
+        <v>147</v>
+      </c>
+      <c r="F541" t="s">
+        <v>147</v>
+      </c>
+      <c r="G541" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H541" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9">
+      <c r="A542" t="s">
+        <v>0</v>
+      </c>
+      <c r="B542" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C542" t="s">
+        <v>903</v>
+      </c>
+      <c r="D542" t="s">
+        <v>147</v>
+      </c>
+      <c r="E542" t="s">
+        <v>147</v>
+      </c>
+      <c r="F542" t="s">
+        <v>147</v>
+      </c>
+      <c r="G542" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H542" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9">
+      <c r="A543" t="s">
+        <v>0</v>
+      </c>
+      <c r="B543" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C543" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D543" t="s">
+        <v>147</v>
+      </c>
+      <c r="E543" t="s">
+        <v>147</v>
+      </c>
+      <c r="F543" t="s">
+        <v>147</v>
+      </c>
+      <c r="G543" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H543" s="7" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9">
+      <c r="A544" t="s">
+        <v>0</v>
+      </c>
+      <c r="B544" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C544" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D544" t="s">
+        <v>147</v>
+      </c>
+      <c r="E544" t="s">
+        <v>147</v>
+      </c>
+      <c r="F544" t="s">
+        <v>147</v>
+      </c>
+      <c r="G544" s="7" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H544" s="7" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9">
+      <c r="A545" t="s">
+        <v>0</v>
+      </c>
+      <c r="B545" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C545" t="s">
+        <v>902</v>
+      </c>
+      <c r="D545" t="s">
+        <v>147</v>
+      </c>
+      <c r="E545" t="s">
+        <v>147</v>
+      </c>
+      <c r="F545" t="s">
+        <v>147</v>
+      </c>
+      <c r="G545" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H545" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9">
+      <c r="A546" t="s">
+        <v>0</v>
+      </c>
+      <c r="B546" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C546" t="s">
+        <v>903</v>
+      </c>
+      <c r="D546" t="s">
+        <v>147</v>
+      </c>
+      <c r="E546" t="s">
+        <v>147</v>
+      </c>
+      <c r="F546" t="s">
+        <v>147</v>
+      </c>
+      <c r="G546" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H546" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9">
+      <c r="A547" t="s">
+        <v>0</v>
+      </c>
+      <c r="B547" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C547" t="s">
+        <v>4</v>
+      </c>
+      <c r="D547" t="s">
+        <v>147</v>
+      </c>
+      <c r="F547" t="s">
+        <v>147</v>
+      </c>
+      <c r="G547" s="7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="H547" s="7" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9">
+      <c r="A548" t="s">
+        <v>0</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C548" t="s">
+        <v>45</v>
+      </c>
+      <c r="D548" t="s">
+        <v>147</v>
+      </c>
+      <c r="E548" t="s">
+        <v>147</v>
+      </c>
+      <c r="F548" t="s">
+        <v>147</v>
+      </c>
+      <c r="G548" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H548" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="I548" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9">
+      <c r="A549" t="s">
+        <v>0</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C549" t="s">
+        <v>902</v>
+      </c>
+      <c r="D549" t="s">
+        <v>147</v>
+      </c>
+      <c r="E549" t="s">
+        <v>147</v>
+      </c>
+      <c r="F549" t="s">
+        <v>147</v>
+      </c>
+      <c r="G549" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H549" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9">
+      <c r="A550" t="s">
+        <v>0</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C550" t="s">
+        <v>903</v>
+      </c>
+      <c r="D550" t="s">
+        <v>147</v>
+      </c>
+      <c r="E550" t="s">
+        <v>147</v>
+      </c>
+      <c r="F550" t="s">
+        <v>147</v>
+      </c>
+      <c r="G550" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H550" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9">
+      <c r="A551" t="s">
+        <v>0</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C551" t="s">
+        <v>4</v>
+      </c>
+      <c r="D551" t="s">
+        <v>147</v>
+      </c>
+      <c r="F551" t="s">
+        <v>147</v>
+      </c>
+      <c r="G551" s="7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="H551" s="7" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9">
+      <c r="A552" t="s">
+        <v>0</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C552" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D552" t="s">
+        <v>147</v>
+      </c>
+      <c r="E552" t="s">
+        <v>147</v>
+      </c>
+      <c r="F552" t="s">
+        <v>147</v>
+      </c>
+      <c r="G552" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="H552" s="7" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I552" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9">
+      <c r="A553" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C553" t="s">
+        <v>902</v>
+      </c>
+      <c r="D553" t="s">
+        <v>147</v>
+      </c>
+      <c r="E553" t="s">
+        <v>147</v>
+      </c>
+      <c r="F553" t="s">
+        <v>147</v>
+      </c>
+      <c r="G553" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H553" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A554" t="s">
+        <v>0</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C554" t="s">
+        <v>903</v>
+      </c>
+      <c r="D554" t="s">
+        <v>147</v>
+      </c>
+      <c r="E554" t="s">
+        <v>147</v>
+      </c>
+      <c r="F554" t="s">
+        <v>147</v>
+      </c>
+      <c r="G554" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H554" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9">
+      <c r="A555" t="s">
+        <v>0</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C555" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D555" t="s">
+        <v>147</v>
+      </c>
+      <c r="F555" t="s">
+        <v>147</v>
+      </c>
+      <c r="G555" s="7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H555" s="7" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9">
+      <c r="A556" t="s">
+        <v>0</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C556" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D556" t="s">
+        <v>147</v>
+      </c>
+      <c r="E556" t="s">
+        <v>147</v>
+      </c>
+      <c r="F556" t="s">
+        <v>147</v>
+      </c>
+      <c r="G556" s="7" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H556" s="7" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9">
+      <c r="A557" t="s">
+        <v>0</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C557" t="s">
+        <v>902</v>
+      </c>
+      <c r="D557" t="s">
+        <v>147</v>
+      </c>
+      <c r="E557" t="s">
+        <v>147</v>
+      </c>
+      <c r="F557" t="s">
+        <v>147</v>
+      </c>
+      <c r="G557" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H557" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9">
+      <c r="A558" t="s">
+        <v>0</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C558" t="s">
+        <v>903</v>
+      </c>
+      <c r="D558" t="s">
+        <v>147</v>
+      </c>
+      <c r="E558" t="s">
+        <v>147</v>
+      </c>
+      <c r="F558" t="s">
+        <v>147</v>
+      </c>
+      <c r="G558" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H558" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C551">
     <filterColumn colId="2"/>

</xml_diff>

<commit_message>
custom core product and FromData/ToDate defaults
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5185" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="1179">
   <si>
     <t>DATA</t>
   </si>
@@ -4121,11 +4121,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="K101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomRight" activeCell="A102" sqref="A102:B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7365,10 +7365,10 @@
   <dimension ref="A1:I558"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G542" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D521" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I553" sqref="I553"/>
+      <selection pane="bottomRight" activeCell="A531" sqref="A531:XFD531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20982,13 +20982,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21072,6 +21072,17 @@
         <v>779</v>
       </c>
       <c r="C6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E7" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Custom InsCoreDataProduct and Fe CoreDataProduct
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5193" uniqueCount="1180">
   <si>
     <t>DATA</t>
   </si>
@@ -3689,6 +3689,9 @@
   </si>
   <si>
     <t>DriverLicenceMasterData/CommunityParticipants</t>
+  </si>
+  <si>
+    <t>ShowExtraFields</t>
   </si>
 </sst>
 </file>
@@ -3798,7 +3801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3824,6 +3827,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4119,13 +4125,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T108"/>
+  <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="K101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="Q92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A102" sqref="A102:B102"/>
+      <selection pane="bottomRight" activeCell="A100" sqref="A100:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4152,7 +4158,7 @@
     <col min="20" max="20" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
@@ -4174,7 +4180,7 @@
       <c r="G1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
         <v>921</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -4213,8 +4219,11 @@
       <c r="T1" s="10" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="10" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4237,7 +4246,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4260,7 +4269,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4295,7 +4304,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="90">
+    <row r="5" spans="1:21" ht="90">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4345,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4379,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4401,7 +4410,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4432,7 +4441,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4463,7 +4472,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4494,7 +4503,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -4532,7 +4541,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4561,7 +4570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4584,7 +4593,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4625,7 +4634,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4654,7 +4663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -6955,7 +6964,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:21">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -6993,7 +7002,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:20">
+    <row r="98" spans="1:21">
       <c r="A98" t="s">
         <v>153</v>
       </c>
@@ -7016,7 +7025,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:21">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -7051,7 +7060,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:21">
       <c r="A100" t="s">
         <v>153</v>
       </c>
@@ -7091,8 +7100,11 @@
       <c r="R100" s="7" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="101" spans="1:20">
+      <c r="U100" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21">
       <c r="A101" t="s">
         <v>153</v>
       </c>
@@ -7127,7 +7139,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="30">
+    <row r="102" spans="1:21" ht="30">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -7161,8 +7173,11 @@
       <c r="R102" s="7" t="s">
         <v>1100</v>
       </c>
-    </row>
-    <row r="103" spans="1:20">
+      <c r="U102" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -7191,7 +7206,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="15.75">
+    <row r="104" spans="1:21" ht="15.75">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -7220,7 +7235,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="30">
+    <row r="105" spans="1:21" ht="30">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -7255,7 +7270,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:21">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -7284,7 +7299,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:21">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -7313,7 +7328,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:21">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -7368,7 +7383,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D521" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A531" sqref="A531:XFD531"/>
+      <selection pane="bottomRight" activeCell="E528" sqref="E528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20107,9 +20122,6 @@
         <v>1120</v>
       </c>
       <c r="D527" t="s">
-        <v>147</v>
-      </c>
-      <c r="E527" t="s">
         <v>147</v>
       </c>
       <c r="F527" t="s">
@@ -20982,13 +20994,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21083,6 +21095,17 @@
         <v>1078</v>
       </c>
       <c r="E7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E8" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add custom binded properties
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5193" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5200" uniqueCount="1187">
   <si>
     <t>DATA</t>
   </si>
@@ -3412,9 +3412,6 @@
     <t>ExamClass,LegalBasis</t>
   </si>
   <si>
-    <t>SysLanguage,ExamClass,LegalBasis</t>
-  </si>
-  <si>
     <t>FE-Produkt</t>
   </si>
   <si>
@@ -3692,6 +3689,30 @@
   </si>
   <si>
     <t>ShowExtraFields</t>
+  </si>
+  <si>
+    <t>examType</t>
+  </si>
+  <si>
+    <t>SysLanguage,ExamClass,LegalBasis,ExamType</t>
+  </si>
+  <si>
+    <t>SelectProduct</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>CustomView</t>
+  </si>
+  <si>
+    <t>CustomViewBindingProperty</t>
+  </si>
+  <si>
+    <t>CustomDataBindingProperty</t>
+  </si>
+  <si>
+    <t>insCoreDataProductName</t>
   </si>
 </sst>
 </file>
@@ -4128,10 +4149,10 @@
   <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="I92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A100" sqref="A100:B100"/>
+      <selection pane="bottomRight" activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4220,7 +4241,7 @@
         <v>947</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -4292,16 +4313,16 @@
         <v>147</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="P4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>1104</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>1105</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="90">
@@ -7150,28 +7171,28 @@
         <v>151</v>
       </c>
       <c r="J102" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K102" t="s">
         <v>1086</v>
       </c>
-      <c r="K102" t="s">
+      <c r="L102" t="s">
         <v>1087</v>
       </c>
-      <c r="L102" t="s">
-        <v>1088</v>
-      </c>
       <c r="N102" t="s">
         <v>147</v>
       </c>
       <c r="O102" s="7" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="P102" t="s">
+        <v>1097</v>
+      </c>
+      <c r="Q102" s="7" t="s">
         <v>1098</v>
       </c>
-      <c r="Q102" s="7" t="s">
+      <c r="R102" s="7" t="s">
         <v>1099</v>
-      </c>
-      <c r="R102" s="7" t="s">
-        <v>1100</v>
       </c>
       <c r="U102" t="s">
         <v>147</v>
@@ -7191,7 +7212,7 @@
         <v>147</v>
       </c>
       <c r="H103" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="I103" t="s">
         <v>1078</v>
@@ -7220,7 +7241,7 @@
         <v>147</v>
       </c>
       <c r="H104" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="I104" t="s">
         <v>1078</v>
@@ -7229,10 +7250,10 @@
         <v>1085</v>
       </c>
       <c r="K104" s="12" t="s">
+        <v>1088</v>
+      </c>
+      <c r="L104" t="s">
         <v>1089</v>
-      </c>
-      <c r="L104" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="105" spans="1:21" ht="30">
@@ -7246,28 +7267,28 @@
         <v>151</v>
       </c>
       <c r="J105" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="K105" t="s">
+        <v>1090</v>
+      </c>
+      <c r="L105" t="s">
         <v>1091</v>
       </c>
-      <c r="L105" t="s">
-        <v>1092</v>
-      </c>
       <c r="N105" t="s">
         <v>147</v>
       </c>
       <c r="O105" s="7" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="P105" t="s">
+        <v>1100</v>
+      </c>
+      <c r="Q105" s="7" t="s">
         <v>1101</v>
       </c>
-      <c r="Q105" s="7" t="s">
+      <c r="R105" s="7" t="s">
         <v>1102</v>
-      </c>
-      <c r="R105" s="7" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="106" spans="1:21">
@@ -7284,7 +7305,7 @@
         <v>147</v>
       </c>
       <c r="H106" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="I106" t="s">
         <v>1081</v>
@@ -7293,10 +7314,10 @@
         <v>990</v>
       </c>
       <c r="K106" t="s">
+        <v>1093</v>
+      </c>
+      <c r="L106" t="s">
         <v>1094</v>
-      </c>
-      <c r="L106" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="107" spans="1:21">
@@ -7313,16 +7334,16 @@
         <v>147</v>
       </c>
       <c r="H107" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="I107" t="s">
         <v>1081</v>
       </c>
       <c r="J107" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="K107" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="L107" t="s">
         <v>146</v>
@@ -7342,16 +7363,16 @@
         <v>147</v>
       </c>
       <c r="H108" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="I108" t="s">
         <v>42</v>
       </c>
       <c r="K108" t="s">
+        <v>1095</v>
+      </c>
+      <c r="L108" t="s">
         <v>1096</v>
-      </c>
-      <c r="L108" t="s">
-        <v>1097</v>
       </c>
     </row>
   </sheetData>
@@ -7377,13 +7398,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I558"/>
+  <dimension ref="A1:L558"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D521" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I506" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E528" sqref="E528"/>
+      <selection pane="bottomRight" activeCell="L514" sqref="L514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7396,9 +7417,12 @@
     <col min="7" max="7" width="37.42578125" style="7" customWidth="1"/>
     <col min="8" max="8" width="29.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="30.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A1" s="4" t="s">
         <v>90</v>
       </c>
@@ -7426,8 +7450,17 @@
       <c r="I1" s="1" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>1184</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7453,7 +7486,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -7479,7 +7512,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -7502,7 +7535,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -7528,7 +7561,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -7554,7 +7587,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -7580,7 +7613,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -7603,7 +7636,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -7626,7 +7659,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45">
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -7646,7 +7679,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45">
+    <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7666,7 +7699,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -7686,7 +7719,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -7706,7 +7739,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -7726,7 +7759,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -7746,7 +7779,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -19445,7 +19478,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="497" spans="1:9" ht="75">
+    <row r="497" spans="1:12" ht="75">
       <c r="A497" t="s">
         <v>153</v>
       </c>
@@ -19465,7 +19498,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="498" spans="1:9" ht="30">
+    <row r="498" spans="1:12" ht="30">
       <c r="A498" t="s">
         <v>153</v>
       </c>
@@ -19485,7 +19518,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="499" spans="1:9" ht="30">
+    <row r="499" spans="1:12" ht="30">
       <c r="A499" t="s">
         <v>153</v>
       </c>
@@ -19505,7 +19538,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="500" spans="1:9" ht="30">
+    <row r="500" spans="1:12" ht="30">
       <c r="A500" t="s">
         <v>153</v>
       </c>
@@ -19525,7 +19558,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="501" spans="1:9" ht="75">
+    <row r="501" spans="1:12" ht="75">
       <c r="A501" t="s">
         <v>153</v>
       </c>
@@ -19548,7 +19581,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="502" spans="1:9">
+    <row r="502" spans="1:12">
       <c r="A502" t="s">
         <v>153</v>
       </c>
@@ -19568,7 +19601,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="503" spans="1:9">
+    <row r="503" spans="1:12">
       <c r="A503" t="s">
         <v>153</v>
       </c>
@@ -19591,7 +19624,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="504" spans="1:9">
+    <row r="504" spans="1:12">
       <c r="A504" t="s">
         <v>153</v>
       </c>
@@ -19617,7 +19650,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="505" spans="1:9">
+    <row r="505" spans="1:12">
       <c r="A505" t="s">
         <v>153</v>
       </c>
@@ -19643,7 +19676,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="506" spans="1:9">
+    <row r="506" spans="1:12">
       <c r="A506" t="s">
         <v>153</v>
       </c>
@@ -19666,7 +19699,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="507" spans="1:9">
+    <row r="507" spans="1:12">
       <c r="A507" t="s">
         <v>153</v>
       </c>
@@ -19695,7 +19728,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="508" spans="1:9">
+    <row r="508" spans="1:12">
       <c r="A508" t="s">
         <v>153</v>
       </c>
@@ -19721,7 +19754,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="509" spans="1:9">
+    <row r="509" spans="1:12">
       <c r="A509" t="s">
         <v>153</v>
       </c>
@@ -19744,7 +19777,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="510" spans="1:9">
+    <row r="510" spans="1:12">
       <c r="A510" t="s">
         <v>153</v>
       </c>
@@ -19770,7 +19803,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="511" spans="1:9">
+    <row r="511" spans="1:12">
       <c r="A511" t="s">
         <v>153</v>
       </c>
@@ -19796,7 +19829,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="512" spans="1:9">
+    <row r="512" spans="1:12">
       <c r="A512" t="s">
         <v>0</v>
       </c>
@@ -19818,8 +19851,17 @@
       <c r="H512" s="7" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="513" spans="1:8">
+      <c r="J512" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K512" t="s">
+        <v>1182</v>
+      </c>
+      <c r="L512" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="513" spans="1:9">
       <c r="A513" t="s">
         <v>0</v>
       </c>
@@ -19827,16 +19869,16 @@
         <v>1078</v>
       </c>
       <c r="C513" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G513" s="7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H513" s="7" t="s">
         <v>1122</v>
       </c>
-      <c r="H513" s="7" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="514" spans="1:8" ht="15.75">
+    </row>
+    <row r="514" spans="1:9" ht="15.75">
       <c r="A514" t="s">
         <v>0</v>
       </c>
@@ -19844,7 +19886,7 @@
         <v>1078</v>
       </c>
       <c r="C514" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D514" t="s">
         <v>147</v>
@@ -19853,13 +19895,13 @@
         <v>147</v>
       </c>
       <c r="G514" s="12" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H514" s="7" t="s">
         <v>1124</v>
       </c>
-      <c r="H514" s="7" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="515" spans="1:8" ht="15.75">
+    </row>
+    <row r="515" spans="1:9" ht="15.75">
       <c r="A515" t="s">
         <v>0</v>
       </c>
@@ -19867,19 +19909,19 @@
         <v>1078</v>
       </c>
       <c r="C515" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D515" t="s">
         <v>147</v>
       </c>
       <c r="G515" s="12" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="H515" s="7" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="516" spans="1:8" ht="15.75">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9" ht="15.75">
       <c r="A516" t="s">
         <v>0</v>
       </c>
@@ -19887,7 +19929,7 @@
         <v>1078</v>
       </c>
       <c r="C516" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D516" t="s">
         <v>147</v>
@@ -19896,13 +19938,16 @@
         <v>147</v>
       </c>
       <c r="G516" s="12" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H516" s="7" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="517" spans="1:8" ht="15.75">
+        <v>1140</v>
+      </c>
+      <c r="I516" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="517" spans="1:9" ht="15.75">
       <c r="A517" t="s">
         <v>0</v>
       </c>
@@ -19910,7 +19955,7 @@
         <v>1078</v>
       </c>
       <c r="C517" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D517" t="s">
         <v>147</v>
@@ -19919,13 +19964,13 @@
         <v>147</v>
       </c>
       <c r="G517" s="12" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="H517" s="7" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="518" spans="1:8" ht="15.75">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="518" spans="1:9" ht="15.75">
       <c r="A518" t="s">
         <v>0</v>
       </c>
@@ -19933,7 +19978,7 @@
         <v>1078</v>
       </c>
       <c r="C518" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D518" t="s">
         <v>147</v>
@@ -19942,13 +19987,13 @@
         <v>147</v>
       </c>
       <c r="G518" s="12" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="H518" s="7" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="519" spans="1:8" ht="15.75">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="519" spans="1:9" ht="15.75">
       <c r="A519" t="s">
         <v>0</v>
       </c>
@@ -19956,7 +20001,7 @@
         <v>1078</v>
       </c>
       <c r="C519" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D519" t="s">
         <v>147</v>
@@ -19965,13 +20010,13 @@
         <v>147</v>
       </c>
       <c r="G519" s="12" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="H519" s="7" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="520" spans="1:8" ht="15.75">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="520" spans="1:9" ht="15.75">
       <c r="A520" t="s">
         <v>0</v>
       </c>
@@ -19979,19 +20024,19 @@
         <v>1078</v>
       </c>
       <c r="C520" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D520" t="s">
         <v>147</v>
       </c>
       <c r="G520" s="12" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="H520" s="7" t="s">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="521" spans="1:8" ht="15.75">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="521" spans="1:9" ht="15.75">
       <c r="A521" t="s">
         <v>0</v>
       </c>
@@ -19999,19 +20044,19 @@
         <v>1078</v>
       </c>
       <c r="C521" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D521" t="s">
         <v>147</v>
       </c>
       <c r="G521" s="12" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="H521" s="7" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="522" spans="1:8" ht="15.75">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="522" spans="1:9" ht="15.75">
       <c r="A522" t="s">
         <v>0</v>
       </c>
@@ -20019,19 +20064,19 @@
         <v>1078</v>
       </c>
       <c r="C522" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D522" t="s">
         <v>147</v>
       </c>
       <c r="G522" s="12" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="H522" s="7" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="523" spans="1:8">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="523" spans="1:9">
       <c r="A523" t="s">
         <v>0</v>
       </c>
@@ -20039,19 +20084,19 @@
         <v>1078</v>
       </c>
       <c r="C523" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D523" t="s">
         <v>147</v>
       </c>
       <c r="G523" s="7" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="H523" s="7" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="524" spans="1:8">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="524" spans="1:9">
       <c r="A524" t="s">
         <v>0</v>
       </c>
@@ -20059,19 +20104,19 @@
         <v>1078</v>
       </c>
       <c r="C524" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D524" t="s">
         <v>147</v>
       </c>
       <c r="G524" s="7" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="H524" s="7" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="525" spans="1:8">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="525" spans="1:9">
       <c r="A525" t="s">
         <v>0</v>
       </c>
@@ -20079,19 +20124,19 @@
         <v>1078</v>
       </c>
       <c r="C525" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D525" t="s">
         <v>147</v>
       </c>
       <c r="G525" s="7" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="H525" s="7" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="526" spans="1:8">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="526" spans="1:9">
       <c r="A526" t="s">
         <v>0</v>
       </c>
@@ -20105,13 +20150,13 @@
         <v>147</v>
       </c>
       <c r="G526" s="7" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="H526" s="7" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="527" spans="1:8">
+    <row r="527" spans="1:9">
       <c r="A527" t="s">
         <v>0</v>
       </c>
@@ -20119,7 +20164,7 @@
         <v>1078</v>
       </c>
       <c r="C527" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D527" t="s">
         <v>147</v>
@@ -20128,13 +20173,13 @@
         <v>147</v>
       </c>
       <c r="G527" s="7" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="H527" s="7" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="528" spans="1:8">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="528" spans="1:9">
       <c r="A528" t="s">
         <v>0</v>
       </c>
@@ -20142,7 +20187,7 @@
         <v>1078</v>
       </c>
       <c r="C528" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D528" t="s">
         <v>147</v>
@@ -20151,10 +20196,10 @@
         <v>147</v>
       </c>
       <c r="G528" s="7" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="H528" s="7" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="529" spans="1:9">
@@ -20217,7 +20262,7 @@
         <v>1079</v>
       </c>
       <c r="C531" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D531" t="s">
         <v>147</v>
@@ -20382,7 +20427,7 @@
         <v>147</v>
       </c>
       <c r="G537" s="12" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="H537" s="7" t="s">
         <v>103</v>
@@ -20399,7 +20444,7 @@
         <v>1080</v>
       </c>
       <c r="C538" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D538" t="s">
         <v>147</v>
@@ -20422,7 +20467,7 @@
         <v>1080</v>
       </c>
       <c r="C539" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D539" t="s">
         <v>147</v>
@@ -20437,7 +20482,7 @@
         <v>135</v>
       </c>
       <c r="H539" s="7" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="I539" t="s">
         <v>940</v>
@@ -20529,7 +20574,7 @@
         <v>1081</v>
       </c>
       <c r="C543" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D543" t="s">
         <v>147</v>
@@ -20541,10 +20586,10 @@
         <v>147</v>
       </c>
       <c r="G543" s="7" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="H543" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="544" spans="1:9">
@@ -20555,7 +20600,7 @@
         <v>1081</v>
       </c>
       <c r="C544" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D544" t="s">
         <v>147</v>
@@ -20567,7 +20612,7 @@
         <v>147</v>
       </c>
       <c r="G544" s="7" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="H544" s="7" t="s">
         <v>783</v>
@@ -20642,10 +20687,10 @@
         <v>147</v>
       </c>
       <c r="G547" s="7" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H547" s="7" t="s">
         <v>1091</v>
-      </c>
-      <c r="H547" s="7" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="548" spans="1:9">
@@ -20746,10 +20791,10 @@
         <v>147</v>
       </c>
       <c r="G551" s="7" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H551" s="7" t="s">
         <v>1091</v>
-      </c>
-      <c r="H551" s="7" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="552" spans="1:9">
@@ -20760,7 +20805,7 @@
         <v>1083</v>
       </c>
       <c r="C552" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D552" t="s">
         <v>147</v>
@@ -20775,10 +20820,10 @@
         <v>421</v>
       </c>
       <c r="H552" s="7" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="I552" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="553" spans="1:9">
@@ -20841,7 +20886,7 @@
         <v>1084</v>
       </c>
       <c r="C555" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D555" t="s">
         <v>147</v>
@@ -20850,10 +20895,10 @@
         <v>147</v>
       </c>
       <c r="G555" s="7" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H555" s="7" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="556" spans="1:9">
@@ -20864,22 +20909,22 @@
         <v>1084</v>
       </c>
       <c r="C556" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D556" t="s">
+        <v>147</v>
+      </c>
+      <c r="E556" t="s">
+        <v>147</v>
+      </c>
+      <c r="F556" t="s">
+        <v>147</v>
+      </c>
+      <c r="G556" s="7" t="s">
         <v>1165</v>
       </c>
-      <c r="D556" t="s">
-        <v>147</v>
-      </c>
-      <c r="E556" t="s">
-        <v>147</v>
-      </c>
-      <c r="F556" t="s">
-        <v>147</v>
-      </c>
-      <c r="G556" s="7" t="s">
+      <c r="H556" s="7" t="s">
         <v>1166</v>
-      </c>
-      <c r="H556" s="7" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="557" spans="1:9">
@@ -20996,7 +21041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Fix for previous commit
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5324" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5327" uniqueCount="1205">
   <si>
     <t>DATA</t>
   </si>
@@ -3764,6 +3764,9 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>masterDataRolePermissionRsps</t>
   </si>
 </sst>
 </file>
@@ -4207,10 +4210,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="H50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomRight" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6202,7 +6205,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -6229,6 +6232,15 @@
       </c>
       <c r="O68" s="7" t="s">
         <v>1196</v>
+      </c>
+      <c r="P68" t="s">
+        <v>1204</v>
+      </c>
+      <c r="Q68" s="7" t="s">
+        <v>1200</v>
+      </c>
+      <c r="R68" s="7" t="s">
+        <v>896</v>
       </c>
       <c r="S68" t="s">
         <v>789</v>

</xml_diff>

<commit_message>
Master data sys tables
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5376" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5378" uniqueCount="1216">
   <si>
     <t>DATA</t>
   </si>
@@ -3791,6 +3791,15 @@
   </si>
   <si>
     <t>ChangePassword</t>
+  </si>
+  <si>
+    <t>sysTableId</t>
+  </si>
+  <si>
+    <t>EditModeType</t>
+  </si>
+  <si>
+    <t>editModeType</t>
   </si>
 </sst>
 </file>
@@ -4234,10 +4243,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A69" sqref="A69:XFD69"/>
+      <selection pane="bottomRight" activeCell="J113" sqref="J113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6959,8 +6968,11 @@
       <c r="C92" t="s">
         <v>1057</v>
       </c>
-      <c r="F92" t="s">
-        <v>147</v>
+      <c r="G92" t="s">
+        <v>147</v>
+      </c>
+      <c r="H92" t="s">
+        <v>1213</v>
       </c>
       <c r="K92" t="s">
         <v>895</v>
@@ -7171,8 +7183,8 @@
       <c r="C99" t="s">
         <v>1057</v>
       </c>
-      <c r="F99" t="s">
-        <v>147</v>
+      <c r="J99" t="s">
+        <v>1214</v>
       </c>
       <c r="K99" t="s">
         <v>894</v>
@@ -7539,10 +7551,10 @@
   <dimension ref="A1:M575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H326" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H473" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K343" sqref="K343"/>
+      <selection pane="bottomRight" activeCell="I492" sqref="I492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19594,6 +19606,9 @@
       </c>
       <c r="H489" s="7" t="s">
         <v>876</v>
+      </c>
+      <c r="I489" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="490" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added sysColumns to sys tables
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -15,7 +15,7 @@
     <sheet name="web.Model{C}" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$568</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$570</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tables{T}'!$A$1:$L$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'web.Model{C}'!$A$1:$C$380</definedName>
   </definedNames>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5378" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5391" uniqueCount="1219">
   <si>
     <t>DATA</t>
   </si>
@@ -3790,9 +3790,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>ChangePassword</t>
-  </si>
-  <si>
     <t>sysTableId</t>
   </si>
   <si>
@@ -3800,6 +3797,18 @@
   </si>
   <si>
     <t>editModeType</t>
+  </si>
+  <si>
+    <t>SYS_TABLE</t>
+  </si>
+  <si>
+    <t>DE: Column</t>
+  </si>
+  <si>
+    <t>sysColumns</t>
+  </si>
+  <si>
+    <t>Settings/SysColumns</t>
   </si>
 </sst>
 </file>
@@ -4243,10 +4252,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J113" sqref="J113"/>
+      <selection pane="bottomRight" activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6972,7 +6981,10 @@
         <v>147</v>
       </c>
       <c r="H92" t="s">
-        <v>1213</v>
+        <v>1212</v>
+      </c>
+      <c r="I92" t="s">
+        <v>1215</v>
       </c>
       <c r="K92" t="s">
         <v>895</v>
@@ -6980,9 +6992,6 @@
       <c r="L92" t="s">
         <v>899</v>
       </c>
-      <c r="N92" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -7184,7 +7193,7 @@
         <v>1057</v>
       </c>
       <c r="J99" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K99" t="s">
         <v>894</v>
@@ -7194,6 +7203,18 @@
       </c>
       <c r="N99" t="s">
         <v>147</v>
+      </c>
+      <c r="O99" s="7" t="s">
+        <v>1218</v>
+      </c>
+      <c r="P99" t="s">
+        <v>1217</v>
+      </c>
+      <c r="Q99" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
@@ -7548,13 +7569,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M575"/>
+  <dimension ref="A1:M577"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H473" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D323" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I492" sqref="I492"/>
+      <selection pane="bottomRight" activeCell="E338" sqref="E338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15846,7 +15867,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>153</v>
       </c>
@@ -15859,9 +15880,6 @@
       <c r="D337" t="s">
         <v>147</v>
       </c>
-      <c r="E337" t="s">
-        <v>147</v>
-      </c>
       <c r="F337" t="s">
         <v>147</v>
       </c>
@@ -15875,7 +15893,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>153</v>
       </c>
@@ -15904,7 +15922,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>153</v>
       </c>
@@ -15930,7 +15948,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>153</v>
       </c>
@@ -15956,7 +15974,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>153</v>
       </c>
@@ -15982,7 +16000,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>153</v>
       </c>
@@ -16008,7 +16026,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>153</v>
       </c>
@@ -16030,11 +16048,8 @@
       <c r="H343" s="7" t="s">
         <v>1211</v>
       </c>
-      <c r="J343" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>153</v>
       </c>
@@ -16063,7 +16078,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>153</v>
       </c>
@@ -16089,7 +16104,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>153</v>
       </c>
@@ -16115,7 +16130,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>153</v>
       </c>
@@ -16141,7 +16156,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>153</v>
       </c>
@@ -16164,7 +16179,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>153</v>
       </c>
@@ -16190,7 +16205,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>153</v>
       </c>
@@ -16216,7 +16231,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>153</v>
       </c>
@@ -16242,7 +16257,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>153</v>
       </c>
@@ -18748,9 +18763,6 @@
       <c r="D454" t="s">
         <v>147</v>
       </c>
-      <c r="E454" t="s">
-        <v>147</v>
-      </c>
       <c r="G454" s="7" t="s">
         <v>873</v>
       </c>
@@ -18809,25 +18821,19 @@
         <v>153</v>
       </c>
       <c r="B457" t="s">
-        <v>286</v>
+        <v>779</v>
       </c>
       <c r="C457" t="s">
-        <v>363</v>
+        <v>902</v>
       </c>
       <c r="D457" t="s">
         <v>147</v>
       </c>
-      <c r="E457" t="s">
-        <v>147</v>
-      </c>
-      <c r="F457" t="s">
-        <v>147</v>
-      </c>
       <c r="G457" s="7" t="s">
-        <v>529</v>
+        <v>904</v>
       </c>
       <c r="H457" s="7" t="s">
-        <v>785</v>
+        <v>906</v>
       </c>
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.3">
@@ -18835,22 +18841,19 @@
         <v>153</v>
       </c>
       <c r="B458" t="s">
-        <v>286</v>
+        <v>779</v>
       </c>
       <c r="C458" t="s">
-        <v>12</v>
+        <v>903</v>
       </c>
       <c r="D458" t="s">
         <v>147</v>
       </c>
-      <c r="E458" t="s">
-        <v>147</v>
-      </c>
       <c r="G458" s="7" t="s">
-        <v>533</v>
+        <v>905</v>
       </c>
       <c r="H458" s="7" t="s">
-        <v>789</v>
+        <v>907</v>
       </c>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.3">
@@ -18861,7 +18864,7 @@
         <v>286</v>
       </c>
       <c r="C459" t="s">
-        <v>534</v>
+        <v>363</v>
       </c>
       <c r="D459" t="s">
         <v>147</v>
@@ -18869,11 +18872,14 @@
       <c r="E459" t="s">
         <v>147</v>
       </c>
+      <c r="F459" t="s">
+        <v>147</v>
+      </c>
       <c r="G459" s="7" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="H459" s="7" t="s">
-        <v>841</v>
+        <v>785</v>
       </c>
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.3">
@@ -18884,7 +18890,7 @@
         <v>286</v>
       </c>
       <c r="C460" t="s">
-        <v>902</v>
+        <v>12</v>
       </c>
       <c r="D460" t="s">
         <v>147</v>
@@ -18892,14 +18898,11 @@
       <c r="E460" t="s">
         <v>147</v>
       </c>
-      <c r="F460" t="s">
-        <v>147</v>
-      </c>
       <c r="G460" s="7" t="s">
-        <v>904</v>
+        <v>533</v>
       </c>
       <c r="H460" s="7" t="s">
-        <v>906</v>
+        <v>789</v>
       </c>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.3">
@@ -18910,7 +18913,7 @@
         <v>286</v>
       </c>
       <c r="C461" t="s">
-        <v>903</v>
+        <v>534</v>
       </c>
       <c r="D461" t="s">
         <v>147</v>
@@ -18918,14 +18921,11 @@
       <c r="E461" t="s">
         <v>147</v>
       </c>
-      <c r="F461" t="s">
-        <v>147</v>
-      </c>
       <c r="G461" s="7" t="s">
-        <v>905</v>
+        <v>535</v>
       </c>
       <c r="H461" s="7" t="s">
-        <v>907</v>
+        <v>841</v>
       </c>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.3">
@@ -18933,10 +18933,10 @@
         <v>153</v>
       </c>
       <c r="B462" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C462" t="s">
-        <v>363</v>
+        <v>902</v>
       </c>
       <c r="D462" t="s">
         <v>147</v>
@@ -18948,10 +18948,10 @@
         <v>147</v>
       </c>
       <c r="G462" s="7" t="s">
-        <v>521</v>
+        <v>904</v>
       </c>
       <c r="H462" s="7" t="s">
-        <v>785</v>
+        <v>906</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.3">
@@ -18959,10 +18959,10 @@
         <v>153</v>
       </c>
       <c r="B463" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C463" t="s">
-        <v>536</v>
+        <v>903</v>
       </c>
       <c r="D463" t="s">
         <v>147</v>
@@ -18970,14 +18970,17 @@
       <c r="E463" t="s">
         <v>147</v>
       </c>
+      <c r="F463" t="s">
+        <v>147</v>
+      </c>
       <c r="G463" s="7" t="s">
-        <v>537</v>
+        <v>905</v>
       </c>
       <c r="H463" s="7" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="464" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>153</v>
       </c>
@@ -18985,19 +18988,25 @@
         <v>289</v>
       </c>
       <c r="C464" t="s">
-        <v>538</v>
+        <v>363</v>
       </c>
       <c r="D464" t="s">
         <v>147</v>
       </c>
+      <c r="E464" t="s">
+        <v>147</v>
+      </c>
+      <c r="F464" t="s">
+        <v>147</v>
+      </c>
       <c r="G464" s="7" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
       <c r="H464" s="7" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="465" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>153</v>
       </c>
@@ -19005,19 +19014,22 @@
         <v>289</v>
       </c>
       <c r="C465" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D465" t="s">
         <v>147</v>
       </c>
+      <c r="E465" t="s">
+        <v>147</v>
+      </c>
       <c r="G465" s="7" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="H465" s="7" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="466" spans="1:9" x14ac:dyDescent="0.3">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>153</v>
       </c>
@@ -19025,22 +19037,19 @@
         <v>289</v>
       </c>
       <c r="C466" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D466" t="s">
         <v>147</v>
       </c>
-      <c r="E466" t="s">
-        <v>147</v>
-      </c>
       <c r="G466" s="7" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="H466" s="7" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="467" spans="1:9" x14ac:dyDescent="0.3">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>153</v>
       </c>
@@ -19048,22 +19057,16 @@
         <v>289</v>
       </c>
       <c r="C467" t="s">
-        <v>902</v>
+        <v>540</v>
       </c>
       <c r="D467" t="s">
         <v>147</v>
       </c>
-      <c r="E467" t="s">
-        <v>147</v>
-      </c>
-      <c r="F467" t="s">
-        <v>147</v>
-      </c>
       <c r="G467" s="7" t="s">
-        <v>904</v>
+        <v>541</v>
       </c>
       <c r="H467" s="7" t="s">
-        <v>906</v>
+        <v>844</v>
       </c>
     </row>
     <row r="468" spans="1:9" x14ac:dyDescent="0.3">
@@ -19074,7 +19077,7 @@
         <v>289</v>
       </c>
       <c r="C468" t="s">
-        <v>903</v>
+        <v>542</v>
       </c>
       <c r="D468" t="s">
         <v>147</v>
@@ -19082,14 +19085,11 @@
       <c r="E468" t="s">
         <v>147</v>
       </c>
-      <c r="F468" t="s">
-        <v>147</v>
-      </c>
       <c r="G468" s="7" t="s">
-        <v>905</v>
+        <v>543</v>
       </c>
       <c r="H468" s="7" t="s">
-        <v>907</v>
+        <v>635</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -19097,10 +19097,10 @@
         <v>153</v>
       </c>
       <c r="B469" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="C469" t="s">
-        <v>506</v>
+        <v>902</v>
       </c>
       <c r="D469" t="s">
         <v>147</v>
@@ -19112,10 +19112,10 @@
         <v>147</v>
       </c>
       <c r="G469" s="7" t="s">
-        <v>263</v>
+        <v>904</v>
       </c>
       <c r="H469" s="7" t="s">
-        <v>264</v>
+        <v>906</v>
       </c>
     </row>
     <row r="470" spans="1:9" x14ac:dyDescent="0.3">
@@ -19123,10 +19123,10 @@
         <v>153</v>
       </c>
       <c r="B470" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="C470" t="s">
-        <v>507</v>
+        <v>903</v>
       </c>
       <c r="D470" t="s">
         <v>147</v>
@@ -19134,11 +19134,14 @@
       <c r="E470" t="s">
         <v>147</v>
       </c>
+      <c r="F470" t="s">
+        <v>147</v>
+      </c>
       <c r="G470" s="7" t="s">
-        <v>508</v>
+        <v>905</v>
       </c>
       <c r="H470" s="7" t="s">
-        <v>838</v>
+        <v>907</v>
       </c>
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.3">
@@ -19149,19 +19152,22 @@
         <v>261</v>
       </c>
       <c r="C471" t="s">
-        <v>16</v>
+        <v>506</v>
       </c>
       <c r="D471" t="s">
         <v>147</v>
       </c>
+      <c r="E471" t="s">
+        <v>147</v>
+      </c>
+      <c r="F471" t="s">
+        <v>147</v>
+      </c>
       <c r="G471" s="7" t="s">
-        <v>509</v>
+        <v>263</v>
       </c>
       <c r="H471" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I471" t="s">
-        <v>974</v>
+        <v>264</v>
       </c>
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.3">
@@ -19172,19 +19178,19 @@
         <v>261</v>
       </c>
       <c r="C472" t="s">
-        <v>55</v>
+        <v>507</v>
       </c>
       <c r="D472" t="s">
         <v>147</v>
       </c>
+      <c r="E472" t="s">
+        <v>147</v>
+      </c>
       <c r="G472" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H472" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="I472" t="s">
-        <v>975</v>
+        <v>838</v>
       </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.3">
@@ -19195,22 +19201,19 @@
         <v>261</v>
       </c>
       <c r="C473" t="s">
-        <v>902</v>
+        <v>16</v>
       </c>
       <c r="D473" t="s">
         <v>147</v>
       </c>
-      <c r="E473" t="s">
-        <v>147</v>
-      </c>
-      <c r="F473" t="s">
-        <v>147</v>
-      </c>
       <c r="G473" s="7" t="s">
-        <v>904</v>
+        <v>509</v>
       </c>
       <c r="H473" s="7" t="s">
-        <v>906</v>
+        <v>288</v>
+      </c>
+      <c r="I473" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.3">
@@ -19221,22 +19224,19 @@
         <v>261</v>
       </c>
       <c r="C474" t="s">
-        <v>903</v>
+        <v>55</v>
       </c>
       <c r="D474" t="s">
         <v>147</v>
       </c>
-      <c r="E474" t="s">
-        <v>147</v>
-      </c>
-      <c r="F474" t="s">
-        <v>147</v>
-      </c>
       <c r="G474" s="7" t="s">
-        <v>905</v>
+        <v>510</v>
       </c>
       <c r="H474" s="7" t="s">
-        <v>907</v>
+        <v>281</v>
+      </c>
+      <c r="I474" t="s">
+        <v>975</v>
       </c>
     </row>
     <row r="475" spans="1:9" x14ac:dyDescent="0.3">
@@ -19244,10 +19244,10 @@
         <v>153</v>
       </c>
       <c r="B475" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="C475" t="s">
-        <v>544</v>
+        <v>902</v>
       </c>
       <c r="D475" t="s">
         <v>147</v>
@@ -19259,10 +19259,10 @@
         <v>147</v>
       </c>
       <c r="G475" s="7" t="s">
-        <v>293</v>
+        <v>904</v>
       </c>
       <c r="H475" s="7" t="s">
-        <v>845</v>
+        <v>906</v>
       </c>
     </row>
     <row r="476" spans="1:9" x14ac:dyDescent="0.3">
@@ -19270,10 +19270,10 @@
         <v>153</v>
       </c>
       <c r="B476" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="C476" t="s">
-        <v>15</v>
+        <v>903</v>
       </c>
       <c r="D476" t="s">
         <v>147</v>
@@ -19281,11 +19281,14 @@
       <c r="E476" t="s">
         <v>147</v>
       </c>
+      <c r="F476" t="s">
+        <v>147</v>
+      </c>
       <c r="G476" s="7" t="s">
-        <v>545</v>
+        <v>905</v>
       </c>
       <c r="H476" s="7" t="s">
-        <v>645</v>
+        <v>907</v>
       </c>
     </row>
     <row r="477" spans="1:9" x14ac:dyDescent="0.3">
@@ -19296,7 +19299,7 @@
         <v>292</v>
       </c>
       <c r="C477" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D477" t="s">
         <v>147</v>
@@ -19304,11 +19307,14 @@
       <c r="E477" t="s">
         <v>147</v>
       </c>
+      <c r="F477" t="s">
+        <v>147</v>
+      </c>
       <c r="G477" s="7" t="s">
-        <v>547</v>
+        <v>293</v>
       </c>
       <c r="H477" s="7" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="478" spans="1:9" x14ac:dyDescent="0.3">
@@ -19319,7 +19325,7 @@
         <v>292</v>
       </c>
       <c r="C478" t="s">
-        <v>902</v>
+        <v>15</v>
       </c>
       <c r="D478" t="s">
         <v>147</v>
@@ -19327,14 +19333,11 @@
       <c r="E478" t="s">
         <v>147</v>
       </c>
-      <c r="F478" t="s">
-        <v>147</v>
-      </c>
       <c r="G478" s="7" t="s">
-        <v>904</v>
+        <v>545</v>
       </c>
       <c r="H478" s="7" t="s">
-        <v>906</v>
+        <v>645</v>
       </c>
     </row>
     <row r="479" spans="1:9" x14ac:dyDescent="0.3">
@@ -19345,7 +19348,7 @@
         <v>292</v>
       </c>
       <c r="C479" t="s">
-        <v>903</v>
+        <v>546</v>
       </c>
       <c r="D479" t="s">
         <v>147</v>
@@ -19353,14 +19356,11 @@
       <c r="E479" t="s">
         <v>147</v>
       </c>
-      <c r="F479" t="s">
-        <v>147</v>
-      </c>
       <c r="G479" s="7" t="s">
-        <v>905</v>
+        <v>547</v>
       </c>
       <c r="H479" s="7" t="s">
-        <v>907</v>
+        <v>846</v>
       </c>
     </row>
     <row r="480" spans="1:9" x14ac:dyDescent="0.3">
@@ -19368,22 +19368,25 @@
         <v>153</v>
       </c>
       <c r="B480" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="C480" t="s">
-        <v>511</v>
+        <v>902</v>
       </c>
       <c r="D480" t="s">
         <v>147</v>
       </c>
+      <c r="E480" t="s">
+        <v>147</v>
+      </c>
       <c r="F480" t="s">
         <v>147</v>
       </c>
       <c r="G480" s="7" t="s">
-        <v>512</v>
+        <v>904</v>
       </c>
       <c r="H480" s="7" t="s">
-        <v>839</v>
+        <v>906</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -19391,10 +19394,10 @@
         <v>153</v>
       </c>
       <c r="B481" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="C481" t="s">
-        <v>12</v>
+        <v>903</v>
       </c>
       <c r="D481" t="s">
         <v>147</v>
@@ -19402,11 +19405,14 @@
       <c r="E481" t="s">
         <v>147</v>
       </c>
+      <c r="F481" t="s">
+        <v>147</v>
+      </c>
       <c r="G481" s="7" t="s">
-        <v>513</v>
+        <v>905</v>
       </c>
       <c r="H481" s="7" t="s">
-        <v>789</v>
+        <v>907</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -19417,19 +19423,19 @@
         <v>265</v>
       </c>
       <c r="C482" t="s">
-        <v>9</v>
+        <v>511</v>
       </c>
       <c r="D482" t="s">
         <v>147</v>
       </c>
-      <c r="E482" t="s">
+      <c r="F482" t="s">
         <v>147</v>
       </c>
       <c r="G482" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H482" s="7" t="s">
-        <v>635</v>
+        <v>839</v>
       </c>
     </row>
     <row r="483" spans="1:9" x14ac:dyDescent="0.3">
@@ -19440,7 +19446,7 @@
         <v>265</v>
       </c>
       <c r="C483" t="s">
-        <v>902</v>
+        <v>12</v>
       </c>
       <c r="D483" t="s">
         <v>147</v>
@@ -19448,14 +19454,11 @@
       <c r="E483" t="s">
         <v>147</v>
       </c>
-      <c r="F483" t="s">
-        <v>147</v>
-      </c>
       <c r="G483" s="7" t="s">
-        <v>904</v>
+        <v>513</v>
       </c>
       <c r="H483" s="7" t="s">
-        <v>906</v>
+        <v>789</v>
       </c>
     </row>
     <row r="484" spans="1:9" x14ac:dyDescent="0.3">
@@ -19466,7 +19469,7 @@
         <v>265</v>
       </c>
       <c r="C484" t="s">
-        <v>903</v>
+        <v>9</v>
       </c>
       <c r="D484" t="s">
         <v>147</v>
@@ -19474,14 +19477,11 @@
       <c r="E484" t="s">
         <v>147</v>
       </c>
-      <c r="F484" t="s">
-        <v>147</v>
-      </c>
       <c r="G484" s="7" t="s">
-        <v>905</v>
+        <v>514</v>
       </c>
       <c r="H484" s="7" t="s">
-        <v>907</v>
+        <v>635</v>
       </c>
     </row>
     <row r="485" spans="1:9" x14ac:dyDescent="0.3">
@@ -19489,22 +19489,25 @@
         <v>153</v>
       </c>
       <c r="B485" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C485" t="s">
-        <v>478</v>
+        <v>902</v>
       </c>
       <c r="D485" t="s">
         <v>147</v>
       </c>
+      <c r="E485" t="s">
+        <v>147</v>
+      </c>
       <c r="F485" t="s">
         <v>147</v>
       </c>
       <c r="G485" s="7" t="s">
-        <v>515</v>
+        <v>904</v>
       </c>
       <c r="H485" s="7" t="s">
-        <v>223</v>
+        <v>906</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -19512,10 +19515,10 @@
         <v>153</v>
       </c>
       <c r="B486" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C486" t="s">
-        <v>516</v>
+        <v>903</v>
       </c>
       <c r="D486" t="s">
         <v>147</v>
@@ -19527,10 +19530,10 @@
         <v>147</v>
       </c>
       <c r="G486" s="7" t="s">
-        <v>517</v>
+        <v>905</v>
       </c>
       <c r="H486" s="7" t="s">
-        <v>772</v>
+        <v>907</v>
       </c>
     </row>
     <row r="487" spans="1:9" x14ac:dyDescent="0.3">
@@ -19541,22 +19544,19 @@
         <v>267</v>
       </c>
       <c r="C487" t="s">
-        <v>902</v>
+        <v>478</v>
       </c>
       <c r="D487" t="s">
         <v>147</v>
       </c>
-      <c r="E487" t="s">
-        <v>147</v>
-      </c>
       <c r="F487" t="s">
         <v>147</v>
       </c>
       <c r="G487" s="7" t="s">
-        <v>904</v>
+        <v>515</v>
       </c>
       <c r="H487" s="7" t="s">
-        <v>906</v>
+        <v>223</v>
       </c>
     </row>
     <row r="488" spans="1:9" x14ac:dyDescent="0.3">
@@ -19567,7 +19567,7 @@
         <v>267</v>
       </c>
       <c r="C488" t="s">
-        <v>903</v>
+        <v>516</v>
       </c>
       <c r="D488" t="s">
         <v>147</v>
@@ -19579,10 +19579,10 @@
         <v>147</v>
       </c>
       <c r="G488" s="7" t="s">
-        <v>905</v>
+        <v>517</v>
       </c>
       <c r="H488" s="7" t="s">
-        <v>907</v>
+        <v>772</v>
       </c>
     </row>
     <row r="489" spans="1:9" x14ac:dyDescent="0.3">
@@ -19590,10 +19590,10 @@
         <v>153</v>
       </c>
       <c r="B489" t="s">
-        <v>778</v>
+        <v>267</v>
       </c>
       <c r="C489" t="s">
-        <v>782</v>
+        <v>902</v>
       </c>
       <c r="D489" t="s">
         <v>147</v>
@@ -19601,14 +19601,14 @@
       <c r="E489" t="s">
         <v>147</v>
       </c>
+      <c r="F489" t="s">
+        <v>147</v>
+      </c>
       <c r="G489" s="7" t="s">
-        <v>875</v>
+        <v>904</v>
       </c>
       <c r="H489" s="7" t="s">
-        <v>876</v>
-      </c>
-      <c r="I489" t="s">
-        <v>1215</v>
+        <v>906</v>
       </c>
     </row>
     <row r="490" spans="1:9" x14ac:dyDescent="0.3">
@@ -19616,68 +19616,74 @@
         <v>153</v>
       </c>
       <c r="B490" t="s">
+        <v>267</v>
+      </c>
+      <c r="C490" t="s">
+        <v>903</v>
+      </c>
+      <c r="D490" t="s">
+        <v>147</v>
+      </c>
+      <c r="E490" t="s">
+        <v>147</v>
+      </c>
+      <c r="F490" t="s">
+        <v>147</v>
+      </c>
+      <c r="G490" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H490" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>153</v>
+      </c>
+      <c r="B491" t="s">
         <v>778</v>
       </c>
-      <c r="C490" t="s">
+      <c r="C491" t="s">
+        <v>782</v>
+      </c>
+      <c r="D491" t="s">
+        <v>147</v>
+      </c>
+      <c r="E491" t="s">
+        <v>147</v>
+      </c>
+      <c r="G491" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="H491" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="I491" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>153</v>
+      </c>
+      <c r="B492" t="s">
+        <v>778</v>
+      </c>
+      <c r="C492" t="s">
         <v>9</v>
       </c>
-      <c r="D490" t="s">
-        <v>147</v>
-      </c>
-      <c r="E490" t="s">
-        <v>147</v>
-      </c>
-      <c r="G490" s="7" t="s">
+      <c r="D492" t="s">
+        <v>147</v>
+      </c>
+      <c r="E492" t="s">
+        <v>147</v>
+      </c>
+      <c r="G492" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="H490" s="7" t="s">
+      <c r="H492" s="7" t="s">
         <v>635</v>
-      </c>
-    </row>
-    <row r="491" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A491" t="s">
-        <v>153</v>
-      </c>
-      <c r="B491" t="s">
-        <v>944</v>
-      </c>
-      <c r="C491" t="s">
-        <v>945</v>
-      </c>
-      <c r="D491" t="s">
-        <v>147</v>
-      </c>
-      <c r="E491" t="s">
-        <v>147</v>
-      </c>
-      <c r="F491" t="s">
-        <v>147</v>
-      </c>
-      <c r="G491" s="13" t="s">
-        <v>953</v>
-      </c>
-      <c r="H491" s="7" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="492" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A492" t="s">
-        <v>153</v>
-      </c>
-      <c r="B492" t="s">
-        <v>944</v>
-      </c>
-      <c r="C492" t="s">
-        <v>12</v>
-      </c>
-      <c r="D492" t="s">
-        <v>147</v>
-      </c>
-      <c r="G492" s="13" t="s">
-        <v>955</v>
-      </c>
-      <c r="H492" s="7" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="493" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -19688,19 +19694,25 @@
         <v>944</v>
       </c>
       <c r="C493" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D493" t="s">
         <v>147</v>
       </c>
+      <c r="E493" t="s">
+        <v>147</v>
+      </c>
+      <c r="F493" t="s">
+        <v>147</v>
+      </c>
       <c r="G493" s="13" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="H493" s="7" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>153</v>
       </c>
@@ -19708,16 +19720,16 @@
         <v>944</v>
       </c>
       <c r="C494" t="s">
-        <v>947</v>
+        <v>12</v>
       </c>
       <c r="D494" t="s">
         <v>147</v>
       </c>
-      <c r="G494" s="7" t="s">
-        <v>969</v>
+      <c r="G494" s="13" t="s">
+        <v>955</v>
       </c>
       <c r="H494" s="7" t="s">
-        <v>959</v>
+        <v>789</v>
       </c>
     </row>
     <row r="495" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -19728,22 +19740,19 @@
         <v>944</v>
       </c>
       <c r="C495" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D495" t="s">
         <v>147</v>
       </c>
       <c r="G495" s="13" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="H495" s="7" t="s">
-        <v>967</v>
-      </c>
-      <c r="I495" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="496" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>153</v>
       </c>
@@ -19751,25 +19760,19 @@
         <v>944</v>
       </c>
       <c r="C496" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D496" t="s">
         <v>147</v>
       </c>
-      <c r="F496" t="s">
-        <v>147</v>
-      </c>
-      <c r="G496" s="13" t="s">
-        <v>960</v>
+      <c r="G496" s="7" t="s">
+        <v>969</v>
       </c>
       <c r="H496" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="I496" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="497" spans="1:9" x14ac:dyDescent="0.3">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>153</v>
       </c>
@@ -19777,19 +19780,22 @@
         <v>944</v>
       </c>
       <c r="C497" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D497" t="s">
         <v>147</v>
       </c>
-      <c r="G497" s="7" t="s">
-        <v>964</v>
+      <c r="G497" s="13" t="s">
+        <v>966</v>
       </c>
       <c r="H497" s="7" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="498" spans="1:9" x14ac:dyDescent="0.3">
+        <v>967</v>
+      </c>
+      <c r="I497" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="498" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>153</v>
       </c>
@@ -19797,19 +19803,25 @@
         <v>944</v>
       </c>
       <c r="C498" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D498" t="s">
         <v>147</v>
       </c>
-      <c r="G498" s="7" t="s">
-        <v>965</v>
+      <c r="F498" t="s">
+        <v>147</v>
+      </c>
+      <c r="G498" s="13" t="s">
+        <v>960</v>
       </c>
       <c r="H498" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="499" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>961</v>
+      </c>
+      <c r="I498" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>153</v>
       </c>
@@ -19817,19 +19829,19 @@
         <v>944</v>
       </c>
       <c r="C499" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="D499" t="s">
         <v>147</v>
       </c>
-      <c r="G499" s="13" t="s">
-        <v>958</v>
+      <c r="G499" s="7" t="s">
+        <v>964</v>
       </c>
       <c r="H499" s="7" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="500" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>153</v>
       </c>
@@ -19837,22 +19849,19 @@
         <v>944</v>
       </c>
       <c r="C500" t="s">
-        <v>498</v>
+        <v>951</v>
       </c>
       <c r="D500" t="s">
         <v>147</v>
       </c>
-      <c r="G500" s="13" t="s">
-        <v>182</v>
+      <c r="G500" s="7" t="s">
+        <v>965</v>
       </c>
       <c r="H500" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I500" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="501" spans="1:9" x14ac:dyDescent="0.3">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>153</v>
       </c>
@@ -19860,25 +19869,19 @@
         <v>944</v>
       </c>
       <c r="C501" t="s">
-        <v>902</v>
+        <v>952</v>
       </c>
       <c r="D501" t="s">
         <v>147</v>
       </c>
-      <c r="E501" t="s">
-        <v>147</v>
-      </c>
-      <c r="F501" t="s">
-        <v>147</v>
-      </c>
-      <c r="G501" s="7" t="s">
-        <v>904</v>
+      <c r="G501" s="13" t="s">
+        <v>958</v>
       </c>
       <c r="H501" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="502" spans="1:9" x14ac:dyDescent="0.3">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>153</v>
       </c>
@@ -19886,71 +19889,74 @@
         <v>944</v>
       </c>
       <c r="C502" t="s">
+        <v>498</v>
+      </c>
+      <c r="D502" t="s">
+        <v>147</v>
+      </c>
+      <c r="G502" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="H502" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I502" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>153</v>
+      </c>
+      <c r="B503" t="s">
+        <v>944</v>
+      </c>
+      <c r="C503" t="s">
+        <v>902</v>
+      </c>
+      <c r="D503" t="s">
+        <v>147</v>
+      </c>
+      <c r="E503" t="s">
+        <v>147</v>
+      </c>
+      <c r="F503" t="s">
+        <v>147</v>
+      </c>
+      <c r="G503" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H503" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>153</v>
+      </c>
+      <c r="B504" t="s">
+        <v>944</v>
+      </c>
+      <c r="C504" t="s">
         <v>903</v>
       </c>
-      <c r="D502" t="s">
-        <v>147</v>
-      </c>
-      <c r="E502" t="s">
-        <v>147</v>
-      </c>
-      <c r="F502" t="s">
-        <v>147</v>
-      </c>
-      <c r="G502" s="7" t="s">
+      <c r="D504" t="s">
+        <v>147</v>
+      </c>
+      <c r="E504" t="s">
+        <v>147</v>
+      </c>
+      <c r="F504" t="s">
+        <v>147</v>
+      </c>
+      <c r="G504" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H502" s="7" t="s">
+      <c r="H504" s="7" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="503" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A503" t="s">
-        <v>153</v>
-      </c>
-      <c r="B503" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C503" t="s">
-        <v>1011</v>
-      </c>
-      <c r="D503" t="s">
-        <v>147</v>
-      </c>
-      <c r="E503" t="s">
-        <v>147</v>
-      </c>
-      <c r="F503" t="s">
-        <v>147</v>
-      </c>
-      <c r="G503" s="13" t="s">
-        <v>1026</v>
-      </c>
-      <c r="H503" s="7" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="504" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A504" t="s">
-        <v>153</v>
-      </c>
-      <c r="B504" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C504" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D504" t="s">
-        <v>147</v>
-      </c>
-      <c r="G504" s="13" t="s">
-        <v>1028</v>
-      </c>
-      <c r="H504" s="7" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="505" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>153</v>
       </c>
@@ -19958,19 +19964,25 @@
         <v>1009</v>
       </c>
       <c r="C505" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="D505" t="s">
         <v>147</v>
       </c>
+      <c r="E505" t="s">
+        <v>147</v>
+      </c>
+      <c r="F505" t="s">
+        <v>147</v>
+      </c>
       <c r="G505" s="13" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="H505" s="7" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="506" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="506" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>153</v>
       </c>
@@ -19978,19 +19990,19 @@
         <v>1009</v>
       </c>
       <c r="C506" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D506" t="s">
         <v>147</v>
       </c>
-      <c r="G506" s="7" t="s">
-        <v>1033</v>
+      <c r="G506" s="13" t="s">
+        <v>1028</v>
       </c>
       <c r="H506" s="7" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="507" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="507" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>153</v>
       </c>
@@ -19998,22 +20010,19 @@
         <v>1009</v>
       </c>
       <c r="C507" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="D507" t="s">
         <v>147</v>
       </c>
-      <c r="F507" t="s">
-        <v>147</v>
-      </c>
-      <c r="G507" s="12" t="s">
-        <v>1034</v>
+      <c r="G507" s="13" t="s">
+        <v>1030</v>
       </c>
       <c r="H507" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="508" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>153</v>
       </c>
@@ -20021,16 +20030,16 @@
         <v>1009</v>
       </c>
       <c r="C508" t="s">
-        <v>586</v>
+        <v>1014</v>
       </c>
       <c r="D508" t="s">
         <v>147</v>
       </c>
-      <c r="G508" s="12" t="s">
-        <v>1035</v>
+      <c r="G508" s="7" t="s">
+        <v>1033</v>
       </c>
       <c r="H508" s="7" t="s">
-        <v>858</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="509" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20041,16 +20050,19 @@
         <v>1009</v>
       </c>
       <c r="C509" t="s">
-        <v>584</v>
+        <v>1015</v>
       </c>
       <c r="D509" t="s">
         <v>147</v>
       </c>
+      <c r="F509" t="s">
+        <v>147</v>
+      </c>
       <c r="G509" s="12" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="H509" s="7" t="s">
-        <v>857</v>
+        <v>242</v>
       </c>
     </row>
     <row r="510" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20061,16 +20073,16 @@
         <v>1009</v>
       </c>
       <c r="C510" t="s">
-        <v>1016</v>
+        <v>586</v>
       </c>
       <c r="D510" t="s">
         <v>147</v>
       </c>
       <c r="G510" s="12" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="H510" s="7" t="s">
-        <v>1038</v>
+        <v>858</v>
       </c>
     </row>
     <row r="511" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20081,16 +20093,16 @@
         <v>1009</v>
       </c>
       <c r="C511" t="s">
-        <v>1017</v>
+        <v>584</v>
       </c>
       <c r="D511" t="s">
         <v>147</v>
       </c>
       <c r="G511" s="12" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="H511" s="7" t="s">
-        <v>1040</v>
+        <v>857</v>
       </c>
     </row>
     <row r="512" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20101,19 +20113,19 @@
         <v>1009</v>
       </c>
       <c r="C512" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D512" t="s">
         <v>147</v>
       </c>
       <c r="G512" s="12" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="H512" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="513" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="513" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>153</v>
       </c>
@@ -20121,19 +20133,19 @@
         <v>1009</v>
       </c>
       <c r="C513" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D513" t="s">
         <v>147</v>
       </c>
-      <c r="G513" s="7" t="s">
-        <v>1042</v>
+      <c r="G513" s="12" t="s">
+        <v>1039</v>
       </c>
       <c r="H513" s="7" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="514" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="514" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>153</v>
       </c>
@@ -20141,16 +20153,16 @@
         <v>1009</v>
       </c>
       <c r="C514" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="D514" t="s">
         <v>147</v>
       </c>
-      <c r="G514" s="7" t="s">
-        <v>1044</v>
+      <c r="G514" s="12" t="s">
+        <v>1041</v>
       </c>
       <c r="H514" s="7" t="s">
-        <v>1045</v>
+        <v>227</v>
       </c>
     </row>
     <row r="515" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -20161,19 +20173,19 @@
         <v>1009</v>
       </c>
       <c r="C515" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D515" t="s">
         <v>147</v>
       </c>
       <c r="G515" s="7" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="H515" s="7" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="516" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>153</v>
       </c>
@@ -20181,16 +20193,16 @@
         <v>1009</v>
       </c>
       <c r="C516" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D516" t="s">
         <v>147</v>
       </c>
       <c r="G516" s="7" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="H516" s="7" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="517" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -20201,19 +20213,19 @@
         <v>1009</v>
       </c>
       <c r="C517" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D517" t="s">
         <v>147</v>
       </c>
       <c r="G517" s="7" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="H517" s="7" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="518" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="518" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>153</v>
       </c>
@@ -20221,22 +20233,19 @@
         <v>1009</v>
       </c>
       <c r="C518" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D518" t="s">
         <v>147</v>
       </c>
-      <c r="F518" t="s">
-        <v>147</v>
-      </c>
       <c r="G518" s="7" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="H518" s="7" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="519" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="519" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>153</v>
       </c>
@@ -20244,19 +20253,19 @@
         <v>1009</v>
       </c>
       <c r="C519" t="s">
-        <v>559</v>
+        <v>1023</v>
       </c>
       <c r="D519" t="s">
         <v>147</v>
       </c>
       <c r="G519" s="7" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="H519" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="520" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="520" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>153</v>
       </c>
@@ -20264,19 +20273,19 @@
         <v>1009</v>
       </c>
       <c r="C520" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D520" t="s">
         <v>147</v>
       </c>
-      <c r="E520" t="s">
+      <c r="F520" t="s">
         <v>147</v>
       </c>
       <c r="G520" s="7" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="H520" s="7" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="521" spans="1:9" x14ac:dyDescent="0.3">
@@ -20287,22 +20296,16 @@
         <v>1009</v>
       </c>
       <c r="C521" t="s">
-        <v>902</v>
+        <v>559</v>
       </c>
       <c r="D521" t="s">
         <v>147</v>
       </c>
-      <c r="E521" t="s">
-        <v>147</v>
-      </c>
-      <c r="F521" t="s">
-        <v>147</v>
-      </c>
       <c r="G521" s="7" t="s">
-        <v>904</v>
+        <v>1054</v>
       </c>
       <c r="H521" s="7" t="s">
-        <v>906</v>
+        <v>260</v>
       </c>
     </row>
     <row r="522" spans="1:9" x14ac:dyDescent="0.3">
@@ -20313,7 +20316,7 @@
         <v>1009</v>
       </c>
       <c r="C522" t="s">
-        <v>903</v>
+        <v>1025</v>
       </c>
       <c r="D522" t="s">
         <v>147</v>
@@ -20321,14 +20324,11 @@
       <c r="E522" t="s">
         <v>147</v>
       </c>
-      <c r="F522" t="s">
-        <v>147</v>
-      </c>
       <c r="G522" s="7" t="s">
-        <v>905</v>
+        <v>1055</v>
       </c>
       <c r="H522" s="7" t="s">
-        <v>907</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="523" spans="1:9" x14ac:dyDescent="0.3">
@@ -20336,22 +20336,25 @@
         <v>153</v>
       </c>
       <c r="B523" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C523" t="s">
-        <v>398</v>
+        <v>902</v>
       </c>
       <c r="D523" t="s">
         <v>147</v>
       </c>
+      <c r="E523" t="s">
+        <v>147</v>
+      </c>
       <c r="F523" t="s">
         <v>147</v>
       </c>
       <c r="G523" s="7" t="s">
-        <v>1010</v>
+        <v>904</v>
       </c>
       <c r="H523" s="7" t="s">
-        <v>225</v>
+        <v>906</v>
       </c>
     </row>
     <row r="524" spans="1:9" x14ac:dyDescent="0.3">
@@ -20359,10 +20362,10 @@
         <v>153</v>
       </c>
       <c r="B524" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C524" t="s">
-        <v>7</v>
+        <v>903</v>
       </c>
       <c r="D524" t="s">
         <v>147</v>
@@ -20374,13 +20377,10 @@
         <v>147</v>
       </c>
       <c r="G524" s="7" t="s">
-        <v>521</v>
+        <v>905</v>
       </c>
       <c r="H524" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="I524" t="s">
-        <v>937</v>
+        <v>907</v>
       </c>
     </row>
     <row r="525" spans="1:9" x14ac:dyDescent="0.3">
@@ -20391,22 +20391,19 @@
         <v>1058</v>
       </c>
       <c r="C525" t="s">
-        <v>1064</v>
+        <v>398</v>
       </c>
       <c r="D525" t="s">
         <v>147</v>
       </c>
-      <c r="E525" t="s">
-        <v>147</v>
-      </c>
       <c r="F525" t="s">
         <v>147</v>
       </c>
       <c r="G525" s="7" t="s">
-        <v>789</v>
+        <v>1010</v>
       </c>
       <c r="H525" s="7" t="s">
-        <v>789</v>
+        <v>225</v>
       </c>
     </row>
     <row r="526" spans="1:9" x14ac:dyDescent="0.3">
@@ -20417,7 +20414,7 @@
         <v>1058</v>
       </c>
       <c r="C526" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D526" t="s">
         <v>147</v>
@@ -20425,11 +20422,17 @@
       <c r="E526" t="s">
         <v>147</v>
       </c>
+      <c r="F526" t="s">
+        <v>147</v>
+      </c>
       <c r="G526" s="7" t="s">
-        <v>1065</v>
+        <v>521</v>
       </c>
       <c r="H526" s="7" t="s">
-        <v>635</v>
+        <v>291</v>
+      </c>
+      <c r="I526" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="527" spans="1:9" x14ac:dyDescent="0.3">
@@ -20440,7 +20443,7 @@
         <v>1058</v>
       </c>
       <c r="C527" t="s">
-        <v>902</v>
+        <v>1064</v>
       </c>
       <c r="D527" t="s">
         <v>147</v>
@@ -20452,10 +20455,10 @@
         <v>147</v>
       </c>
       <c r="G527" s="7" t="s">
-        <v>904</v>
+        <v>789</v>
       </c>
       <c r="H527" s="7" t="s">
-        <v>906</v>
+        <v>789</v>
       </c>
     </row>
     <row r="528" spans="1:9" x14ac:dyDescent="0.3">
@@ -20466,7 +20469,7 @@
         <v>1058</v>
       </c>
       <c r="C528" t="s">
-        <v>903</v>
+        <v>9</v>
       </c>
       <c r="D528" t="s">
         <v>147</v>
@@ -20474,66 +20477,66 @@
       <c r="E528" t="s">
         <v>147</v>
       </c>
-      <c r="F528" t="s">
-        <v>147</v>
-      </c>
       <c r="G528" s="7" t="s">
-        <v>905</v>
+        <v>1065</v>
       </c>
       <c r="H528" s="7" t="s">
-        <v>907</v>
+        <v>635</v>
       </c>
     </row>
     <row r="529" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="B529" t="s">
-        <v>1074</v>
+        <v>1058</v>
       </c>
       <c r="C529" t="s">
-        <v>398</v>
+        <v>902</v>
       </c>
       <c r="D529" t="s">
         <v>147</v>
       </c>
+      <c r="E529" t="s">
+        <v>147</v>
+      </c>
       <c r="F529" t="s">
         <v>147</v>
       </c>
       <c r="G529" s="7" t="s">
-        <v>1010</v>
+        <v>904</v>
       </c>
       <c r="H529" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="J529" t="s">
-        <v>1177</v>
-      </c>
-      <c r="K529" t="s">
-        <v>1178</v>
-      </c>
-      <c r="L529" t="s">
-        <v>1182</v>
+        <v>906</v>
       </c>
     </row>
     <row r="530" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="B530" t="s">
-        <v>1074</v>
+        <v>1058</v>
       </c>
       <c r="C530" t="s">
-        <v>1102</v>
+        <v>903</v>
+      </c>
+      <c r="D530" t="s">
+        <v>147</v>
+      </c>
+      <c r="E530" t="s">
+        <v>147</v>
+      </c>
+      <c r="F530" t="s">
+        <v>147</v>
       </c>
       <c r="G530" s="7" t="s">
-        <v>1117</v>
+        <v>905</v>
       </c>
       <c r="H530" s="7" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="531" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="531" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>0</v>
       </c>
@@ -20541,7 +20544,7 @@
         <v>1074</v>
       </c>
       <c r="C531" t="s">
-        <v>1103</v>
+        <v>398</v>
       </c>
       <c r="D531" t="s">
         <v>147</v>
@@ -20549,14 +20552,23 @@
       <c r="F531" t="s">
         <v>147</v>
       </c>
-      <c r="G531" s="12" t="s">
-        <v>1119</v>
+      <c r="G531" s="7" t="s">
+        <v>1010</v>
       </c>
       <c r="H531" s="7" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="532" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+      <c r="J531" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K531" t="s">
+        <v>1178</v>
+      </c>
+      <c r="L531" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="532" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>0</v>
       </c>
@@ -20564,16 +20576,13 @@
         <v>1074</v>
       </c>
       <c r="C532" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D532" t="s">
-        <v>147</v>
-      </c>
-      <c r="G532" s="12" t="s">
-        <v>1122</v>
+        <v>1102</v>
+      </c>
+      <c r="G532" s="7" t="s">
+        <v>1117</v>
       </c>
       <c r="H532" s="7" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="533" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20584,7 +20593,7 @@
         <v>1074</v>
       </c>
       <c r="C533" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D533" t="s">
         <v>147</v>
@@ -20593,13 +20602,10 @@
         <v>147</v>
       </c>
       <c r="G533" s="12" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="H533" s="7" t="s">
-        <v>1136</v>
-      </c>
-      <c r="I533" t="s">
-        <v>1175</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="534" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20610,19 +20616,16 @@
         <v>1074</v>
       </c>
       <c r="C534" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D534" t="s">
         <v>147</v>
       </c>
-      <c r="F534" t="s">
-        <v>147</v>
-      </c>
       <c r="G534" s="12" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="H534" s="7" t="s">
-        <v>1137</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="535" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20633,7 +20636,7 @@
         <v>1074</v>
       </c>
       <c r="C535" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D535" t="s">
         <v>147</v>
@@ -20642,10 +20645,13 @@
         <v>147</v>
       </c>
       <c r="G535" s="12" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="H535" s="7" t="s">
-        <v>1138</v>
+        <v>1136</v>
+      </c>
+      <c r="I535" t="s">
+        <v>1175</v>
       </c>
     </row>
     <row r="536" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20656,7 +20662,7 @@
         <v>1074</v>
       </c>
       <c r="C536" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="D536" t="s">
         <v>147</v>
@@ -20665,10 +20671,10 @@
         <v>147</v>
       </c>
       <c r="G536" s="12" t="s">
-        <v>1134</v>
+        <v>1124</v>
       </c>
       <c r="H536" s="7" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="537" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20679,16 +20685,19 @@
         <v>1074</v>
       </c>
       <c r="C537" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D537" t="s">
         <v>147</v>
       </c>
+      <c r="F537" t="s">
+        <v>147</v>
+      </c>
       <c r="G537" s="12" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="H537" s="7" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="538" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20699,16 +20708,19 @@
         <v>1074</v>
       </c>
       <c r="C538" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D538" t="s">
         <v>147</v>
       </c>
+      <c r="F538" t="s">
+        <v>147</v>
+      </c>
       <c r="G538" s="12" t="s">
-        <v>1127</v>
+        <v>1134</v>
       </c>
       <c r="H538" s="7" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="539" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -20719,19 +20731,19 @@
         <v>1074</v>
       </c>
       <c r="C539" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D539" t="s">
         <v>147</v>
       </c>
       <c r="G539" s="12" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="H539" s="7" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="540" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="540" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>0</v>
       </c>
@@ -20739,19 +20751,19 @@
         <v>1074</v>
       </c>
       <c r="C540" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D540" t="s">
         <v>147</v>
       </c>
-      <c r="G540" s="7" t="s">
-        <v>1130</v>
+      <c r="G540" s="12" t="s">
+        <v>1127</v>
       </c>
       <c r="H540" s="7" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="541" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="541" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>0</v>
       </c>
@@ -20759,16 +20771,16 @@
         <v>1074</v>
       </c>
       <c r="C541" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D541" t="s">
         <v>147</v>
       </c>
-      <c r="G541" s="7" t="s">
-        <v>1129</v>
+      <c r="G541" s="12" t="s">
+        <v>1128</v>
       </c>
       <c r="H541" s="7" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="542" spans="1:12" x14ac:dyDescent="0.3">
@@ -20779,16 +20791,16 @@
         <v>1074</v>
       </c>
       <c r="C542" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D542" t="s">
         <v>147</v>
       </c>
       <c r="G542" s="7" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="H542" s="7" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="543" spans="1:12" x14ac:dyDescent="0.3">
@@ -20799,16 +20811,16 @@
         <v>1074</v>
       </c>
       <c r="C543" t="s">
-        <v>576</v>
+        <v>1113</v>
       </c>
       <c r="D543" t="s">
         <v>147</v>
       </c>
       <c r="G543" s="7" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="H543" s="7" t="s">
-        <v>854</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="544" spans="1:12" x14ac:dyDescent="0.3">
@@ -20819,19 +20831,16 @@
         <v>1074</v>
       </c>
       <c r="C544" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D544" t="s">
         <v>147</v>
       </c>
-      <c r="F544" t="s">
-        <v>147</v>
-      </c>
       <c r="G544" s="7" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="H544" s="7" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="545" spans="1:9" x14ac:dyDescent="0.3">
@@ -20842,19 +20851,16 @@
         <v>1074</v>
       </c>
       <c r="C545" t="s">
-        <v>1116</v>
+        <v>576</v>
       </c>
       <c r="D545" t="s">
         <v>147</v>
       </c>
-      <c r="F545" t="s">
-        <v>147</v>
-      </c>
       <c r="G545" s="7" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="H545" s="7" t="s">
-        <v>1147</v>
+        <v>854</v>
       </c>
     </row>
     <row r="546" spans="1:9" x14ac:dyDescent="0.3">
@@ -20865,22 +20871,19 @@
         <v>1074</v>
       </c>
       <c r="C546" t="s">
-        <v>902</v>
+        <v>1115</v>
       </c>
       <c r="D546" t="s">
         <v>147</v>
       </c>
-      <c r="E546" t="s">
-        <v>147</v>
-      </c>
       <c r="F546" t="s">
         <v>147</v>
       </c>
       <c r="G546" s="7" t="s">
-        <v>904</v>
+        <v>1133</v>
       </c>
       <c r="H546" s="7" t="s">
-        <v>906</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="547" spans="1:9" x14ac:dyDescent="0.3">
@@ -20891,22 +20894,19 @@
         <v>1074</v>
       </c>
       <c r="C547" t="s">
-        <v>903</v>
+        <v>1116</v>
       </c>
       <c r="D547" t="s">
         <v>147</v>
       </c>
-      <c r="E547" t="s">
-        <v>147</v>
-      </c>
       <c r="F547" t="s">
         <v>147</v>
       </c>
       <c r="G547" s="7" t="s">
-        <v>905</v>
+        <v>1135</v>
       </c>
       <c r="H547" s="7" t="s">
-        <v>907</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="548" spans="1:9" x14ac:dyDescent="0.3">
@@ -20914,22 +20914,25 @@
         <v>0</v>
       </c>
       <c r="B548" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C548" t="s">
-        <v>1148</v>
+        <v>902</v>
       </c>
       <c r="D548" t="s">
         <v>147</v>
       </c>
+      <c r="E548" t="s">
+        <v>147</v>
+      </c>
       <c r="F548" t="s">
         <v>147</v>
       </c>
       <c r="G548" s="7" t="s">
-        <v>1010</v>
+        <v>904</v>
       </c>
       <c r="H548" s="7" t="s">
-        <v>225</v>
+        <v>906</v>
       </c>
     </row>
     <row r="549" spans="1:9" x14ac:dyDescent="0.3">
@@ -20937,10 +20940,10 @@
         <v>0</v>
       </c>
       <c r="B549" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C549" t="s">
-        <v>7</v>
+        <v>903</v>
       </c>
       <c r="D549" t="s">
         <v>147</v>
@@ -20952,13 +20955,10 @@
         <v>147</v>
       </c>
       <c r="G549" s="7" t="s">
-        <v>521</v>
+        <v>905</v>
       </c>
       <c r="H549" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="I549" t="s">
-        <v>937</v>
+        <v>907</v>
       </c>
     </row>
     <row r="550" spans="1:9" x14ac:dyDescent="0.3">
@@ -20969,22 +20969,19 @@
         <v>1075</v>
       </c>
       <c r="C550" t="s">
-        <v>1064</v>
+        <v>1148</v>
       </c>
       <c r="D550" t="s">
         <v>147</v>
       </c>
-      <c r="E550" t="s">
-        <v>147</v>
-      </c>
       <c r="F550" t="s">
         <v>147</v>
       </c>
       <c r="G550" s="7" t="s">
-        <v>789</v>
+        <v>1010</v>
       </c>
       <c r="H550" s="7" t="s">
-        <v>789</v>
+        <v>225</v>
       </c>
     </row>
     <row r="551" spans="1:9" x14ac:dyDescent="0.3">
@@ -20995,7 +20992,7 @@
         <v>1075</v>
       </c>
       <c r="C551" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D551" t="s">
         <v>147</v>
@@ -21003,11 +21000,17 @@
       <c r="E551" t="s">
         <v>147</v>
       </c>
+      <c r="F551" t="s">
+        <v>147</v>
+      </c>
       <c r="G551" s="7" t="s">
-        <v>1065</v>
+        <v>521</v>
       </c>
       <c r="H551" s="7" t="s">
-        <v>635</v>
+        <v>291</v>
+      </c>
+      <c r="I551" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="552" spans="1:9" x14ac:dyDescent="0.3">
@@ -21018,7 +21021,7 @@
         <v>1075</v>
       </c>
       <c r="C552" t="s">
-        <v>902</v>
+        <v>1064</v>
       </c>
       <c r="D552" t="s">
         <v>147</v>
@@ -21030,10 +21033,10 @@
         <v>147</v>
       </c>
       <c r="G552" s="7" t="s">
-        <v>904</v>
+        <v>789</v>
       </c>
       <c r="H552" s="7" t="s">
-        <v>906</v>
+        <v>789</v>
       </c>
     </row>
     <row r="553" spans="1:9" x14ac:dyDescent="0.3">
@@ -21044,7 +21047,7 @@
         <v>1075</v>
       </c>
       <c r="C553" t="s">
-        <v>903</v>
+        <v>9</v>
       </c>
       <c r="D553" t="s">
         <v>147</v>
@@ -21052,25 +21055,22 @@
       <c r="E553" t="s">
         <v>147</v>
       </c>
-      <c r="F553" t="s">
-        <v>147</v>
-      </c>
       <c r="G553" s="7" t="s">
-        <v>905</v>
+        <v>1065</v>
       </c>
       <c r="H553" s="7" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="554" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>0</v>
       </c>
       <c r="B554" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C554" t="s">
-        <v>11</v>
+        <v>902</v>
       </c>
       <c r="D554" t="s">
         <v>147</v>
@@ -21081,14 +21081,11 @@
       <c r="F554" t="s">
         <v>147</v>
       </c>
-      <c r="G554" s="12" t="s">
-        <v>1149</v>
+      <c r="G554" s="7" t="s">
+        <v>904</v>
       </c>
       <c r="H554" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I554" t="s">
-        <v>934</v>
+        <v>906</v>
       </c>
     </row>
     <row r="555" spans="1:9" x14ac:dyDescent="0.3">
@@ -21096,25 +21093,28 @@
         <v>0</v>
       </c>
       <c r="B555" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C555" t="s">
-        <v>1148</v>
+        <v>903</v>
       </c>
       <c r="D555" t="s">
         <v>147</v>
       </c>
+      <c r="E555" t="s">
+        <v>147</v>
+      </c>
       <c r="F555" t="s">
         <v>147</v>
       </c>
       <c r="G555" s="7" t="s">
-        <v>1010</v>
+        <v>905</v>
       </c>
       <c r="H555" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="556" spans="1:9" x14ac:dyDescent="0.3">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>0</v>
       </c>
@@ -21122,7 +21122,7 @@
         <v>1076</v>
       </c>
       <c r="C556" t="s">
-        <v>1150</v>
+        <v>11</v>
       </c>
       <c r="D556" t="s">
         <v>147</v>
@@ -21133,14 +21133,14 @@
       <c r="F556" t="s">
         <v>147</v>
       </c>
-      <c r="G556" s="7" t="s">
-        <v>135</v>
+      <c r="G556" s="12" t="s">
+        <v>1149</v>
       </c>
       <c r="H556" s="7" t="s">
-        <v>1151</v>
+        <v>103</v>
       </c>
       <c r="I556" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.3">
@@ -21151,22 +21151,19 @@
         <v>1076</v>
       </c>
       <c r="C557" t="s">
-        <v>41</v>
+        <v>1148</v>
       </c>
       <c r="D557" t="s">
         <v>147</v>
       </c>
-      <c r="E557" t="s">
-        <v>147</v>
-      </c>
       <c r="F557" t="s">
         <v>147</v>
       </c>
       <c r="G557" s="7" t="s">
-        <v>485</v>
+        <v>1010</v>
       </c>
       <c r="H557" s="7" t="s">
-        <v>658</v>
+        <v>225</v>
       </c>
     </row>
     <row r="558" spans="1:9" x14ac:dyDescent="0.3">
@@ -21177,7 +21174,7 @@
         <v>1076</v>
       </c>
       <c r="C558" t="s">
-        <v>902</v>
+        <v>1150</v>
       </c>
       <c r="D558" t="s">
         <v>147</v>
@@ -21189,10 +21186,13 @@
         <v>147</v>
       </c>
       <c r="G558" s="7" t="s">
-        <v>904</v>
+        <v>135</v>
       </c>
       <c r="H558" s="7" t="s">
-        <v>906</v>
+        <v>1151</v>
+      </c>
+      <c r="I558" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="559" spans="1:9" x14ac:dyDescent="0.3">
@@ -21203,7 +21203,7 @@
         <v>1076</v>
       </c>
       <c r="C559" t="s">
-        <v>903</v>
+        <v>41</v>
       </c>
       <c r="D559" t="s">
         <v>147</v>
@@ -21215,10 +21215,10 @@
         <v>147</v>
       </c>
       <c r="G559" s="7" t="s">
-        <v>905</v>
+        <v>485</v>
       </c>
       <c r="H559" s="7" t="s">
-        <v>907</v>
+        <v>658</v>
       </c>
     </row>
     <row r="560" spans="1:9" x14ac:dyDescent="0.3">
@@ -21226,10 +21226,10 @@
         <v>0</v>
       </c>
       <c r="B560" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C560" t="s">
-        <v>1152</v>
+        <v>902</v>
       </c>
       <c r="D560" t="s">
         <v>147</v>
@@ -21241,10 +21241,10 @@
         <v>147</v>
       </c>
       <c r="G560" s="7" t="s">
-        <v>1156</v>
+        <v>904</v>
       </c>
       <c r="H560" s="7" t="s">
-        <v>1154</v>
+        <v>906</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.3">
@@ -21252,10 +21252,10 @@
         <v>0</v>
       </c>
       <c r="B561" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C561" t="s">
-        <v>1153</v>
+        <v>903</v>
       </c>
       <c r="D561" t="s">
         <v>147</v>
@@ -21267,10 +21267,10 @@
         <v>147</v>
       </c>
       <c r="G561" s="7" t="s">
-        <v>1155</v>
+        <v>905</v>
       </c>
       <c r="H561" s="7" t="s">
-        <v>783</v>
+        <v>907</v>
       </c>
     </row>
     <row r="562" spans="1:9" x14ac:dyDescent="0.3">
@@ -21281,7 +21281,7 @@
         <v>1077</v>
       </c>
       <c r="C562" t="s">
-        <v>902</v>
+        <v>1152</v>
       </c>
       <c r="D562" t="s">
         <v>147</v>
@@ -21293,10 +21293,10 @@
         <v>147</v>
       </c>
       <c r="G562" s="7" t="s">
-        <v>904</v>
+        <v>1156</v>
       </c>
       <c r="H562" s="7" t="s">
-        <v>906</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="563" spans="1:9" x14ac:dyDescent="0.3">
@@ -21307,7 +21307,7 @@
         <v>1077</v>
       </c>
       <c r="C563" t="s">
-        <v>903</v>
+        <v>1153</v>
       </c>
       <c r="D563" t="s">
         <v>147</v>
@@ -21319,10 +21319,10 @@
         <v>147</v>
       </c>
       <c r="G563" s="7" t="s">
-        <v>905</v>
+        <v>1155</v>
       </c>
       <c r="H563" s="7" t="s">
-        <v>907</v>
+        <v>783</v>
       </c>
     </row>
     <row r="564" spans="1:9" x14ac:dyDescent="0.3">
@@ -21330,22 +21330,25 @@
         <v>0</v>
       </c>
       <c r="B564" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C564" t="s">
-        <v>4</v>
+        <v>902</v>
       </c>
       <c r="D564" t="s">
         <v>147</v>
       </c>
+      <c r="E564" t="s">
+        <v>147</v>
+      </c>
       <c r="F564" t="s">
         <v>147</v>
       </c>
       <c r="G564" s="7" t="s">
-        <v>1086</v>
+        <v>904</v>
       </c>
       <c r="H564" s="7" t="s">
-        <v>1087</v>
+        <v>906</v>
       </c>
     </row>
     <row r="565" spans="1:9" x14ac:dyDescent="0.3">
@@ -21353,10 +21356,10 @@
         <v>0</v>
       </c>
       <c r="B565" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C565" t="s">
-        <v>45</v>
+        <v>903</v>
       </c>
       <c r="D565" t="s">
         <v>147</v>
@@ -21368,13 +21371,10 @@
         <v>147</v>
       </c>
       <c r="G565" s="7" t="s">
-        <v>253</v>
+        <v>905</v>
       </c>
       <c r="H565" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="I565" t="s">
-        <v>1000</v>
+        <v>907</v>
       </c>
     </row>
     <row r="566" spans="1:9" x14ac:dyDescent="0.3">
@@ -21385,22 +21385,19 @@
         <v>1078</v>
       </c>
       <c r="C566" t="s">
-        <v>902</v>
+        <v>4</v>
       </c>
       <c r="D566" t="s">
         <v>147</v>
       </c>
-      <c r="E566" t="s">
-        <v>147</v>
-      </c>
       <c r="F566" t="s">
         <v>147</v>
       </c>
       <c r="G566" s="7" t="s">
-        <v>904</v>
+        <v>1086</v>
       </c>
       <c r="H566" s="7" t="s">
-        <v>906</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="567" spans="1:9" x14ac:dyDescent="0.3">
@@ -21411,7 +21408,7 @@
         <v>1078</v>
       </c>
       <c r="C567" t="s">
-        <v>903</v>
+        <v>45</v>
       </c>
       <c r="D567" t="s">
         <v>147</v>
@@ -21423,10 +21420,13 @@
         <v>147</v>
       </c>
       <c r="G567" s="7" t="s">
-        <v>905</v>
+        <v>253</v>
       </c>
       <c r="H567" s="7" t="s">
-        <v>907</v>
+        <v>254</v>
+      </c>
+      <c r="I567" t="s">
+        <v>1000</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.3">
@@ -21434,22 +21434,25 @@
         <v>0</v>
       </c>
       <c r="B568" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C568" t="s">
-        <v>4</v>
+        <v>902</v>
       </c>
       <c r="D568" t="s">
         <v>147</v>
       </c>
+      <c r="E568" t="s">
+        <v>147</v>
+      </c>
       <c r="F568" t="s">
         <v>147</v>
       </c>
       <c r="G568" s="7" t="s">
-        <v>1086</v>
+        <v>904</v>
       </c>
       <c r="H568" s="7" t="s">
-        <v>1087</v>
+        <v>906</v>
       </c>
     </row>
     <row r="569" spans="1:9" x14ac:dyDescent="0.3">
@@ -21457,10 +21460,10 @@
         <v>0</v>
       </c>
       <c r="B569" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C569" t="s">
-        <v>1157</v>
+        <v>903</v>
       </c>
       <c r="D569" t="s">
         <v>147</v>
@@ -21472,13 +21475,10 @@
         <v>147</v>
       </c>
       <c r="G569" s="7" t="s">
-        <v>421</v>
+        <v>905</v>
       </c>
       <c r="H569" s="7" t="s">
-        <v>1158</v>
-      </c>
-      <c r="I569" t="s">
-        <v>1172</v>
+        <v>907</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.3">
@@ -21489,25 +21489,22 @@
         <v>1079</v>
       </c>
       <c r="C570" t="s">
-        <v>902</v>
+        <v>4</v>
       </c>
       <c r="D570" t="s">
         <v>147</v>
       </c>
-      <c r="E570" t="s">
-        <v>147</v>
-      </c>
       <c r="F570" t="s">
         <v>147</v>
       </c>
       <c r="G570" s="7" t="s">
-        <v>904</v>
+        <v>1086</v>
       </c>
       <c r="H570" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="571" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="571" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>0</v>
       </c>
@@ -21515,7 +21512,7 @@
         <v>1079</v>
       </c>
       <c r="C571" t="s">
-        <v>903</v>
+        <v>1157</v>
       </c>
       <c r="D571" t="s">
         <v>147</v>
@@ -21527,10 +21524,13 @@
         <v>147</v>
       </c>
       <c r="G571" s="7" t="s">
-        <v>905</v>
+        <v>421</v>
       </c>
       <c r="H571" s="7" t="s">
-        <v>907</v>
+        <v>1158</v>
+      </c>
+      <c r="I571" t="s">
+        <v>1172</v>
       </c>
     </row>
     <row r="572" spans="1:9" x14ac:dyDescent="0.3">
@@ -21538,33 +21538,36 @@
         <v>0</v>
       </c>
       <c r="B572" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C572" t="s">
-        <v>1159</v>
+        <v>902</v>
       </c>
       <c r="D572" t="s">
         <v>147</v>
       </c>
+      <c r="E572" t="s">
+        <v>147</v>
+      </c>
       <c r="F572" t="s">
         <v>147</v>
       </c>
       <c r="G572" s="7" t="s">
-        <v>1164</v>
+        <v>904</v>
       </c>
       <c r="H572" s="7" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="573" spans="1:9" x14ac:dyDescent="0.3">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="573" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>0</v>
       </c>
       <c r="B573" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C573" t="s">
-        <v>1160</v>
+        <v>903</v>
       </c>
       <c r="D573" t="s">
         <v>147</v>
@@ -21576,10 +21579,10 @@
         <v>147</v>
       </c>
       <c r="G573" s="7" t="s">
-        <v>1161</v>
+        <v>905</v>
       </c>
       <c r="H573" s="7" t="s">
-        <v>1162</v>
+        <v>907</v>
       </c>
     </row>
     <row r="574" spans="1:9" x14ac:dyDescent="0.3">
@@ -21590,22 +21593,19 @@
         <v>1080</v>
       </c>
       <c r="C574" t="s">
-        <v>902</v>
+        <v>1159</v>
       </c>
       <c r="D574" t="s">
         <v>147</v>
       </c>
-      <c r="E574" t="s">
-        <v>147</v>
-      </c>
       <c r="F574" t="s">
         <v>147</v>
       </c>
       <c r="G574" s="7" t="s">
-        <v>904</v>
+        <v>1164</v>
       </c>
       <c r="H574" s="7" t="s">
-        <v>906</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="575" spans="1:9" x14ac:dyDescent="0.3">
@@ -21616,26 +21616,78 @@
         <v>1080</v>
       </c>
       <c r="C575" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D575" t="s">
+        <v>147</v>
+      </c>
+      <c r="E575" t="s">
+        <v>147</v>
+      </c>
+      <c r="F575" t="s">
+        <v>147</v>
+      </c>
+      <c r="G575" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H575" s="7" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="576" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A576" t="s">
+        <v>0</v>
+      </c>
+      <c r="B576" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C576" t="s">
+        <v>902</v>
+      </c>
+      <c r="D576" t="s">
+        <v>147</v>
+      </c>
+      <c r="E576" t="s">
+        <v>147</v>
+      </c>
+      <c r="F576" t="s">
+        <v>147</v>
+      </c>
+      <c r="G576" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H576" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A577" t="s">
+        <v>0</v>
+      </c>
+      <c r="B577" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C577" t="s">
         <v>903</v>
       </c>
-      <c r="D575" t="s">
-        <v>147</v>
-      </c>
-      <c r="E575" t="s">
-        <v>147</v>
-      </c>
-      <c r="F575" t="s">
-        <v>147</v>
-      </c>
-      <c r="G575" s="7" t="s">
+      <c r="D577" t="s">
+        <v>147</v>
+      </c>
+      <c r="E577" t="s">
+        <v>147</v>
+      </c>
+      <c r="F577" t="s">
+        <v>147</v>
+      </c>
+      <c r="G577" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H575" s="7" t="s">
+      <c r="H577" s="7" t="s">
         <v>907</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C568"/>
+  <autoFilter ref="A1:C570"/>
   <sortState ref="A2:H552">
     <sortCondition ref="B2:B552"/>
   </sortState>

</xml_diff>

<commit_message>
Small fix for localization
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5391" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5397" uniqueCount="1220">
   <si>
     <t>DATA</t>
   </si>
@@ -3809,6 +3809,9 @@
   </si>
   <si>
     <t>Settings/SysColumns</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -4251,11 +4254,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="P86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N92" sqref="N92"/>
+      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6199,6 +6202,9 @@
       <c r="C66" t="s">
         <v>1057</v>
       </c>
+      <c r="D66" t="s">
+        <v>1219</v>
+      </c>
       <c r="G66" t="s">
         <v>147</v>
       </c>
@@ -6228,6 +6234,9 @@
       <c r="C67" t="s">
         <v>1057</v>
       </c>
+      <c r="D67" t="s">
+        <v>1219</v>
+      </c>
       <c r="K67" t="s">
         <v>891</v>
       </c>
@@ -6257,6 +6266,9 @@
       <c r="C68" t="s">
         <v>1057</v>
       </c>
+      <c r="D68" t="s">
+        <v>1219</v>
+      </c>
       <c r="J68" t="s">
         <v>1202</v>
       </c>
@@ -6301,6 +6313,9 @@
       <c r="C69" t="s">
         <v>1057</v>
       </c>
+      <c r="D69" t="s">
+        <v>1219</v>
+      </c>
       <c r="J69" t="s">
         <v>223</v>
       </c>
@@ -6977,6 +6992,9 @@
       <c r="C92" t="s">
         <v>1057</v>
       </c>
+      <c r="D92" t="s">
+        <v>1219</v>
+      </c>
       <c r="G92" t="s">
         <v>147</v>
       </c>
@@ -7191,6 +7209,9 @@
       </c>
       <c r="C99" t="s">
         <v>1057</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1219</v>
       </c>
       <c r="J99" t="s">
         <v>1213</v>
@@ -7571,7 +7592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M577"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D323" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Small fix for saving password
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412"/>
+    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5397" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="1220">
   <si>
     <t>DATA</t>
   </si>
@@ -4254,11 +4254,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P86" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="P50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21767,11 +21767,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21811,6 +21811,9 @@
         <v>766</v>
       </c>
       <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some small fixes for Settings tab
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="web.Model{C}" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$568</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$572</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tables{T}'!$A$1:$L$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'web.Model{C}'!$A$1:$C$380</definedName>
   </definedNames>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5384" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5422" uniqueCount="1220">
   <si>
     <t>DATA</t>
   </si>
@@ -3790,9 +3790,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>ChangePassword</t>
-  </si>
-  <si>
     <t>sysTableId</t>
   </si>
   <si>
@@ -3800,6 +3797,21 @@
   </si>
   <si>
     <t>editModeType</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>DE: Columns</t>
+  </si>
+  <si>
+    <t>sysColumns</t>
+  </si>
+  <si>
+    <t>Settings/SysColumns</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -4243,10 +4255,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J113" sqref="J113"/>
+      <selection pane="bottomRight" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6190,6 +6202,9 @@
       <c r="C66" t="s">
         <v>1057</v>
       </c>
+      <c r="D66" t="s">
+        <v>1219</v>
+      </c>
       <c r="G66" t="s">
         <v>147</v>
       </c>
@@ -6219,6 +6234,9 @@
       <c r="C67" t="s">
         <v>1057</v>
       </c>
+      <c r="D67" t="s">
+        <v>1219</v>
+      </c>
       <c r="K67" t="s">
         <v>891</v>
       </c>
@@ -6248,6 +6266,9 @@
       <c r="C68" t="s">
         <v>1057</v>
       </c>
+      <c r="D68" t="s">
+        <v>1219</v>
+      </c>
       <c r="J68" t="s">
         <v>1202</v>
       </c>
@@ -6292,6 +6313,9 @@
       <c r="C69" t="s">
         <v>1057</v>
       </c>
+      <c r="D69" t="s">
+        <v>1219</v>
+      </c>
       <c r="J69" t="s">
         <v>223</v>
       </c>
@@ -6968,11 +6992,17 @@
       <c r="C92" t="s">
         <v>1057</v>
       </c>
+      <c r="D92" t="s">
+        <v>1219</v>
+      </c>
       <c r="G92" t="s">
         <v>147</v>
       </c>
       <c r="H92" t="s">
-        <v>1213</v>
+        <v>1212</v>
+      </c>
+      <c r="I92" t="s">
+        <v>778</v>
       </c>
       <c r="K92" t="s">
         <v>895</v>
@@ -6980,9 +7010,6 @@
       <c r="L92" t="s">
         <v>899</v>
       </c>
-      <c r="N92" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -7183,8 +7210,11 @@
       <c r="C99" t="s">
         <v>1057</v>
       </c>
+      <c r="D99" t="s">
+        <v>1219</v>
+      </c>
       <c r="J99" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K99" t="s">
         <v>894</v>
@@ -7193,6 +7223,21 @@
         <v>900</v>
       </c>
       <c r="N99" t="s">
+        <v>147</v>
+      </c>
+      <c r="O99" s="7" t="s">
+        <v>1218</v>
+      </c>
+      <c r="P99" t="s">
+        <v>1217</v>
+      </c>
+      <c r="Q99" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>1215</v>
+      </c>
+      <c r="U99" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7548,13 +7593,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M575"/>
+  <dimension ref="A1:M579"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I530" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D326" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M546" sqref="M546"/>
+      <selection pane="bottomRight" activeCell="E332" sqref="E332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15774,6 +15819,9 @@
       <c r="D332" t="s">
         <v>147</v>
       </c>
+      <c r="E332" t="s">
+        <v>147</v>
+      </c>
       <c r="F332" t="s">
         <v>147</v>
       </c>
@@ -15797,6 +15845,9 @@
       <c r="D333" t="s">
         <v>147</v>
       </c>
+      <c r="E333" t="s">
+        <v>147</v>
+      </c>
       <c r="F333" t="s">
         <v>147</v>
       </c>
@@ -15885,7 +15936,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>153</v>
       </c>
@@ -15898,9 +15949,6 @@
       <c r="D337" t="s">
         <v>147</v>
       </c>
-      <c r="E337" t="s">
-        <v>147</v>
-      </c>
       <c r="F337" t="s">
         <v>147</v>
       </c>
@@ -15914,7 +15962,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>153</v>
       </c>
@@ -15943,7 +15991,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>153</v>
       </c>
@@ -15969,7 +16017,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>153</v>
       </c>
@@ -15995,7 +16043,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>153</v>
       </c>
@@ -16021,7 +16069,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>153</v>
       </c>
@@ -16047,7 +16095,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>153</v>
       </c>
@@ -16069,11 +16117,8 @@
       <c r="H343" s="7" t="s">
         <v>1211</v>
       </c>
-      <c r="J343" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>153</v>
       </c>
@@ -16102,7 +16147,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>153</v>
       </c>
@@ -16128,7 +16173,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>153</v>
       </c>
@@ -16154,7 +16199,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>153</v>
       </c>
@@ -16180,7 +16225,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>153</v>
       </c>
@@ -16203,7 +16248,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>153</v>
       </c>
@@ -16229,7 +16274,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>153</v>
       </c>
@@ -16255,7 +16300,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>153</v>
       </c>
@@ -16281,7 +16326,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>153</v>
       </c>
@@ -18782,7 +18827,7 @@
         <v>779</v>
       </c>
       <c r="C454" t="s">
-        <v>780</v>
+        <v>12</v>
       </c>
       <c r="D454" t="s">
         <v>147</v>
@@ -18790,11 +18835,14 @@
       <c r="E454" t="s">
         <v>147</v>
       </c>
+      <c r="F454" t="s">
+        <v>147</v>
+      </c>
       <c r="G454" s="7" t="s">
-        <v>873</v>
+        <v>789</v>
       </c>
       <c r="H454" s="7" t="s">
-        <v>91</v>
+        <v>789</v>
       </c>
     </row>
     <row r="455" spans="1:8" x14ac:dyDescent="0.3">
@@ -18805,19 +18853,16 @@
         <v>779</v>
       </c>
       <c r="C455" t="s">
-        <v>9</v>
+        <v>780</v>
       </c>
       <c r="D455" t="s">
         <v>147</v>
       </c>
-      <c r="E455" t="s">
-        <v>147</v>
-      </c>
       <c r="G455" s="7" t="s">
-        <v>484</v>
+        <v>873</v>
       </c>
       <c r="H455" s="7" t="s">
-        <v>635</v>
+        <v>91</v>
       </c>
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.3">
@@ -18828,7 +18873,7 @@
         <v>779</v>
       </c>
       <c r="C456" t="s">
-        <v>781</v>
+        <v>9</v>
       </c>
       <c r="D456" t="s">
         <v>147</v>
@@ -18837,10 +18882,10 @@
         <v>147</v>
       </c>
       <c r="G456" s="7" t="s">
-        <v>874</v>
+        <v>484</v>
       </c>
       <c r="H456" s="7" t="s">
-        <v>877</v>
+        <v>635</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.3">
@@ -18848,10 +18893,10 @@
         <v>153</v>
       </c>
       <c r="B457" t="s">
-        <v>286</v>
+        <v>779</v>
       </c>
       <c r="C457" t="s">
-        <v>363</v>
+        <v>781</v>
       </c>
       <c r="D457" t="s">
         <v>147</v>
@@ -18859,14 +18904,11 @@
       <c r="E457" t="s">
         <v>147</v>
       </c>
-      <c r="F457" t="s">
-        <v>147</v>
-      </c>
       <c r="G457" s="7" t="s">
-        <v>529</v>
+        <v>874</v>
       </c>
       <c r="H457" s="7" t="s">
-        <v>785</v>
+        <v>877</v>
       </c>
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.3">
@@ -18877,7 +18919,7 @@
         <v>286</v>
       </c>
       <c r="C458" t="s">
-        <v>12</v>
+        <v>363</v>
       </c>
       <c r="D458" t="s">
         <v>147</v>
@@ -18885,11 +18927,14 @@
       <c r="E458" t="s">
         <v>147</v>
       </c>
+      <c r="F458" t="s">
+        <v>147</v>
+      </c>
       <c r="G458" s="7" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="H458" s="7" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.3">
@@ -18900,7 +18945,7 @@
         <v>286</v>
       </c>
       <c r="C459" t="s">
-        <v>534</v>
+        <v>12</v>
       </c>
       <c r="D459" t="s">
         <v>147</v>
@@ -18909,10 +18954,10 @@
         <v>147</v>
       </c>
       <c r="G459" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H459" s="7" t="s">
-        <v>841</v>
+        <v>789</v>
       </c>
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.3">
@@ -18923,7 +18968,7 @@
         <v>286</v>
       </c>
       <c r="C460" t="s">
-        <v>902</v>
+        <v>534</v>
       </c>
       <c r="D460" t="s">
         <v>147</v>
@@ -18931,14 +18976,11 @@
       <c r="E460" t="s">
         <v>147</v>
       </c>
-      <c r="F460" t="s">
-        <v>147</v>
-      </c>
       <c r="G460" s="7" t="s">
-        <v>904</v>
+        <v>535</v>
       </c>
       <c r="H460" s="7" t="s">
-        <v>906</v>
+        <v>841</v>
       </c>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.3">
@@ -18949,7 +18991,7 @@
         <v>286</v>
       </c>
       <c r="C461" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D461" t="s">
         <v>147</v>
@@ -18961,10 +19003,10 @@
         <v>147</v>
       </c>
       <c r="G461" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H461" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.3">
@@ -18972,10 +19014,10 @@
         <v>153</v>
       </c>
       <c r="B462" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C462" t="s">
-        <v>363</v>
+        <v>903</v>
       </c>
       <c r="D462" t="s">
         <v>147</v>
@@ -18987,10 +19029,10 @@
         <v>147</v>
       </c>
       <c r="G462" s="7" t="s">
-        <v>521</v>
+        <v>905</v>
       </c>
       <c r="H462" s="7" t="s">
-        <v>785</v>
+        <v>907</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.3">
@@ -19001,7 +19043,7 @@
         <v>289</v>
       </c>
       <c r="C463" t="s">
-        <v>536</v>
+        <v>363</v>
       </c>
       <c r="D463" t="s">
         <v>147</v>
@@ -19009,14 +19051,17 @@
       <c r="E463" t="s">
         <v>147</v>
       </c>
+      <c r="F463" t="s">
+        <v>147</v>
+      </c>
       <c r="G463" s="7" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="H463" s="7" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="464" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>153</v>
       </c>
@@ -19024,16 +19069,19 @@
         <v>289</v>
       </c>
       <c r="C464" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D464" t="s">
         <v>147</v>
       </c>
+      <c r="E464" t="s">
+        <v>147</v>
+      </c>
       <c r="G464" s="7" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H464" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="465" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -19044,19 +19092,19 @@
         <v>289</v>
       </c>
       <c r="C465" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D465" t="s">
         <v>147</v>
       </c>
       <c r="G465" s="7" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H465" s="7" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="466" spans="1:9" x14ac:dyDescent="0.3">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>153</v>
       </c>
@@ -19064,19 +19112,16 @@
         <v>289</v>
       </c>
       <c r="C466" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D466" t="s">
         <v>147</v>
       </c>
-      <c r="E466" t="s">
-        <v>147</v>
-      </c>
       <c r="G466" s="7" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H466" s="7" t="s">
-        <v>635</v>
+        <v>844</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.3">
@@ -19087,7 +19132,7 @@
         <v>289</v>
       </c>
       <c r="C467" t="s">
-        <v>902</v>
+        <v>542</v>
       </c>
       <c r="D467" t="s">
         <v>147</v>
@@ -19095,14 +19140,11 @@
       <c r="E467" t="s">
         <v>147</v>
       </c>
-      <c r="F467" t="s">
-        <v>147</v>
-      </c>
       <c r="G467" s="7" t="s">
-        <v>904</v>
+        <v>543</v>
       </c>
       <c r="H467" s="7" t="s">
-        <v>906</v>
+        <v>635</v>
       </c>
     </row>
     <row r="468" spans="1:9" x14ac:dyDescent="0.3">
@@ -19113,7 +19155,7 @@
         <v>289</v>
       </c>
       <c r="C468" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D468" t="s">
         <v>147</v>
@@ -19125,10 +19167,10 @@
         <v>147</v>
       </c>
       <c r="G468" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H468" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -19136,10 +19178,10 @@
         <v>153</v>
       </c>
       <c r="B469" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="C469" t="s">
-        <v>506</v>
+        <v>903</v>
       </c>
       <c r="D469" t="s">
         <v>147</v>
@@ -19151,10 +19193,10 @@
         <v>147</v>
       </c>
       <c r="G469" s="7" t="s">
-        <v>263</v>
+        <v>905</v>
       </c>
       <c r="H469" s="7" t="s">
-        <v>264</v>
+        <v>907</v>
       </c>
     </row>
     <row r="470" spans="1:9" x14ac:dyDescent="0.3">
@@ -19165,7 +19207,7 @@
         <v>261</v>
       </c>
       <c r="C470" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D470" t="s">
         <v>147</v>
@@ -19173,11 +19215,14 @@
       <c r="E470" t="s">
         <v>147</v>
       </c>
+      <c r="F470" t="s">
+        <v>147</v>
+      </c>
       <c r="G470" s="7" t="s">
-        <v>508</v>
+        <v>263</v>
       </c>
       <c r="H470" s="7" t="s">
-        <v>838</v>
+        <v>264</v>
       </c>
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.3">
@@ -19188,19 +19233,19 @@
         <v>261</v>
       </c>
       <c r="C471" t="s">
-        <v>16</v>
+        <v>507</v>
       </c>
       <c r="D471" t="s">
         <v>147</v>
       </c>
+      <c r="E471" t="s">
+        <v>147</v>
+      </c>
       <c r="G471" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H471" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I471" t="s">
-        <v>974</v>
+        <v>838</v>
       </c>
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.3">
@@ -19211,19 +19256,19 @@
         <v>261</v>
       </c>
       <c r="C472" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D472" t="s">
         <v>147</v>
       </c>
       <c r="G472" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H472" s="7" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="I472" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.3">
@@ -19234,22 +19279,19 @@
         <v>261</v>
       </c>
       <c r="C473" t="s">
-        <v>902</v>
+        <v>55</v>
       </c>
       <c r="D473" t="s">
         <v>147</v>
       </c>
-      <c r="E473" t="s">
-        <v>147</v>
-      </c>
-      <c r="F473" t="s">
-        <v>147</v>
-      </c>
       <c r="G473" s="7" t="s">
-        <v>904</v>
+        <v>510</v>
       </c>
       <c r="H473" s="7" t="s">
-        <v>906</v>
+        <v>281</v>
+      </c>
+      <c r="I473" t="s">
+        <v>975</v>
       </c>
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.3">
@@ -19260,7 +19302,7 @@
         <v>261</v>
       </c>
       <c r="C474" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D474" t="s">
         <v>147</v>
@@ -19272,10 +19314,10 @@
         <v>147</v>
       </c>
       <c r="G474" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H474" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="475" spans="1:9" x14ac:dyDescent="0.3">
@@ -19283,10 +19325,10 @@
         <v>153</v>
       </c>
       <c r="B475" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="C475" t="s">
-        <v>544</v>
+        <v>903</v>
       </c>
       <c r="D475" t="s">
         <v>147</v>
@@ -19298,10 +19340,10 @@
         <v>147</v>
       </c>
       <c r="G475" s="7" t="s">
-        <v>293</v>
+        <v>905</v>
       </c>
       <c r="H475" s="7" t="s">
-        <v>845</v>
+        <v>907</v>
       </c>
     </row>
     <row r="476" spans="1:9" x14ac:dyDescent="0.3">
@@ -19312,7 +19354,7 @@
         <v>292</v>
       </c>
       <c r="C476" t="s">
-        <v>15</v>
+        <v>544</v>
       </c>
       <c r="D476" t="s">
         <v>147</v>
@@ -19320,11 +19362,14 @@
       <c r="E476" t="s">
         <v>147</v>
       </c>
+      <c r="F476" t="s">
+        <v>147</v>
+      </c>
       <c r="G476" s="7" t="s">
-        <v>545</v>
+        <v>293</v>
       </c>
       <c r="H476" s="7" t="s">
-        <v>645</v>
+        <v>845</v>
       </c>
     </row>
     <row r="477" spans="1:9" x14ac:dyDescent="0.3">
@@ -19335,7 +19380,7 @@
         <v>292</v>
       </c>
       <c r="C477" t="s">
-        <v>546</v>
+        <v>15</v>
       </c>
       <c r="D477" t="s">
         <v>147</v>
@@ -19344,10 +19389,10 @@
         <v>147</v>
       </c>
       <c r="G477" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H477" s="7" t="s">
-        <v>846</v>
+        <v>645</v>
       </c>
     </row>
     <row r="478" spans="1:9" x14ac:dyDescent="0.3">
@@ -19358,7 +19403,7 @@
         <v>292</v>
       </c>
       <c r="C478" t="s">
-        <v>902</v>
+        <v>546</v>
       </c>
       <c r="D478" t="s">
         <v>147</v>
@@ -19366,14 +19411,11 @@
       <c r="E478" t="s">
         <v>147</v>
       </c>
-      <c r="F478" t="s">
-        <v>147</v>
-      </c>
       <c r="G478" s="7" t="s">
-        <v>904</v>
+        <v>547</v>
       </c>
       <c r="H478" s="7" t="s">
-        <v>906</v>
+        <v>846</v>
       </c>
     </row>
     <row r="479" spans="1:9" x14ac:dyDescent="0.3">
@@ -19384,7 +19426,7 @@
         <v>292</v>
       </c>
       <c r="C479" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D479" t="s">
         <v>147</v>
@@ -19396,10 +19438,10 @@
         <v>147</v>
       </c>
       <c r="G479" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H479" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="480" spans="1:9" x14ac:dyDescent="0.3">
@@ -19407,22 +19449,25 @@
         <v>153</v>
       </c>
       <c r="B480" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="C480" t="s">
-        <v>511</v>
+        <v>903</v>
       </c>
       <c r="D480" t="s">
         <v>147</v>
       </c>
+      <c r="E480" t="s">
+        <v>147</v>
+      </c>
       <c r="F480" t="s">
         <v>147</v>
       </c>
       <c r="G480" s="7" t="s">
-        <v>512</v>
+        <v>905</v>
       </c>
       <c r="H480" s="7" t="s">
-        <v>839</v>
+        <v>907</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -19433,19 +19478,19 @@
         <v>265</v>
       </c>
       <c r="C481" t="s">
-        <v>12</v>
+        <v>511</v>
       </c>
       <c r="D481" t="s">
         <v>147</v>
       </c>
-      <c r="E481" t="s">
+      <c r="F481" t="s">
         <v>147</v>
       </c>
       <c r="G481" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H481" s="7" t="s">
-        <v>789</v>
+        <v>839</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -19456,7 +19501,7 @@
         <v>265</v>
       </c>
       <c r="C482" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D482" t="s">
         <v>147</v>
@@ -19465,10 +19510,10 @@
         <v>147</v>
       </c>
       <c r="G482" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H482" s="7" t="s">
-        <v>635</v>
+        <v>789</v>
       </c>
     </row>
     <row r="483" spans="1:9" x14ac:dyDescent="0.3">
@@ -19479,7 +19524,7 @@
         <v>265</v>
       </c>
       <c r="C483" t="s">
-        <v>902</v>
+        <v>9</v>
       </c>
       <c r="D483" t="s">
         <v>147</v>
@@ -19487,14 +19532,11 @@
       <c r="E483" t="s">
         <v>147</v>
       </c>
-      <c r="F483" t="s">
-        <v>147</v>
-      </c>
       <c r="G483" s="7" t="s">
-        <v>904</v>
+        <v>514</v>
       </c>
       <c r="H483" s="7" t="s">
-        <v>906</v>
+        <v>635</v>
       </c>
     </row>
     <row r="484" spans="1:9" x14ac:dyDescent="0.3">
@@ -19505,7 +19547,7 @@
         <v>265</v>
       </c>
       <c r="C484" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D484" t="s">
         <v>147</v>
@@ -19517,10 +19559,10 @@
         <v>147</v>
       </c>
       <c r="G484" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H484" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="485" spans="1:9" x14ac:dyDescent="0.3">
@@ -19528,22 +19570,25 @@
         <v>153</v>
       </c>
       <c r="B485" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C485" t="s">
-        <v>478</v>
+        <v>903</v>
       </c>
       <c r="D485" t="s">
         <v>147</v>
       </c>
+      <c r="E485" t="s">
+        <v>147</v>
+      </c>
       <c r="F485" t="s">
         <v>147</v>
       </c>
       <c r="G485" s="7" t="s">
-        <v>515</v>
+        <v>905</v>
       </c>
       <c r="H485" s="7" t="s">
-        <v>223</v>
+        <v>907</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -19554,22 +19599,19 @@
         <v>267</v>
       </c>
       <c r="C486" t="s">
-        <v>516</v>
+        <v>478</v>
       </c>
       <c r="D486" t="s">
         <v>147</v>
       </c>
-      <c r="E486" t="s">
-        <v>147</v>
-      </c>
       <c r="F486" t="s">
         <v>147</v>
       </c>
       <c r="G486" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H486" s="7" t="s">
-        <v>772</v>
+        <v>223</v>
       </c>
     </row>
     <row r="487" spans="1:9" x14ac:dyDescent="0.3">
@@ -19580,7 +19622,7 @@
         <v>267</v>
       </c>
       <c r="C487" t="s">
-        <v>902</v>
+        <v>516</v>
       </c>
       <c r="D487" t="s">
         <v>147</v>
@@ -19592,10 +19634,10 @@
         <v>147</v>
       </c>
       <c r="G487" s="7" t="s">
-        <v>904</v>
+        <v>517</v>
       </c>
       <c r="H487" s="7" t="s">
-        <v>906</v>
+        <v>772</v>
       </c>
     </row>
     <row r="488" spans="1:9" x14ac:dyDescent="0.3">
@@ -19606,7 +19648,7 @@
         <v>267</v>
       </c>
       <c r="C488" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D488" t="s">
         <v>147</v>
@@ -19618,10 +19660,10 @@
         <v>147</v>
       </c>
       <c r="G488" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H488" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="489" spans="1:9" x14ac:dyDescent="0.3">
@@ -19629,10 +19671,10 @@
         <v>153</v>
       </c>
       <c r="B489" t="s">
-        <v>778</v>
+        <v>267</v>
       </c>
       <c r="C489" t="s">
-        <v>782</v>
+        <v>903</v>
       </c>
       <c r="D489" t="s">
         <v>147</v>
@@ -19640,14 +19682,14 @@
       <c r="E489" t="s">
         <v>147</v>
       </c>
+      <c r="F489" t="s">
+        <v>147</v>
+      </c>
       <c r="G489" s="7" t="s">
-        <v>875</v>
+        <v>905</v>
       </c>
       <c r="H489" s="7" t="s">
-        <v>876</v>
-      </c>
-      <c r="I489" t="s">
-        <v>1215</v>
+        <v>907</v>
       </c>
     </row>
     <row r="490" spans="1:9" x14ac:dyDescent="0.3">
@@ -19658,85 +19700,88 @@
         <v>778</v>
       </c>
       <c r="C490" t="s">
+        <v>12</v>
+      </c>
+      <c r="D490" t="s">
+        <v>147</v>
+      </c>
+      <c r="F490" t="s">
+        <v>147</v>
+      </c>
+      <c r="G490" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="H490" s="7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>153</v>
+      </c>
+      <c r="B491" t="s">
+        <v>778</v>
+      </c>
+      <c r="C491" t="s">
+        <v>782</v>
+      </c>
+      <c r="D491" t="s">
+        <v>147</v>
+      </c>
+      <c r="E491" t="s">
+        <v>147</v>
+      </c>
+      <c r="G491" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="H491" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="I491" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>153</v>
+      </c>
+      <c r="B492" t="s">
+        <v>778</v>
+      </c>
+      <c r="C492" t="s">
         <v>9</v>
       </c>
-      <c r="D490" t="s">
-        <v>147</v>
-      </c>
-      <c r="E490" t="s">
-        <v>147</v>
-      </c>
-      <c r="G490" s="7" t="s">
+      <c r="D492" t="s">
+        <v>147</v>
+      </c>
+      <c r="G492" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="H490" s="7" t="s">
+      <c r="H492" s="7" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="491" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A491" t="s">
-        <v>153</v>
-      </c>
-      <c r="B491" t="s">
-        <v>944</v>
-      </c>
-      <c r="C491" t="s">
-        <v>945</v>
-      </c>
-      <c r="D491" t="s">
-        <v>147</v>
-      </c>
-      <c r="E491" t="s">
-        <v>147</v>
-      </c>
-      <c r="F491" t="s">
-        <v>147</v>
-      </c>
-      <c r="G491" s="13" t="s">
-        <v>953</v>
-      </c>
-      <c r="H491" s="7" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="492" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A492" t="s">
-        <v>153</v>
-      </c>
-      <c r="B492" t="s">
-        <v>944</v>
-      </c>
-      <c r="C492" t="s">
-        <v>12</v>
-      </c>
-      <c r="D492" t="s">
-        <v>147</v>
-      </c>
-      <c r="G492" s="13" t="s">
-        <v>955</v>
-      </c>
-      <c r="H492" s="7" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="493" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>153</v>
       </c>
       <c r="B493" t="s">
-        <v>944</v>
+        <v>778</v>
       </c>
       <c r="C493" t="s">
-        <v>946</v>
+        <v>902</v>
       </c>
       <c r="D493" t="s">
         <v>147</v>
       </c>
-      <c r="G493" s="13" t="s">
-        <v>956</v>
+      <c r="F493" t="s">
+        <v>147</v>
+      </c>
+      <c r="G493" s="7" t="s">
+        <v>904</v>
       </c>
       <c r="H493" s="7" t="s">
-        <v>957</v>
+        <v>906</v>
       </c>
     </row>
     <row r="494" spans="1:9" x14ac:dyDescent="0.3">
@@ -19744,19 +19789,22 @@
         <v>153</v>
       </c>
       <c r="B494" t="s">
-        <v>944</v>
+        <v>778</v>
       </c>
       <c r="C494" t="s">
-        <v>947</v>
+        <v>903</v>
       </c>
       <c r="D494" t="s">
         <v>147</v>
       </c>
+      <c r="F494" t="s">
+        <v>147</v>
+      </c>
       <c r="G494" s="7" t="s">
-        <v>969</v>
+        <v>905</v>
       </c>
       <c r="H494" s="7" t="s">
-        <v>959</v>
+        <v>907</v>
       </c>
     </row>
     <row r="495" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -19767,19 +19815,22 @@
         <v>944</v>
       </c>
       <c r="C495" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="D495" t="s">
         <v>147</v>
       </c>
+      <c r="E495" t="s">
+        <v>147</v>
+      </c>
+      <c r="F495" t="s">
+        <v>147</v>
+      </c>
       <c r="G495" s="13" t="s">
-        <v>966</v>
+        <v>953</v>
       </c>
       <c r="H495" s="7" t="s">
-        <v>967</v>
-      </c>
-      <c r="I495" t="s">
-        <v>976</v>
+        <v>954</v>
       </c>
     </row>
     <row r="496" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -19790,25 +19841,19 @@
         <v>944</v>
       </c>
       <c r="C496" t="s">
-        <v>949</v>
+        <v>12</v>
       </c>
       <c r="D496" t="s">
         <v>147</v>
       </c>
-      <c r="F496" t="s">
-        <v>147</v>
-      </c>
       <c r="G496" s="13" t="s">
-        <v>960</v>
+        <v>955</v>
       </c>
       <c r="H496" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="I496" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="497" spans="1:9" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>153</v>
       </c>
@@ -19816,16 +19861,16 @@
         <v>944</v>
       </c>
       <c r="C497" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="D497" t="s">
         <v>147</v>
       </c>
-      <c r="G497" s="7" t="s">
-        <v>964</v>
+      <c r="G497" s="13" t="s">
+        <v>956</v>
       </c>
       <c r="H497" s="7" t="s">
-        <v>962</v>
+        <v>957</v>
       </c>
     </row>
     <row r="498" spans="1:9" x14ac:dyDescent="0.3">
@@ -19836,19 +19881,19 @@
         <v>944</v>
       </c>
       <c r="C498" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="D498" t="s">
         <v>147</v>
       </c>
       <c r="G498" s="7" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="H498" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="499" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>153</v>
       </c>
@@ -19856,16 +19901,19 @@
         <v>944</v>
       </c>
       <c r="C499" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="D499" t="s">
         <v>147</v>
       </c>
       <c r="G499" s="13" t="s">
-        <v>958</v>
+        <v>966</v>
       </c>
       <c r="H499" s="7" t="s">
-        <v>968</v>
+        <v>967</v>
+      </c>
+      <c r="I499" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="500" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -19876,19 +19924,22 @@
         <v>944</v>
       </c>
       <c r="C500" t="s">
-        <v>498</v>
+        <v>949</v>
       </c>
       <c r="D500" t="s">
         <v>147</v>
       </c>
+      <c r="F500" t="s">
+        <v>147</v>
+      </c>
       <c r="G500" s="13" t="s">
-        <v>182</v>
+        <v>960</v>
       </c>
       <c r="H500" s="7" t="s">
-        <v>183</v>
+        <v>961</v>
       </c>
       <c r="I500" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="501" spans="1:9" x14ac:dyDescent="0.3">
@@ -19899,22 +19950,16 @@
         <v>944</v>
       </c>
       <c r="C501" t="s">
-        <v>902</v>
+        <v>950</v>
       </c>
       <c r="D501" t="s">
         <v>147</v>
       </c>
-      <c r="E501" t="s">
-        <v>147</v>
-      </c>
-      <c r="F501" t="s">
-        <v>147</v>
-      </c>
       <c r="G501" s="7" t="s">
-        <v>904</v>
+        <v>964</v>
       </c>
       <c r="H501" s="7" t="s">
-        <v>906</v>
+        <v>962</v>
       </c>
     </row>
     <row r="502" spans="1:9" x14ac:dyDescent="0.3">
@@ -19925,88 +19970,85 @@
         <v>944</v>
       </c>
       <c r="C502" t="s">
-        <v>903</v>
+        <v>951</v>
       </c>
       <c r="D502" t="s">
         <v>147</v>
       </c>
-      <c r="E502" t="s">
-        <v>147</v>
-      </c>
-      <c r="F502" t="s">
-        <v>147</v>
-      </c>
       <c r="G502" s="7" t="s">
-        <v>905</v>
+        <v>965</v>
       </c>
       <c r="H502" s="7" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="503" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>153</v>
       </c>
       <c r="B503" t="s">
-        <v>1009</v>
+        <v>944</v>
       </c>
       <c r="C503" t="s">
-        <v>1011</v>
+        <v>952</v>
       </c>
       <c r="D503" t="s">
         <v>147</v>
       </c>
-      <c r="E503" t="s">
-        <v>147</v>
-      </c>
-      <c r="F503" t="s">
-        <v>147</v>
-      </c>
       <c r="G503" s="13" t="s">
-        <v>1026</v>
+        <v>958</v>
       </c>
       <c r="H503" s="7" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="504" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>153</v>
       </c>
       <c r="B504" t="s">
-        <v>1009</v>
+        <v>944</v>
       </c>
       <c r="C504" t="s">
-        <v>1012</v>
+        <v>498</v>
       </c>
       <c r="D504" t="s">
         <v>147</v>
       </c>
       <c r="G504" s="13" t="s">
-        <v>1028</v>
+        <v>182</v>
       </c>
       <c r="H504" s="7" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="505" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="I504" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="505" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>153</v>
       </c>
       <c r="B505" t="s">
-        <v>1009</v>
+        <v>944</v>
       </c>
       <c r="C505" t="s">
-        <v>1013</v>
+        <v>902</v>
       </c>
       <c r="D505" t="s">
         <v>147</v>
       </c>
-      <c r="G505" s="13" t="s">
-        <v>1030</v>
+      <c r="E505" t="s">
+        <v>147</v>
+      </c>
+      <c r="F505" t="s">
+        <v>147</v>
+      </c>
+      <c r="G505" s="7" t="s">
+        <v>904</v>
       </c>
       <c r="H505" s="7" t="s">
-        <v>1031</v>
+        <v>906</v>
       </c>
     </row>
     <row r="506" spans="1:9" x14ac:dyDescent="0.3">
@@ -20014,19 +20056,25 @@
         <v>153</v>
       </c>
       <c r="B506" t="s">
-        <v>1009</v>
+        <v>944</v>
       </c>
       <c r="C506" t="s">
-        <v>1014</v>
+        <v>903</v>
       </c>
       <c r="D506" t="s">
         <v>147</v>
       </c>
+      <c r="E506" t="s">
+        <v>147</v>
+      </c>
+      <c r="F506" t="s">
+        <v>147</v>
+      </c>
       <c r="G506" s="7" t="s">
-        <v>1033</v>
+        <v>905</v>
       </c>
       <c r="H506" s="7" t="s">
-        <v>1032</v>
+        <v>907</v>
       </c>
     </row>
     <row r="507" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20037,22 +20085,25 @@
         <v>1009</v>
       </c>
       <c r="C507" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D507" t="s">
         <v>147</v>
       </c>
+      <c r="E507" t="s">
+        <v>147</v>
+      </c>
       <c r="F507" t="s">
         <v>147</v>
       </c>
-      <c r="G507" s="12" t="s">
-        <v>1034</v>
+      <c r="G507" s="13" t="s">
+        <v>1026</v>
       </c>
       <c r="H507" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="508" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>153</v>
       </c>
@@ -20060,19 +20111,19 @@
         <v>1009</v>
       </c>
       <c r="C508" t="s">
-        <v>586</v>
+        <v>1012</v>
       </c>
       <c r="D508" t="s">
         <v>147</v>
       </c>
-      <c r="G508" s="12" t="s">
-        <v>1035</v>
+      <c r="G508" s="13" t="s">
+        <v>1028</v>
       </c>
       <c r="H508" s="7" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="509" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>153</v>
       </c>
@@ -20080,19 +20131,19 @@
         <v>1009</v>
       </c>
       <c r="C509" t="s">
-        <v>584</v>
+        <v>1013</v>
       </c>
       <c r="D509" t="s">
         <v>147</v>
       </c>
-      <c r="G509" s="12" t="s">
-        <v>1036</v>
+      <c r="G509" s="13" t="s">
+        <v>1030</v>
       </c>
       <c r="H509" s="7" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="510" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>153</v>
       </c>
@@ -20100,16 +20151,16 @@
         <v>1009</v>
       </c>
       <c r="C510" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D510" t="s">
         <v>147</v>
       </c>
-      <c r="G510" s="12" t="s">
-        <v>1037</v>
+      <c r="G510" s="7" t="s">
+        <v>1033</v>
       </c>
       <c r="H510" s="7" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="511" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20120,16 +20171,19 @@
         <v>1009</v>
       </c>
       <c r="C511" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D511" t="s">
         <v>147</v>
       </c>
+      <c r="F511" t="s">
+        <v>147</v>
+      </c>
       <c r="G511" s="12" t="s">
-        <v>1039</v>
+        <v>1034</v>
       </c>
       <c r="H511" s="7" t="s">
-        <v>1040</v>
+        <v>242</v>
       </c>
     </row>
     <row r="512" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -20140,19 +20194,19 @@
         <v>1009</v>
       </c>
       <c r="C512" t="s">
-        <v>1018</v>
+        <v>586</v>
       </c>
       <c r="D512" t="s">
         <v>147</v>
       </c>
       <c r="G512" s="12" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="H512" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="513" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="513" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>153</v>
       </c>
@@ -20160,19 +20214,19 @@
         <v>1009</v>
       </c>
       <c r="C513" t="s">
-        <v>1019</v>
+        <v>584</v>
       </c>
       <c r="D513" t="s">
         <v>147</v>
       </c>
-      <c r="G513" s="7" t="s">
-        <v>1042</v>
+      <c r="G513" s="12" t="s">
+        <v>1036</v>
       </c>
       <c r="H513" s="7" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="514" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="514" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>153</v>
       </c>
@@ -20180,19 +20234,19 @@
         <v>1009</v>
       </c>
       <c r="C514" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D514" t="s">
         <v>147</v>
       </c>
-      <c r="G514" s="7" t="s">
-        <v>1044</v>
+      <c r="G514" s="12" t="s">
+        <v>1037</v>
       </c>
       <c r="H514" s="7" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="515" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="515" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>153</v>
       </c>
@@ -20200,19 +20254,19 @@
         <v>1009</v>
       </c>
       <c r="C515" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="D515" t="s">
         <v>147</v>
       </c>
-      <c r="G515" s="7" t="s">
-        <v>1046</v>
+      <c r="G515" s="12" t="s">
+        <v>1039</v>
       </c>
       <c r="H515" s="7" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="516" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>153</v>
       </c>
@@ -20220,16 +20274,16 @@
         <v>1009</v>
       </c>
       <c r="C516" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="D516" t="s">
         <v>147</v>
       </c>
-      <c r="G516" s="7" t="s">
-        <v>1048</v>
+      <c r="G516" s="12" t="s">
+        <v>1041</v>
       </c>
       <c r="H516" s="7" t="s">
-        <v>1049</v>
+        <v>227</v>
       </c>
     </row>
     <row r="517" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -20240,16 +20294,16 @@
         <v>1009</v>
       </c>
       <c r="C517" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="D517" t="s">
         <v>147</v>
       </c>
       <c r="G517" s="7" t="s">
-        <v>1050</v>
+        <v>1042</v>
       </c>
       <c r="H517" s="7" t="s">
-        <v>1051</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="518" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -20260,22 +20314,19 @@
         <v>1009</v>
       </c>
       <c r="C518" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D518" t="s">
         <v>147</v>
       </c>
-      <c r="F518" t="s">
-        <v>147</v>
-      </c>
       <c r="G518" s="7" t="s">
-        <v>1052</v>
+        <v>1044</v>
       </c>
       <c r="H518" s="7" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="519" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="519" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>153</v>
       </c>
@@ -20283,19 +20334,19 @@
         <v>1009</v>
       </c>
       <c r="C519" t="s">
-        <v>559</v>
+        <v>1021</v>
       </c>
       <c r="D519" t="s">
         <v>147</v>
       </c>
       <c r="G519" s="7" t="s">
-        <v>1054</v>
+        <v>1046</v>
       </c>
       <c r="H519" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="520" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="520" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>153</v>
       </c>
@@ -20303,22 +20354,19 @@
         <v>1009</v>
       </c>
       <c r="C520" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="D520" t="s">
         <v>147</v>
       </c>
-      <c r="E520" t="s">
-        <v>147</v>
-      </c>
       <c r="G520" s="7" t="s">
-        <v>1055</v>
+        <v>1048</v>
       </c>
       <c r="H520" s="7" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="521" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="521" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>153</v>
       </c>
@@ -20326,25 +20374,19 @@
         <v>1009</v>
       </c>
       <c r="C521" t="s">
-        <v>902</v>
+        <v>1023</v>
       </c>
       <c r="D521" t="s">
         <v>147</v>
       </c>
-      <c r="E521" t="s">
-        <v>147</v>
-      </c>
-      <c r="F521" t="s">
-        <v>147</v>
-      </c>
       <c r="G521" s="7" t="s">
-        <v>904</v>
+        <v>1050</v>
       </c>
       <c r="H521" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="522" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="522" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>153</v>
       </c>
@@ -20352,22 +20394,19 @@
         <v>1009</v>
       </c>
       <c r="C522" t="s">
-        <v>903</v>
+        <v>1024</v>
       </c>
       <c r="D522" t="s">
         <v>147</v>
       </c>
-      <c r="E522" t="s">
-        <v>147</v>
-      </c>
       <c r="F522" t="s">
         <v>147</v>
       </c>
       <c r="G522" s="7" t="s">
-        <v>905</v>
+        <v>1052</v>
       </c>
       <c r="H522" s="7" t="s">
-        <v>907</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="523" spans="1:9" x14ac:dyDescent="0.3">
@@ -20375,22 +20414,19 @@
         <v>153</v>
       </c>
       <c r="B523" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C523" t="s">
-        <v>398</v>
+        <v>559</v>
       </c>
       <c r="D523" t="s">
         <v>147</v>
       </c>
-      <c r="F523" t="s">
-        <v>147</v>
-      </c>
       <c r="G523" s="7" t="s">
-        <v>1010</v>
+        <v>1054</v>
       </c>
       <c r="H523" s="7" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
     </row>
     <row r="524" spans="1:9" x14ac:dyDescent="0.3">
@@ -20398,10 +20434,10 @@
         <v>153</v>
       </c>
       <c r="B524" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C524" t="s">
-        <v>7</v>
+        <v>1025</v>
       </c>
       <c r="D524" t="s">
         <v>147</v>
@@ -20409,17 +20445,11 @@
       <c r="E524" t="s">
         <v>147</v>
       </c>
-      <c r="F524" t="s">
-        <v>147</v>
-      </c>
       <c r="G524" s="7" t="s">
-        <v>521</v>
+        <v>1055</v>
       </c>
       <c r="H524" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="I524" t="s">
-        <v>937</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="525" spans="1:9" x14ac:dyDescent="0.3">
@@ -20427,10 +20457,10 @@
         <v>153</v>
       </c>
       <c r="B525" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C525" t="s">
-        <v>1064</v>
+        <v>902</v>
       </c>
       <c r="D525" t="s">
         <v>147</v>
@@ -20442,10 +20472,10 @@
         <v>147</v>
       </c>
       <c r="G525" s="7" t="s">
-        <v>789</v>
+        <v>904</v>
       </c>
       <c r="H525" s="7" t="s">
-        <v>789</v>
+        <v>906</v>
       </c>
     </row>
     <row r="526" spans="1:9" x14ac:dyDescent="0.3">
@@ -20453,10 +20483,10 @@
         <v>153</v>
       </c>
       <c r="B526" t="s">
-        <v>1058</v>
+        <v>1009</v>
       </c>
       <c r="C526" t="s">
-        <v>9</v>
+        <v>903</v>
       </c>
       <c r="D526" t="s">
         <v>147</v>
@@ -20464,11 +20494,14 @@
       <c r="E526" t="s">
         <v>147</v>
       </c>
+      <c r="F526" t="s">
+        <v>147</v>
+      </c>
       <c r="G526" s="7" t="s">
-        <v>1065</v>
+        <v>905</v>
       </c>
       <c r="H526" s="7" t="s">
-        <v>635</v>
+        <v>907</v>
       </c>
     </row>
     <row r="527" spans="1:9" x14ac:dyDescent="0.3">
@@ -20479,22 +20512,19 @@
         <v>1058</v>
       </c>
       <c r="C527" t="s">
-        <v>902</v>
+        <v>398</v>
       </c>
       <c r="D527" t="s">
         <v>147</v>
       </c>
-      <c r="E527" t="s">
-        <v>147</v>
-      </c>
       <c r="F527" t="s">
         <v>147</v>
       </c>
       <c r="G527" s="7" t="s">
-        <v>904</v>
+        <v>1010</v>
       </c>
       <c r="H527" s="7" t="s">
-        <v>906</v>
+        <v>225</v>
       </c>
     </row>
     <row r="528" spans="1:9" x14ac:dyDescent="0.3">
@@ -20505,117 +20535,129 @@
         <v>1058</v>
       </c>
       <c r="C528" t="s">
+        <v>7</v>
+      </c>
+      <c r="D528" t="s">
+        <v>147</v>
+      </c>
+      <c r="E528" t="s">
+        <v>147</v>
+      </c>
+      <c r="F528" t="s">
+        <v>147</v>
+      </c>
+      <c r="G528" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="H528" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="I528" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="529" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>153</v>
+      </c>
+      <c r="B529" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C529" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D529" t="s">
+        <v>147</v>
+      </c>
+      <c r="E529" t="s">
+        <v>147</v>
+      </c>
+      <c r="F529" t="s">
+        <v>147</v>
+      </c>
+      <c r="G529" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="H529" s="7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="530" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A530" t="s">
+        <v>153</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C530" t="s">
+        <v>9</v>
+      </c>
+      <c r="D530" t="s">
+        <v>147</v>
+      </c>
+      <c r="E530" t="s">
+        <v>147</v>
+      </c>
+      <c r="G530" s="7" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H530" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="531" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A531" t="s">
+        <v>153</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C531" t="s">
+        <v>902</v>
+      </c>
+      <c r="D531" t="s">
+        <v>147</v>
+      </c>
+      <c r="E531" t="s">
+        <v>147</v>
+      </c>
+      <c r="F531" t="s">
+        <v>147</v>
+      </c>
+      <c r="G531" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H531" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="532" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A532" t="s">
+        <v>153</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C532" t="s">
         <v>903</v>
       </c>
-      <c r="D528" t="s">
-        <v>147</v>
-      </c>
-      <c r="E528" t="s">
-        <v>147</v>
-      </c>
-      <c r="F528" t="s">
-        <v>147</v>
-      </c>
-      <c r="G528" s="7" t="s">
+      <c r="D532" t="s">
+        <v>147</v>
+      </c>
+      <c r="E532" t="s">
+        <v>147</v>
+      </c>
+      <c r="F532" t="s">
+        <v>147</v>
+      </c>
+      <c r="G532" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H528" s="7" t="s">
+      <c r="H532" s="7" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="529" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A529" t="s">
-        <v>0</v>
-      </c>
-      <c r="B529" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C529" t="s">
-        <v>398</v>
-      </c>
-      <c r="D529" t="s">
-        <v>147</v>
-      </c>
-      <c r="F529" t="s">
-        <v>147</v>
-      </c>
-      <c r="G529" s="7" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H529" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="J529" t="s">
-        <v>1177</v>
-      </c>
-      <c r="K529" t="s">
-        <v>1178</v>
-      </c>
-      <c r="L529" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="530" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A530" t="s">
-        <v>0</v>
-      </c>
-      <c r="B530" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C530" t="s">
-        <v>1102</v>
-      </c>
-      <c r="G530" s="7" t="s">
-        <v>1117</v>
-      </c>
-      <c r="H530" s="7" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="531" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A531" t="s">
-        <v>0</v>
-      </c>
-      <c r="B531" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C531" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D531" t="s">
-        <v>147</v>
-      </c>
-      <c r="F531" t="s">
-        <v>147</v>
-      </c>
-      <c r="G531" s="12" t="s">
-        <v>1119</v>
-      </c>
-      <c r="H531" s="7" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="532" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A532" t="s">
-        <v>0</v>
-      </c>
-      <c r="B532" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C532" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D532" t="s">
-        <v>147</v>
-      </c>
-      <c r="G532" s="12" t="s">
-        <v>1122</v>
-      </c>
-      <c r="H532" s="7" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="533" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>0</v>
       </c>
@@ -20623,7 +20665,7 @@
         <v>1074</v>
       </c>
       <c r="C533" t="s">
-        <v>1105</v>
+        <v>398</v>
       </c>
       <c r="D533" t="s">
         <v>147</v>
@@ -20631,17 +20673,23 @@
       <c r="F533" t="s">
         <v>147</v>
       </c>
-      <c r="G533" s="12" t="s">
-        <v>1123</v>
+      <c r="G533" s="7" t="s">
+        <v>1010</v>
       </c>
       <c r="H533" s="7" t="s">
-        <v>1136</v>
-      </c>
-      <c r="I533" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="534" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+      <c r="J533" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K533" t="s">
+        <v>1178</v>
+      </c>
+      <c r="L533" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="534" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>0</v>
       </c>
@@ -20649,22 +20697,16 @@
         <v>1074</v>
       </c>
       <c r="C534" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D534" t="s">
-        <v>147</v>
-      </c>
-      <c r="F534" t="s">
-        <v>147</v>
-      </c>
-      <c r="G534" s="12" t="s">
-        <v>1124</v>
+        <v>1102</v>
+      </c>
+      <c r="G534" s="7" t="s">
+        <v>1117</v>
       </c>
       <c r="H534" s="7" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="535" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="535" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>0</v>
       </c>
@@ -20672,7 +20714,7 @@
         <v>1074</v>
       </c>
       <c r="C535" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="D535" t="s">
         <v>147</v>
@@ -20681,13 +20723,13 @@
         <v>147</v>
       </c>
       <c r="G535" s="12" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="H535" s="7" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="536" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="536" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>0</v>
       </c>
@@ -20695,22 +20737,19 @@
         <v>1074</v>
       </c>
       <c r="C536" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="D536" t="s">
         <v>147</v>
       </c>
-      <c r="F536" t="s">
-        <v>147</v>
-      </c>
       <c r="G536" s="12" t="s">
-        <v>1134</v>
+        <v>1122</v>
       </c>
       <c r="H536" s="7" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="537" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="537" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>0</v>
       </c>
@@ -20718,19 +20757,25 @@
         <v>1074</v>
       </c>
       <c r="C537" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="D537" t="s">
         <v>147</v>
       </c>
+      <c r="F537" t="s">
+        <v>147</v>
+      </c>
       <c r="G537" s="12" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="H537" s="7" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="538" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1136</v>
+      </c>
+      <c r="I537" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="538" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>0</v>
       </c>
@@ -20738,19 +20783,22 @@
         <v>1074</v>
       </c>
       <c r="C538" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="D538" t="s">
         <v>147</v>
       </c>
+      <c r="F538" t="s">
+        <v>147</v>
+      </c>
       <c r="G538" s="12" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="H538" s="7" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="539" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="539" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>0</v>
       </c>
@@ -20758,19 +20806,22 @@
         <v>1074</v>
       </c>
       <c r="C539" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="D539" t="s">
         <v>147</v>
       </c>
+      <c r="F539" t="s">
+        <v>147</v>
+      </c>
       <c r="G539" s="12" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="H539" s="7" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="540" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="540" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>0</v>
       </c>
@@ -20778,19 +20829,22 @@
         <v>1074</v>
       </c>
       <c r="C540" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="D540" t="s">
         <v>147</v>
       </c>
-      <c r="G540" s="7" t="s">
-        <v>1130</v>
+      <c r="F540" t="s">
+        <v>147</v>
+      </c>
+      <c r="G540" s="12" t="s">
+        <v>1134</v>
       </c>
       <c r="H540" s="7" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="541" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="541" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>0</v>
       </c>
@@ -20798,19 +20852,19 @@
         <v>1074</v>
       </c>
       <c r="C541" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="D541" t="s">
         <v>147</v>
       </c>
-      <c r="G541" s="7" t="s">
-        <v>1129</v>
+      <c r="G541" s="12" t="s">
+        <v>1126</v>
       </c>
       <c r="H541" s="7" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="542" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="542" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>0</v>
       </c>
@@ -20818,19 +20872,19 @@
         <v>1074</v>
       </c>
       <c r="C542" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="D542" t="s">
         <v>147</v>
       </c>
-      <c r="G542" s="7" t="s">
-        <v>1131</v>
+      <c r="G542" s="12" t="s">
+        <v>1127</v>
       </c>
       <c r="H542" s="7" t="s">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="543" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="543" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>0</v>
       </c>
@@ -20838,19 +20892,19 @@
         <v>1074</v>
       </c>
       <c r="C543" t="s">
-        <v>576</v>
+        <v>1111</v>
       </c>
       <c r="D543" t="s">
         <v>147</v>
       </c>
-      <c r="G543" s="7" t="s">
-        <v>1132</v>
+      <c r="G543" s="12" t="s">
+        <v>1128</v>
       </c>
       <c r="H543" s="7" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="544" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="544" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>0</v>
       </c>
@@ -20858,25 +20912,19 @@
         <v>1074</v>
       </c>
       <c r="C544" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="D544" t="s">
         <v>147</v>
       </c>
-      <c r="F544" t="s">
-        <v>147</v>
-      </c>
       <c r="G544" s="7" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="H544" s="7" t="s">
-        <v>1146</v>
-      </c>
-      <c r="M544" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="545" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="545" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>0</v>
       </c>
@@ -20884,22 +20932,19 @@
         <v>1074</v>
       </c>
       <c r="C545" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="D545" t="s">
         <v>147</v>
       </c>
-      <c r="F545" t="s">
-        <v>147</v>
-      </c>
       <c r="G545" s="7" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="H545" s="7" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="546" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="546" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>0</v>
       </c>
@@ -20907,25 +20952,19 @@
         <v>1074</v>
       </c>
       <c r="C546" t="s">
-        <v>902</v>
+        <v>1114</v>
       </c>
       <c r="D546" t="s">
         <v>147</v>
       </c>
-      <c r="E546" t="s">
-        <v>147</v>
-      </c>
-      <c r="F546" t="s">
-        <v>147</v>
-      </c>
       <c r="G546" s="7" t="s">
-        <v>904</v>
+        <v>1131</v>
       </c>
       <c r="H546" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="547" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="547" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>0</v>
       </c>
@@ -20933,126 +20972,120 @@
         <v>1074</v>
       </c>
       <c r="C547" t="s">
+        <v>576</v>
+      </c>
+      <c r="D547" t="s">
+        <v>147</v>
+      </c>
+      <c r="G547" s="7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H547" s="7" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="548" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A548" t="s">
+        <v>0</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C548" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D548" t="s">
+        <v>147</v>
+      </c>
+      <c r="F548" t="s">
+        <v>147</v>
+      </c>
+      <c r="G548" s="7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H548" s="7" t="s">
+        <v>1146</v>
+      </c>
+      <c r="M548" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="549" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A549" t="s">
+        <v>0</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C549" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D549" t="s">
+        <v>147</v>
+      </c>
+      <c r="F549" t="s">
+        <v>147</v>
+      </c>
+      <c r="G549" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H549" s="7" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A550" t="s">
+        <v>0</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C550" t="s">
+        <v>902</v>
+      </c>
+      <c r="D550" t="s">
+        <v>147</v>
+      </c>
+      <c r="E550" t="s">
+        <v>147</v>
+      </c>
+      <c r="F550" t="s">
+        <v>147</v>
+      </c>
+      <c r="G550" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H550" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A551" t="s">
+        <v>0</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C551" t="s">
         <v>903</v>
       </c>
-      <c r="D547" t="s">
-        <v>147</v>
-      </c>
-      <c r="E547" t="s">
-        <v>147</v>
-      </c>
-      <c r="F547" t="s">
-        <v>147</v>
-      </c>
-      <c r="G547" s="7" t="s">
+      <c r="D551" t="s">
+        <v>147</v>
+      </c>
+      <c r="E551" t="s">
+        <v>147</v>
+      </c>
+      <c r="F551" t="s">
+        <v>147</v>
+      </c>
+      <c r="G551" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H547" s="7" t="s">
+      <c r="H551" s="7" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="548" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A548" t="s">
-        <v>0</v>
-      </c>
-      <c r="B548" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C548" t="s">
-        <v>1148</v>
-      </c>
-      <c r="D548" t="s">
-        <v>147</v>
-      </c>
-      <c r="F548" t="s">
-        <v>147</v>
-      </c>
-      <c r="G548" s="7" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H548" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="549" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A549" t="s">
-        <v>0</v>
-      </c>
-      <c r="B549" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C549" t="s">
-        <v>7</v>
-      </c>
-      <c r="D549" t="s">
-        <v>147</v>
-      </c>
-      <c r="E549" t="s">
-        <v>147</v>
-      </c>
-      <c r="F549" t="s">
-        <v>147</v>
-      </c>
-      <c r="G549" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="H549" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="I549" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="550" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A550" t="s">
-        <v>0</v>
-      </c>
-      <c r="B550" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C550" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D550" t="s">
-        <v>147</v>
-      </c>
-      <c r="E550" t="s">
-        <v>147</v>
-      </c>
-      <c r="F550" t="s">
-        <v>147</v>
-      </c>
-      <c r="G550" s="7" t="s">
-        <v>789</v>
-      </c>
-      <c r="H550" s="7" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="551" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A551" t="s">
-        <v>0</v>
-      </c>
-      <c r="B551" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C551" t="s">
-        <v>9</v>
-      </c>
-      <c r="D551" t="s">
-        <v>147</v>
-      </c>
-      <c r="E551" t="s">
-        <v>147</v>
-      </c>
-      <c r="G551" s="7" t="s">
-        <v>1065</v>
-      </c>
-      <c r="H551" s="7" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="552" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>0</v>
       </c>
@@ -21060,25 +21093,22 @@
         <v>1075</v>
       </c>
       <c r="C552" t="s">
-        <v>902</v>
+        <v>1148</v>
       </c>
       <c r="D552" t="s">
         <v>147</v>
       </c>
-      <c r="E552" t="s">
-        <v>147</v>
-      </c>
       <c r="F552" t="s">
         <v>147</v>
       </c>
       <c r="G552" s="7" t="s">
-        <v>904</v>
+        <v>1010</v>
       </c>
       <c r="H552" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="553" spans="1:9" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="553" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>0</v>
       </c>
@@ -21086,132 +21116,129 @@
         <v>1075</v>
       </c>
       <c r="C553" t="s">
+        <v>7</v>
+      </c>
+      <c r="D553" t="s">
+        <v>147</v>
+      </c>
+      <c r="E553" t="s">
+        <v>147</v>
+      </c>
+      <c r="F553" t="s">
+        <v>147</v>
+      </c>
+      <c r="G553" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="H553" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="I553" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="554" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A554" t="s">
+        <v>0</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C554" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D554" t="s">
+        <v>147</v>
+      </c>
+      <c r="E554" t="s">
+        <v>147</v>
+      </c>
+      <c r="F554" t="s">
+        <v>147</v>
+      </c>
+      <c r="G554" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="H554" s="7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="555" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A555" t="s">
+        <v>0</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C555" t="s">
+        <v>9</v>
+      </c>
+      <c r="D555" t="s">
+        <v>147</v>
+      </c>
+      <c r="E555" t="s">
+        <v>147</v>
+      </c>
+      <c r="G555" s="7" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H555" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="556" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>0</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C556" t="s">
+        <v>902</v>
+      </c>
+      <c r="D556" t="s">
+        <v>147</v>
+      </c>
+      <c r="E556" t="s">
+        <v>147</v>
+      </c>
+      <c r="F556" t="s">
+        <v>147</v>
+      </c>
+      <c r="G556" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H556" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="557" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A557" t="s">
+        <v>0</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C557" t="s">
         <v>903</v>
       </c>
-      <c r="D553" t="s">
-        <v>147</v>
-      </c>
-      <c r="E553" t="s">
-        <v>147</v>
-      </c>
-      <c r="F553" t="s">
-        <v>147</v>
-      </c>
-      <c r="G553" s="7" t="s">
+      <c r="D557" t="s">
+        <v>147</v>
+      </c>
+      <c r="E557" t="s">
+        <v>147</v>
+      </c>
+      <c r="F557" t="s">
+        <v>147</v>
+      </c>
+      <c r="G557" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H553" s="7" t="s">
+      <c r="H557" s="7" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="554" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A554" t="s">
-        <v>0</v>
-      </c>
-      <c r="B554" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C554" t="s">
-        <v>11</v>
-      </c>
-      <c r="D554" t="s">
-        <v>147</v>
-      </c>
-      <c r="E554" t="s">
-        <v>147</v>
-      </c>
-      <c r="F554" t="s">
-        <v>147</v>
-      </c>
-      <c r="G554" s="12" t="s">
-        <v>1149</v>
-      </c>
-      <c r="H554" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I554" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="555" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A555" t="s">
-        <v>0</v>
-      </c>
-      <c r="B555" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C555" t="s">
-        <v>1148</v>
-      </c>
-      <c r="D555" t="s">
-        <v>147</v>
-      </c>
-      <c r="F555" t="s">
-        <v>147</v>
-      </c>
-      <c r="G555" s="7" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H555" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="556" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A556" t="s">
-        <v>0</v>
-      </c>
-      <c r="B556" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C556" t="s">
-        <v>1150</v>
-      </c>
-      <c r="D556" t="s">
-        <v>147</v>
-      </c>
-      <c r="E556" t="s">
-        <v>147</v>
-      </c>
-      <c r="F556" t="s">
-        <v>147</v>
-      </c>
-      <c r="G556" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="H556" s="7" t="s">
-        <v>1151</v>
-      </c>
-      <c r="I556" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="557" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A557" t="s">
-        <v>0</v>
-      </c>
-      <c r="B557" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C557" t="s">
-        <v>41</v>
-      </c>
-      <c r="D557" t="s">
-        <v>147</v>
-      </c>
-      <c r="E557" t="s">
-        <v>147</v>
-      </c>
-      <c r="F557" t="s">
-        <v>147</v>
-      </c>
-      <c r="G557" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="H557" s="7" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="558" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>0</v>
       </c>
@@ -21219,7 +21246,7 @@
         <v>1076</v>
       </c>
       <c r="C558" t="s">
-        <v>902</v>
+        <v>11</v>
       </c>
       <c r="D558" t="s">
         <v>147</v>
@@ -21230,14 +21257,17 @@
       <c r="F558" t="s">
         <v>147</v>
       </c>
-      <c r="G558" s="7" t="s">
-        <v>904</v>
+      <c r="G558" s="12" t="s">
+        <v>1149</v>
       </c>
       <c r="H558" s="7" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="559" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="I558" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="559" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>0</v>
       </c>
@@ -21245,33 +21275,30 @@
         <v>1076</v>
       </c>
       <c r="C559" t="s">
-        <v>903</v>
+        <v>1148</v>
       </c>
       <c r="D559" t="s">
         <v>147</v>
       </c>
-      <c r="E559" t="s">
-        <v>147</v>
-      </c>
       <c r="F559" t="s">
         <v>147</v>
       </c>
       <c r="G559" s="7" t="s">
-        <v>905</v>
+        <v>1010</v>
       </c>
       <c r="H559" s="7" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="560" spans="1:9" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="560" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>0</v>
       </c>
       <c r="B560" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C560" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="D560" t="s">
         <v>147</v>
@@ -21283,10 +21310,13 @@
         <v>147</v>
       </c>
       <c r="G560" s="7" t="s">
-        <v>1156</v>
+        <v>135</v>
       </c>
       <c r="H560" s="7" t="s">
-        <v>1154</v>
+        <v>1151</v>
+      </c>
+      <c r="I560" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.3">
@@ -21294,10 +21324,10 @@
         <v>0</v>
       </c>
       <c r="B561" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C561" t="s">
-        <v>1153</v>
+        <v>41</v>
       </c>
       <c r="D561" t="s">
         <v>147</v>
@@ -21309,10 +21339,10 @@
         <v>147</v>
       </c>
       <c r="G561" s="7" t="s">
-        <v>1155</v>
+        <v>485</v>
       </c>
       <c r="H561" s="7" t="s">
-        <v>783</v>
+        <v>658</v>
       </c>
     </row>
     <row r="562" spans="1:9" x14ac:dyDescent="0.3">
@@ -21320,7 +21350,7 @@
         <v>0</v>
       </c>
       <c r="B562" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C562" t="s">
         <v>902</v>
@@ -21346,7 +21376,7 @@
         <v>0</v>
       </c>
       <c r="B563" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C563" t="s">
         <v>903</v>
@@ -21372,22 +21402,25 @@
         <v>0</v>
       </c>
       <c r="B564" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C564" t="s">
-        <v>4</v>
+        <v>1152</v>
       </c>
       <c r="D564" t="s">
         <v>147</v>
       </c>
+      <c r="E564" t="s">
+        <v>147</v>
+      </c>
       <c r="F564" t="s">
         <v>147</v>
       </c>
       <c r="G564" s="7" t="s">
-        <v>1086</v>
+        <v>1156</v>
       </c>
       <c r="H564" s="7" t="s">
-        <v>1087</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="565" spans="1:9" x14ac:dyDescent="0.3">
@@ -21395,10 +21428,10 @@
         <v>0</v>
       </c>
       <c r="B565" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C565" t="s">
-        <v>45</v>
+        <v>1153</v>
       </c>
       <c r="D565" t="s">
         <v>147</v>
@@ -21410,13 +21443,10 @@
         <v>147</v>
       </c>
       <c r="G565" s="7" t="s">
-        <v>253</v>
+        <v>1155</v>
       </c>
       <c r="H565" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="I565" t="s">
-        <v>1000</v>
+        <v>783</v>
       </c>
     </row>
     <row r="566" spans="1:9" x14ac:dyDescent="0.3">
@@ -21424,7 +21454,7 @@
         <v>0</v>
       </c>
       <c r="B566" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C566" t="s">
         <v>902</v>
@@ -21450,7 +21480,7 @@
         <v>0</v>
       </c>
       <c r="B567" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C567" t="s">
         <v>903</v>
@@ -21476,7 +21506,7 @@
         <v>0</v>
       </c>
       <c r="B568" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C568" t="s">
         <v>4</v>
@@ -21499,10 +21529,10 @@
         <v>0</v>
       </c>
       <c r="B569" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C569" t="s">
-        <v>1157</v>
+        <v>45</v>
       </c>
       <c r="D569" t="s">
         <v>147</v>
@@ -21514,13 +21544,13 @@
         <v>147</v>
       </c>
       <c r="G569" s="7" t="s">
-        <v>421</v>
+        <v>253</v>
       </c>
       <c r="H569" s="7" t="s">
-        <v>1158</v>
+        <v>254</v>
       </c>
       <c r="I569" t="s">
-        <v>1172</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.3">
@@ -21528,7 +21558,7 @@
         <v>0</v>
       </c>
       <c r="B570" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C570" t="s">
         <v>902</v>
@@ -21549,12 +21579,12 @@
         <v>906</v>
       </c>
     </row>
-    <row r="571" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>0</v>
       </c>
       <c r="B571" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C571" t="s">
         <v>903</v>
@@ -21580,10 +21610,10 @@
         <v>0</v>
       </c>
       <c r="B572" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C572" t="s">
-        <v>1159</v>
+        <v>4</v>
       </c>
       <c r="D572" t="s">
         <v>147</v>
@@ -21592,10 +21622,10 @@
         <v>147</v>
       </c>
       <c r="G572" s="7" t="s">
-        <v>1164</v>
+        <v>1086</v>
       </c>
       <c r="H572" s="7" t="s">
-        <v>1163</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="573" spans="1:9" x14ac:dyDescent="0.3">
@@ -21603,10 +21633,10 @@
         <v>0</v>
       </c>
       <c r="B573" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C573" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="D573" t="s">
         <v>147</v>
@@ -21618,10 +21648,13 @@
         <v>147</v>
       </c>
       <c r="G573" s="7" t="s">
-        <v>1161</v>
+        <v>421</v>
       </c>
       <c r="H573" s="7" t="s">
-        <v>1162</v>
+        <v>1158</v>
+      </c>
+      <c r="I573" t="s">
+        <v>1172</v>
       </c>
     </row>
     <row r="574" spans="1:9" x14ac:dyDescent="0.3">
@@ -21629,7 +21662,7 @@
         <v>0</v>
       </c>
       <c r="B574" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C574" t="s">
         <v>902</v>
@@ -21650,12 +21683,12 @@
         <v>906</v>
       </c>
     </row>
-    <row r="575" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>0</v>
       </c>
       <c r="B575" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C575" t="s">
         <v>903</v>
@@ -21676,8 +21709,109 @@
         <v>907</v>
       </c>
     </row>
+    <row r="576" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A576" t="s">
+        <v>0</v>
+      </c>
+      <c r="B576" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C576" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D576" t="s">
+        <v>147</v>
+      </c>
+      <c r="F576" t="s">
+        <v>147</v>
+      </c>
+      <c r="G576" s="7" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H576" s="7" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A577" t="s">
+        <v>0</v>
+      </c>
+      <c r="B577" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C577" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D577" t="s">
+        <v>147</v>
+      </c>
+      <c r="E577" t="s">
+        <v>147</v>
+      </c>
+      <c r="F577" t="s">
+        <v>147</v>
+      </c>
+      <c r="G577" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H577" s="7" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A578" t="s">
+        <v>0</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C578" t="s">
+        <v>902</v>
+      </c>
+      <c r="D578" t="s">
+        <v>147</v>
+      </c>
+      <c r="E578" t="s">
+        <v>147</v>
+      </c>
+      <c r="F578" t="s">
+        <v>147</v>
+      </c>
+      <c r="G578" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H578" s="7" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="579" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A579" t="s">
+        <v>0</v>
+      </c>
+      <c r="B579" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C579" t="s">
+        <v>903</v>
+      </c>
+      <c r="D579" t="s">
+        <v>147</v>
+      </c>
+      <c r="E579" t="s">
+        <v>147</v>
+      </c>
+      <c r="F579" t="s">
+        <v>147</v>
+      </c>
+      <c r="G579" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="H579" s="7" t="s">
+        <v>907</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C568"/>
+  <autoFilter ref="A1:C572"/>
   <sortState ref="A2:H552">
     <sortCondition ref="B2:B552"/>
   </sortState>
@@ -21725,11 +21859,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add master data site info table
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6003" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6035" uniqueCount="1229">
   <si>
     <t>DATA</t>
   </si>
@@ -3812,6 +3812,33 @@
   </si>
   <si>
     <t>Passwort</t>
+  </si>
+  <si>
+    <t>MASTER_DATA_SITE_INFO</t>
+  </si>
+  <si>
+    <t>Web-Site Überwachung</t>
+  </si>
+  <si>
+    <t>Master data sites</t>
+  </si>
+  <si>
+    <t>Site-Name</t>
+  </si>
+  <si>
+    <t>Site name</t>
+  </si>
+  <si>
+    <t>SITE_PATH</t>
+  </si>
+  <si>
+    <t>TIMEOUT_CHECKING</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Timeout</t>
   </si>
 </sst>
 </file>
@@ -4253,13 +4280,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V109"/>
+  <dimension ref="A1:V110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="M80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M92" sqref="M92"/>
+      <selection pane="bottomRight" activeCell="A110" sqref="A110:B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7589,6 +7616,26 @@
         <v>1092</v>
       </c>
     </row>
+    <row r="110" spans="1:21">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1213</v>
+      </c>
+      <c r="K110" t="s">
+        <v>1221</v>
+      </c>
+      <c r="L110" t="s">
+        <v>1222</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L99">
     <sortState ref="A2:K98">
@@ -7606,13 +7653,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N579"/>
+  <dimension ref="A1:N582"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D447" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F570" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E455" sqref="E455"/>
+      <selection pane="bottomRight" activeCell="H582" sqref="H582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23549,6 +23596,90 @@
       </c>
       <c r="I579" s="7" t="s">
         <v>907</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9">
+      <c r="A580" t="s">
+        <v>153</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C580" t="s">
+        <v>12</v>
+      </c>
+      <c r="D580" t="s">
+        <v>147</v>
+      </c>
+      <c r="E580" t="s">
+        <v>147</v>
+      </c>
+      <c r="F580" t="s">
+        <v>147</v>
+      </c>
+      <c r="G580" t="s">
+        <v>147</v>
+      </c>
+      <c r="H580" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I580" s="7" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="581" spans="1:9">
+      <c r="A581" t="s">
+        <v>153</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C581" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D581" t="s">
+        <v>147</v>
+      </c>
+      <c r="E581" t="s">
+        <v>147</v>
+      </c>
+      <c r="F581" t="s">
+        <v>147</v>
+      </c>
+      <c r="G581" t="s">
+        <v>147</v>
+      </c>
+      <c r="H581" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I581" s="7" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="582" spans="1:9">
+      <c r="A582" t="s">
+        <v>153</v>
+      </c>
+      <c r="B582" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C582" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D582" t="s">
+        <v>147</v>
+      </c>
+      <c r="E582" t="s">
+        <v>147</v>
+      </c>
+      <c r="F582" t="s">
+        <v>147</v>
+      </c>
+      <c r="H582" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="I582" s="7" t="s">
+        <v>1228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enchancements in master data configurations
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6636" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1365">
   <si>
     <t>DATA</t>
   </si>
@@ -4214,6 +4214,39 @@
   </si>
   <si>
     <t>ExamClass,ExamConstraintType</t>
+  </si>
+  <si>
+    <t>masterDataNotificationsMasterDataSubscribersRsp</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Settings/MasterDataNotificationsMasterDataSubscribersRsps</t>
+  </si>
+  <si>
+    <t>masterDataNotificationsId</t>
+  </si>
+  <si>
+    <t>masterDataSubscribers</t>
+  </si>
+  <si>
+    <t>MasterDataSubscribers,NotificationType,AlertCheckStatus</t>
+  </si>
+  <si>
+    <t>notificationType</t>
+  </si>
+  <si>
+    <t>alertCheckStatus</t>
+  </si>
+  <si>
+    <t>checkModuleType</t>
+  </si>
+  <si>
+    <t>MasterDataNotifications,CheckModuleType</t>
+  </si>
+  <si>
+    <t>masterDataNotifications</t>
   </si>
 </sst>
 </file>
@@ -4657,11 +4690,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F71" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="N71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I89" sqref="I89"/>
+      <selection pane="bottomRight" activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6771,7 +6804,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="15" customHeight="1">
+    <row r="65" spans="1:25" ht="15" customHeight="1">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -6797,7 +6830,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="15" customHeight="1">
+    <row r="66" spans="1:25" ht="15" customHeight="1">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -6823,7 +6856,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="15" customHeight="1">
+    <row r="67" spans="1:25" ht="15" customHeight="1">
       <c r="A67" t="s">
         <v>153</v>
       </c>
@@ -6846,7 +6879,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="30" customHeight="1">
+    <row r="68" spans="1:25" ht="30" customHeight="1">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -6872,7 +6905,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="15" customHeight="1">
+    <row r="69" spans="1:25" ht="15" customHeight="1">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -6895,7 +6928,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="15" customHeight="1">
+    <row r="70" spans="1:25" ht="15" customHeight="1">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -6921,7 +6954,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="15" customHeight="1">
+    <row r="71" spans="1:25" ht="15" customHeight="1">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -6947,7 +6980,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="15" customHeight="1">
+    <row r="72" spans="1:25" ht="15" customHeight="1">
       <c r="A72" t="s">
         <v>153</v>
       </c>
@@ -6976,7 +7009,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="15" customHeight="1">
+    <row r="73" spans="1:25" ht="15" customHeight="1">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -6999,7 +7032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="15" customHeight="1">
+    <row r="74" spans="1:25" ht="15" customHeight="1">
       <c r="A74" t="s">
         <v>153</v>
       </c>
@@ -7022,7 +7055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="15" customHeight="1">
+    <row r="75" spans="1:25" ht="15" customHeight="1">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -7048,7 +7081,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="15" customHeight="1">
+    <row r="76" spans="1:25" ht="15" customHeight="1">
       <c r="A76" t="s">
         <v>153</v>
       </c>
@@ -7074,7 +7107,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="15" customHeight="1">
+    <row r="77" spans="1:25" ht="15" customHeight="1">
       <c r="A77" t="s">
         <v>153</v>
       </c>
@@ -7094,7 +7127,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="15" customHeight="1">
+    <row r="78" spans="1:25" ht="15" customHeight="1">
       <c r="A78" t="s">
         <v>153</v>
       </c>
@@ -7129,7 +7162,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="15" customHeight="1">
+    <row r="79" spans="1:25" ht="15" customHeight="1">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -7142,6 +7175,12 @@
       <c r="D79" t="s">
         <v>1211</v>
       </c>
+      <c r="G79" t="s">
+        <v>147</v>
+      </c>
+      <c r="I79" t="s">
+        <v>147</v>
+      </c>
       <c r="O79" t="s">
         <v>1323</v>
       </c>
@@ -7152,7 +7191,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="15" customHeight="1">
+    <row r="80" spans="1:25" ht="15" customHeight="1">
       <c r="A80" t="s">
         <v>153</v>
       </c>
@@ -7165,12 +7204,33 @@
       <c r="D80" t="s">
         <v>1211</v>
       </c>
+      <c r="G80" t="s">
+        <v>147</v>
+      </c>
+      <c r="H80" t="s">
+        <v>147</v>
+      </c>
+      <c r="I80" t="s">
+        <v>147</v>
+      </c>
+      <c r="J80" t="s">
+        <v>147</v>
+      </c>
+      <c r="N80" t="s">
+        <v>1363</v>
+      </c>
       <c r="O80" t="s">
         <v>1324</v>
       </c>
       <c r="P80" t="s">
         <v>1258</v>
       </c>
+      <c r="R80" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="81" spans="1:26" ht="15" customHeight="1">
       <c r="A81" t="s">
@@ -7185,6 +7245,21 @@
       <c r="D81" t="s">
         <v>1211</v>
       </c>
+      <c r="G81" t="s">
+        <v>147</v>
+      </c>
+      <c r="H81" t="s">
+        <v>147</v>
+      </c>
+      <c r="I81" t="s">
+        <v>147</v>
+      </c>
+      <c r="J81" t="s">
+        <v>147</v>
+      </c>
+      <c r="N81" t="s">
+        <v>1359</v>
+      </c>
       <c r="O81" t="s">
         <v>1320</v>
       </c>
@@ -7194,6 +7269,24 @@
       <c r="R81" t="s">
         <v>147</v>
       </c>
+      <c r="S81" s="7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="T81" t="s">
+        <v>1354</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="82" spans="1:26" ht="15" customHeight="1">
       <c r="A82" t="s">
@@ -7208,6 +7301,15 @@
       <c r="D82" t="s">
         <v>1211</v>
       </c>
+      <c r="K82" t="s">
+        <v>147</v>
+      </c>
+      <c r="L82" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M82" t="s">
+        <v>1255</v>
+      </c>
       <c r="O82" t="s">
         <v>1319</v>
       </c>
@@ -7228,6 +7330,12 @@
       <c r="D83" t="s">
         <v>1211</v>
       </c>
+      <c r="G83" t="s">
+        <v>147</v>
+      </c>
+      <c r="I83" t="s">
+        <v>147</v>
+      </c>
       <c r="O83" t="s">
         <v>889</v>
       </c>
@@ -7260,6 +7368,18 @@
       <c r="D84" t="s">
         <v>1211</v>
       </c>
+      <c r="G84" t="s">
+        <v>147</v>
+      </c>
+      <c r="H84" t="s">
+        <v>147</v>
+      </c>
+      <c r="I84" t="s">
+        <v>147</v>
+      </c>
+      <c r="J84" t="s">
+        <v>147</v>
+      </c>
       <c r="N84" t="s">
         <v>1198</v>
       </c>
@@ -7394,6 +7514,18 @@
       <c r="D88" t="s">
         <v>1211</v>
       </c>
+      <c r="G88" t="s">
+        <v>147</v>
+      </c>
+      <c r="H88" t="s">
+        <v>147</v>
+      </c>
+      <c r="I88" t="s">
+        <v>147</v>
+      </c>
+      <c r="J88" t="s">
+        <v>147</v>
+      </c>
       <c r="O88" t="s">
         <v>1325</v>
       </c>
@@ -7401,6 +7533,12 @@
         <v>1261</v>
       </c>
       <c r="R88" t="s">
+        <v>147</v>
+      </c>
+      <c r="W88" t="s">
+        <v>734</v>
+      </c>
+      <c r="X88" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8531,11 +8669,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N637"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D422" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I620" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F424" sqref="F424"/>
+      <selection pane="bottomRight" activeCell="J637" sqref="J637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25665,7 +25803,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="625" spans="1:9">
+    <row r="625" spans="1:10">
       <c r="A625" t="s">
         <v>153</v>
       </c>
@@ -25691,7 +25829,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="626" spans="1:9">
+    <row r="626" spans="1:10">
       <c r="A626" t="s">
         <v>153</v>
       </c>
@@ -25717,7 +25855,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="627" spans="1:9">
+    <row r="627" spans="1:10">
       <c r="A627" t="s">
         <v>153</v>
       </c>
@@ -25742,8 +25880,11 @@
       <c r="I627" s="7" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="628" spans="1:9">
+      <c r="J627" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="628" spans="1:10">
       <c r="A628" t="s">
         <v>153</v>
       </c>
@@ -25769,7 +25910,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="629" spans="1:9">
+    <row r="629" spans="1:10">
       <c r="A629" t="s">
         <v>153</v>
       </c>
@@ -25794,8 +25935,11 @@
       <c r="I629" s="7" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="630" spans="1:9">
+      <c r="J629" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="630" spans="1:10">
       <c r="A630" t="s">
         <v>153</v>
       </c>
@@ -25821,7 +25965,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="631" spans="1:9">
+    <row r="631" spans="1:10">
       <c r="A631" t="s">
         <v>153</v>
       </c>
@@ -25847,7 +25991,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="632" spans="1:9">
+    <row r="632" spans="1:10">
       <c r="A632" t="s">
         <v>153</v>
       </c>
@@ -25873,7 +26017,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="633" spans="1:9">
+    <row r="633" spans="1:10">
       <c r="A633" t="s">
         <v>153</v>
       </c>
@@ -25898,8 +26042,11 @@
       <c r="I633" s="7" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="634" spans="1:9">
+      <c r="J633" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="634" spans="1:10">
       <c r="A634" t="s">
         <v>153</v>
       </c>
@@ -25925,7 +26072,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="635" spans="1:9">
+    <row r="635" spans="1:10">
       <c r="A635" t="s">
         <v>153</v>
       </c>
@@ -25950,8 +26097,11 @@
       <c r="I635" s="7" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="636" spans="1:9">
+      <c r="J635" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="636" spans="1:10">
       <c r="A636" t="s">
         <v>153</v>
       </c>
@@ -25964,9 +26114,6 @@
       <c r="D636" t="s">
         <v>147</v>
       </c>
-      <c r="E636" t="s">
-        <v>147</v>
-      </c>
       <c r="F636" t="s">
         <v>147</v>
       </c>
@@ -25977,7 +26124,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="637" spans="1:9">
+    <row r="637" spans="1:10">
       <c r="A637" t="s">
         <v>153</v>
       </c>
@@ -26001,6 +26148,9 @@
       </c>
       <c r="I637" s="7" t="s">
         <v>1312</v>
+      </c>
+      <c r="J637" t="s">
+        <v>1358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
master data configuration improvements
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6699" uniqueCount="1365">
   <si>
     <t>DATA</t>
   </si>
@@ -4691,10 +4691,10 @@
   <dimension ref="A1:Z124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="N71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="U71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N81" sqref="N81"/>
+      <selection pane="bottomRight" activeCell="B80" sqref="A80:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6804,7 +6804,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="15" customHeight="1">
+    <row r="65" spans="1:26" ht="15" customHeight="1">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="15" customHeight="1">
+    <row r="66" spans="1:26" ht="15" customHeight="1">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="15" customHeight="1">
+    <row r="67" spans="1:26" ht="15" customHeight="1">
       <c r="A67" t="s">
         <v>153</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="30" customHeight="1">
+    <row r="68" spans="1:26" ht="30" customHeight="1">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="15" customHeight="1">
+    <row r="69" spans="1:26" ht="15" customHeight="1">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="15" customHeight="1">
+    <row r="70" spans="1:26" ht="15" customHeight="1">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="15" customHeight="1">
+    <row r="71" spans="1:26" ht="15" customHeight="1">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="15" customHeight="1">
+    <row r="72" spans="1:26" ht="15" customHeight="1">
       <c r="A72" t="s">
         <v>153</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="15" customHeight="1">
+    <row r="73" spans="1:26" ht="15" customHeight="1">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="15" customHeight="1">
+    <row r="74" spans="1:26" ht="15" customHeight="1">
       <c r="A74" t="s">
         <v>153</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="15" customHeight="1">
+    <row r="75" spans="1:26" ht="15" customHeight="1">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="15" customHeight="1">
+    <row r="76" spans="1:26" ht="15" customHeight="1">
       <c r="A76" t="s">
         <v>153</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="15" customHeight="1">
+    <row r="77" spans="1:26" ht="15" customHeight="1">
       <c r="A77" t="s">
         <v>153</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="15" customHeight="1">
+    <row r="78" spans="1:26" ht="15" customHeight="1">
       <c r="A78" t="s">
         <v>153</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="15" customHeight="1">
+    <row r="79" spans="1:26" ht="15" customHeight="1">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="15" customHeight="1">
+    <row r="80" spans="1:26" ht="15" customHeight="1">
       <c r="A80" t="s">
         <v>153</v>
       </c>
@@ -7229,6 +7229,9 @@
         <v>147</v>
       </c>
       <c r="Y80" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z80" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8669,11 +8672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N637"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I620" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D617" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J637" sqref="J637"/>
+      <selection pane="bottomRight" activeCell="E634" sqref="E634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24964,6 +24967,9 @@
       <c r="F592" t="s">
         <v>147</v>
       </c>
+      <c r="G592" t="s">
+        <v>147</v>
+      </c>
       <c r="H592" s="7" t="s">
         <v>787</v>
       </c>
@@ -24990,6 +24996,9 @@
       <c r="F593" t="s">
         <v>147</v>
       </c>
+      <c r="G593" t="s">
+        <v>147</v>
+      </c>
       <c r="H593" s="7" t="s">
         <v>1326</v>
       </c>
@@ -25016,6 +25025,9 @@
       <c r="F594" t="s">
         <v>147</v>
       </c>
+      <c r="G594" t="s">
+        <v>147</v>
+      </c>
       <c r="H594" s="7" t="s">
         <v>1225</v>
       </c>
@@ -25198,6 +25210,9 @@
       <c r="F601" t="s">
         <v>147</v>
       </c>
+      <c r="G601" t="s">
+        <v>147</v>
+      </c>
       <c r="H601" s="7" t="s">
         <v>1332</v>
       </c>
@@ -25224,6 +25239,9 @@
       <c r="F602" t="s">
         <v>147</v>
       </c>
+      <c r="G602" t="s">
+        <v>147</v>
+      </c>
       <c r="H602" s="7" t="s">
         <v>1283</v>
       </c>
@@ -25250,6 +25268,9 @@
       <c r="F603" t="s">
         <v>147</v>
       </c>
+      <c r="G603" t="s">
+        <v>147</v>
+      </c>
       <c r="H603" s="7" t="s">
         <v>871</v>
       </c>
@@ -25276,6 +25297,9 @@
       <c r="F604" t="s">
         <v>147</v>
       </c>
+      <c r="G604" t="s">
+        <v>147</v>
+      </c>
       <c r="H604" s="7" t="s">
         <v>1273</v>
       </c>
@@ -25302,6 +25326,9 @@
       <c r="F605" t="s">
         <v>147</v>
       </c>
+      <c r="G605" t="s">
+        <v>147</v>
+      </c>
       <c r="H605" s="7" t="s">
         <v>787</v>
       </c>
@@ -25328,6 +25355,9 @@
       <c r="F606" t="s">
         <v>147</v>
       </c>
+      <c r="G606" t="s">
+        <v>147</v>
+      </c>
       <c r="H606" s="7" t="s">
         <v>1333</v>
       </c>
@@ -25458,6 +25488,9 @@
       <c r="F611" t="s">
         <v>147</v>
       </c>
+      <c r="G611" t="s">
+        <v>147</v>
+      </c>
       <c r="H611" s="7" t="s">
         <v>787</v>
       </c>
@@ -25484,6 +25517,9 @@
       <c r="F612" t="s">
         <v>147</v>
       </c>
+      <c r="G612" t="s">
+        <v>147</v>
+      </c>
       <c r="H612" s="7" t="s">
         <v>1335</v>
       </c>
@@ -25510,6 +25546,9 @@
       <c r="F613" t="s">
         <v>147</v>
       </c>
+      <c r="G613" t="s">
+        <v>147</v>
+      </c>
       <c r="H613" s="7" t="s">
         <v>1336</v>
       </c>
@@ -25536,6 +25575,9 @@
       <c r="F614" t="s">
         <v>147</v>
       </c>
+      <c r="G614" t="s">
+        <v>147</v>
+      </c>
       <c r="H614" s="7" t="s">
         <v>1225</v>
       </c>
@@ -25848,6 +25890,9 @@
       <c r="F626" t="s">
         <v>147</v>
       </c>
+      <c r="G626" t="s">
+        <v>147</v>
+      </c>
       <c r="H626" s="7" t="s">
         <v>1294</v>
       </c>
@@ -25874,6 +25919,9 @@
       <c r="F627" t="s">
         <v>147</v>
       </c>
+      <c r="G627" t="s">
+        <v>147</v>
+      </c>
       <c r="H627" s="7" t="s">
         <v>1340</v>
       </c>
@@ -25929,6 +25977,9 @@
       <c r="F629" t="s">
         <v>147</v>
       </c>
+      <c r="G629" t="s">
+        <v>147</v>
+      </c>
       <c r="H629" s="7" t="s">
         <v>1268</v>
       </c>
@@ -25958,6 +26009,9 @@
       <c r="F630" t="s">
         <v>147</v>
       </c>
+      <c r="G630" t="s">
+        <v>147</v>
+      </c>
       <c r="H630" s="7" t="s">
         <v>1345</v>
       </c>
@@ -25984,6 +26038,9 @@
       <c r="F631" t="s">
         <v>147</v>
       </c>
+      <c r="G631" t="s">
+        <v>147</v>
+      </c>
       <c r="H631" s="7" t="s">
         <v>1327</v>
       </c>
@@ -26010,6 +26067,9 @@
       <c r="F632" t="s">
         <v>147</v>
       </c>
+      <c r="G632" t="s">
+        <v>147</v>
+      </c>
       <c r="H632" s="7" t="s">
         <v>1341</v>
       </c>
@@ -26030,10 +26090,7 @@
       <c r="D633" t="s">
         <v>147</v>
       </c>
-      <c r="E633" t="s">
-        <v>147</v>
-      </c>
-      <c r="F633" t="s">
+      <c r="G633" t="s">
         <v>147</v>
       </c>
       <c r="H633" s="7" t="s">
@@ -26059,10 +26116,7 @@
       <c r="D634" t="s">
         <v>147</v>
       </c>
-      <c r="E634" t="s">
-        <v>147</v>
-      </c>
-      <c r="F634" t="s">
+      <c r="G634" t="s">
         <v>147</v>
       </c>
       <c r="H634" s="7" t="s">
@@ -26091,6 +26145,9 @@
       <c r="F635" t="s">
         <v>147</v>
       </c>
+      <c r="G635" t="s">
+        <v>147</v>
+      </c>
       <c r="H635" s="7" t="s">
         <v>1339</v>
       </c>
@@ -26117,6 +26174,9 @@
       <c r="F636" t="s">
         <v>147</v>
       </c>
+      <c r="G636" t="s">
+        <v>147</v>
+      </c>
       <c r="H636" s="7" t="s">
         <v>1339</v>
       </c>
@@ -26141,6 +26201,9 @@
         <v>147</v>
       </c>
       <c r="F637" t="s">
+        <v>147</v>
+      </c>
+      <c r="G637" t="s">
         <v>147</v>
       </c>
       <c r="H637" s="7" t="s">
@@ -26200,19 +26263,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -26222,7 +26285,7 @@
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -26242,7 +26305,7 @@
       <c r="A2" t="s">
         <v>153</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>764</v>
       </c>
       <c r="C2" t="s">
@@ -26256,7 +26319,7 @@
       <c r="A3" t="s">
         <v>153</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>776</v>
       </c>
       <c r="C3" t="s">
@@ -26270,7 +26333,7 @@
       <c r="A4" t="s">
         <v>153</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>777</v>
       </c>
       <c r="C4" t="s">
@@ -26284,7 +26347,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>1072</v>
       </c>
       <c r="E5" t="s">
@@ -26295,16 +26358,28 @@
       <c r="A6" t="s">
         <v>153</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>1007</v>
       </c>
       <c r="E6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E7" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add excel export. refactor ApplicationLogToShow view.
</commit_message>
<xml_diff>
--- a/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
+++ b/MasterDataModule/Generation/MasterDataModule.Generation/Declarations/Stammdaten.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7323" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7325" uniqueCount="1413">
   <si>
     <t>DATA</t>
   </si>
@@ -4388,6 +4388,9 @@
   </si>
   <si>
     <t>PermissionDescription</t>
+  </si>
+  <si>
+    <t>ExcelExport</t>
   </si>
 </sst>
 </file>
@@ -4497,7 +4500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4528,6 +4531,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4829,13 +4838,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB133"/>
+  <dimension ref="A1:AC133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W83" sqref="W83"/>
+      <selection pane="bottomRight" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4861,10 +4870,10 @@
     <col min="22" max="22" width="19" style="7" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="28" max="28" width="32" customWidth="1"/>
+    <col min="28" max="28" width="32" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="30">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
@@ -4946,11 +4955,14 @@
       <c r="AA1" s="10" t="s">
         <v>1410</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="16" t="s">
         <v>1411</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1">
+      <c r="AC1" s="10" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -4975,12 +4987,12 @@
       <c r="AA2">
         <v>1</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AB2" s="17" t="str">
         <f>O2</f>
         <v>Applikation-Logs</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5017,12 +5029,12 @@
       <c r="AA3">
         <v>2</v>
       </c>
-      <c r="AB3" t="str">
+      <c r="AB3" s="17" t="str">
         <f t="shared" ref="AB3:AB66" si="0">O3</f>
         <v>ARGE-Version</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1">
+    <row r="4" spans="1:29" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5050,12 +5062,12 @@
       <c r="AA4">
         <v>3</v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AB4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Behörde</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="105" customHeight="1">
+    <row r="5" spans="1:29" ht="105" customHeight="1">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -5092,12 +5104,12 @@
       <c r="AA5">
         <v>4</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AB5" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Fahrschulgemeinschaft</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1">
+    <row r="6" spans="1:29" ht="15" customHeight="1">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -5125,12 +5137,12 @@
       <c r="AA6">
         <v>5</v>
       </c>
-      <c r="AB6" t="str">
+      <c r="AB6" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Mitglied der Fahrschulgemeinschaft</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1">
+    <row r="7" spans="1:29" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -5176,12 +5188,15 @@
       <c r="AA7">
         <v>6</v>
       </c>
-      <c r="AB7" t="str">
+      <c r="AB7" s="17" t="str">
         <f t="shared" si="0"/>
         <v>FE-Produkt</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1">
+      <c r="AC7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -5212,12 +5227,12 @@
       <c r="AA8">
         <v>7</v>
       </c>
-      <c r="AB8" t="str">
+      <c r="AB8" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Rechtsgrund/Klasse</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1">
+    <row r="9" spans="1:29" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -5248,12 +5263,12 @@
       <c r="AA9">
         <v>8</v>
       </c>
-      <c r="AB9" t="str">
+      <c r="AB9" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Lokalisierung</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1">
+    <row r="10" spans="1:29" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -5290,12 +5305,12 @@
       <c r="AA10">
         <v>9</v>
       </c>
-      <c r="AB10" t="str">
+      <c r="AB10" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Fahrschule</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -5326,12 +5341,12 @@
       <c r="AA11">
         <v>10</v>
       </c>
-      <c r="AB11" t="str">
+      <c r="AB11" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Anerkennung der Fahrschule</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1">
+    <row r="12" spans="1:29" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -5362,12 +5377,12 @@
       <c r="AA12">
         <v>11</v>
       </c>
-      <c r="AB12" t="str">
+      <c r="AB12" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Fahrschule Information</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="105">
+    <row r="13" spans="1:29" ht="105">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -5410,12 +5425,12 @@
       <c r="AA13">
         <v>12</v>
       </c>
-      <c r="AB13" t="str">
+      <c r="AB13" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Klasse</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1">
+    <row r="14" spans="1:29" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -5451,12 +5466,12 @@
       <c r="AA14">
         <v>13</v>
       </c>
-      <c r="AB14" t="str">
+      <c r="AB14" s="17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ARGE-Klassenbezeichnung </v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1">
+    <row r="15" spans="1:29" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5489,12 +5504,12 @@
       <c r="AA15">
         <v>14</v>
       </c>
-      <c r="AB15" t="str">
+      <c r="AB15" s="17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Inklusivklasse </v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:29" ht="30">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -5527,7 +5542,7 @@
       <c r="AA16">
         <v>15</v>
       </c>
-      <c r="AB16" t="str">
+      <c r="AB16" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung Alt-Klasse zu einer FE-Klasse</v>
       </c>
@@ -5565,7 +5580,7 @@
       <c r="AA17">
         <v>16</v>
       </c>
-      <c r="AB17" t="str">
+      <c r="AB17" s="17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Voraussetzungsklasse </v>
       </c>
@@ -5603,7 +5618,7 @@
       <c r="AA18">
         <v>17</v>
       </c>
-      <c r="AB18" t="str">
+      <c r="AB18" s="17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Ausschlussklasse </v>
       </c>
@@ -5660,7 +5675,7 @@
       <c r="AA19">
         <v>18</v>
       </c>
-      <c r="AB19" t="str">
+      <c r="AB19" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Auflagen/Beschränkungen</v>
       </c>
@@ -5696,7 +5711,7 @@
       <c r="AA20">
         <v>19</v>
       </c>
-      <c r="AB20" t="str">
+      <c r="AB20" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung FE-Klasse zu einer FE-Auflage</v>
       </c>
@@ -5726,7 +5741,7 @@
       <c r="AA21">
         <v>20</v>
       </c>
-      <c r="AB21" t="str">
+      <c r="AB21" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Prüfleistungsergebnis</v>
       </c>
@@ -5786,7 +5801,7 @@
       <c r="AA22">
         <v>21</v>
       </c>
-      <c r="AB22" t="str">
+      <c r="AB22" s="17" t="str">
         <f t="shared" si="0"/>
         <v>FE-Anerkennung</v>
       </c>
@@ -5822,7 +5837,7 @@
       <c r="AA23">
         <v>22</v>
       </c>
-      <c r="AB23" t="str">
+      <c r="AB23" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung FE-Klasse zu einer Anerkennung</v>
       </c>
@@ -5855,7 +5870,7 @@
       <c r="AA24">
         <v>23</v>
       </c>
-      <c r="AB24" t="str">
+      <c r="AB24" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Prüfraum</v>
       </c>
@@ -5912,12 +5927,12 @@
       <c r="AA25">
         <v>24</v>
       </c>
-      <c r="AB25" t="str">
+      <c r="AB25" s="17" t="str">
         <f t="shared" si="0"/>
         <v>FE-Prüfort</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" ht="30">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -5948,7 +5963,7 @@
       <c r="AA26">
         <v>25</v>
       </c>
-      <c r="AB26" t="str">
+      <c r="AB26" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung FE-Anerkennung zu einem FE-Prüfort</v>
       </c>
@@ -6005,7 +6020,7 @@
       <c r="AA27">
         <v>26</v>
       </c>
-      <c r="AB27" t="str">
+      <c r="AB27" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Feiertag</v>
       </c>
@@ -6041,7 +6056,7 @@
       <c r="AA28">
         <v>27</v>
       </c>
-      <c r="AB28" t="str">
+      <c r="AB28" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung Bundesland zu einem Feiertag</v>
       </c>
@@ -6086,7 +6101,7 @@
       <c r="AA29">
         <v>28</v>
       </c>
-      <c r="AB29" t="str">
+      <c r="AB29" s="17" t="str">
         <f t="shared" si="0"/>
         <v>FE-Sprache</v>
       </c>
@@ -6122,7 +6137,7 @@
       <c r="AA30">
         <v>29</v>
       </c>
-      <c r="AB30" t="str">
+      <c r="AB30" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Rechtsgrund</v>
       </c>
@@ -6179,7 +6194,7 @@
       <c r="AA31">
         <v>30</v>
       </c>
-      <c r="AB31" t="str">
+      <c r="AB31" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Treffpunkt</v>
       </c>
@@ -6215,7 +6230,7 @@
       <c r="AA32">
         <v>31</v>
       </c>
-      <c r="AB32" t="str">
+      <c r="AB32" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung FE-Treffpunkt zu einer Organisationseinheit</v>
       </c>
@@ -6260,7 +6275,7 @@
       <c r="AA33">
         <v>32</v>
       </c>
-      <c r="AB33" t="str">
+      <c r="AB33" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Fehlermeldung</v>
       </c>
@@ -6305,7 +6320,7 @@
       <c r="AA34">
         <v>33</v>
       </c>
-      <c r="AB34" t="str">
+      <c r="AB34" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Rückgabegrund</v>
       </c>
@@ -6350,7 +6365,7 @@
       <c r="AA35">
         <v>34</v>
       </c>
-      <c r="AB35" t="str">
+      <c r="AB35" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Fahrschulinformationstyp</v>
       </c>
@@ -6383,7 +6398,7 @@
       <c r="AA36">
         <v>35</v>
       </c>
-      <c r="AB36" t="str">
+      <c r="AB36" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Auszahlungsrecht</v>
       </c>
@@ -6416,7 +6431,7 @@
       <c r="AA37">
         <v>36</v>
       </c>
-      <c r="AB37" t="str">
+      <c r="AB37" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Mitarbeiter</v>
       </c>
@@ -6461,7 +6476,7 @@
       <c r="AA38">
         <v>37</v>
       </c>
-      <c r="AB38" t="str">
+      <c r="AB38" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Kostenstelle</v>
       </c>
@@ -6506,7 +6521,7 @@
       <c r="AA39">
         <v>38</v>
       </c>
-      <c r="AB39" t="str">
+      <c r="AB39" s="17" t="str">
         <f t="shared" si="0"/>
         <v>OE/TSC</v>
       </c>
@@ -6551,7 +6566,7 @@
       <c r="AA40">
         <v>39</v>
       </c>
-      <c r="AB40" t="str">
+      <c r="AB40" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Rolle</v>
       </c>
@@ -6596,7 +6611,7 @@
       <c r="AA41">
         <v>40</v>
       </c>
-      <c r="AB41" t="str">
+      <c r="AB41" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Vorgesetzter</v>
       </c>
@@ -6638,7 +6653,7 @@
       <c r="AA42">
         <v>41</v>
       </c>
-      <c r="AB42" t="str">
+      <c r="AB42" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Login Information</v>
       </c>
@@ -6671,7 +6686,7 @@
       <c r="AA43">
         <v>42</v>
       </c>
-      <c r="AB43" t="str">
+      <c r="AB43" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnungsarten zwischen Mitarbeiter und OE</v>
       </c>
@@ -6704,7 +6719,7 @@
       <c r="AA44">
         <v>43</v>
       </c>
-      <c r="AB44" t="str">
+      <c r="AB44" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Mitfahrerart</v>
       </c>
@@ -6746,7 +6761,7 @@
       <c r="AA45">
         <v>44</v>
       </c>
-      <c r="AB45" t="str">
+      <c r="AB45" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung Verfügbarer Prüfschritt zu Prüfschritt</v>
       </c>
@@ -6776,12 +6791,12 @@
       <c r="AA46">
         <v>45</v>
       </c>
-      <c r="AB46" t="str">
+      <c r="AB46" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Systemtext</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" ht="30">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -6818,7 +6833,7 @@
       <c r="AA47">
         <v>46</v>
       </c>
-      <c r="AB47" t="str">
+      <c r="AB47" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung sptrachabhängiger Systemtexte zu einem Systemtext</v>
       </c>
@@ -6869,7 +6884,7 @@
       <c r="AA48">
         <v>47</v>
       </c>
-      <c r="AB48" t="str">
+      <c r="AB48" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt</v>
       </c>
@@ -6902,7 +6917,7 @@
       <c r="AA49">
         <v>48</v>
       </c>
-      <c r="AB49" t="str">
+      <c r="AB49" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Arbeitswerte</v>
       </c>
@@ -6944,7 +6959,7 @@
       <c r="AA50">
         <v>49</v>
       </c>
-      <c r="AB50" t="str">
+      <c r="AB50" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Lokalisierung</v>
       </c>
@@ -6974,7 +6989,7 @@
       <c r="AA51">
         <v>50</v>
       </c>
-      <c r="AB51" t="str">
+      <c r="AB51" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-Prüfschritt</v>
       </c>
@@ -7004,7 +7019,7 @@
       <c r="AA52">
         <v>51</v>
       </c>
-      <c r="AB52" t="str">
+      <c r="AB52" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-Nächste Prüfung</v>
       </c>
@@ -7037,7 +7052,7 @@
       <c r="AA53">
         <v>52</v>
       </c>
-      <c r="AB53" t="str">
+      <c r="AB53" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-SP-Intervall</v>
       </c>
@@ -7070,7 +7085,7 @@
       <c r="AA54">
         <v>53</v>
       </c>
-      <c r="AB54" t="str">
+      <c r="AB54" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-AU-OBD-Status</v>
       </c>
@@ -7100,7 +7115,7 @@
       <c r="AA55">
         <v>54</v>
       </c>
-      <c r="AB55" t="str">
+      <c r="AB55" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-optische Mängel</v>
       </c>
@@ -7130,7 +7145,7 @@
       <c r="AA56">
         <v>55</v>
       </c>
-      <c r="AB56" t="str">
+      <c r="AB56" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-PFP-Baugruppen</v>
       </c>
@@ -7172,7 +7187,7 @@
       <c r="AA57">
         <v>56</v>
       </c>
-      <c r="AB57" t="str">
+      <c r="AB57" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Zuordnung PFP-Prüfpositionen zu PFP-Baugruppe</v>
       </c>
@@ -7202,7 +7217,7 @@
       <c r="AA58">
         <v>57</v>
       </c>
-      <c r="AB58" t="str">
+      <c r="AB58" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-PFP-Prüfpositionen</v>
       </c>
@@ -7232,7 +7247,7 @@
       <c r="AA59">
         <v>58</v>
       </c>
-      <c r="AB59" t="str">
+      <c r="AB59" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-PFP-Fahrzeugtypen (Silhouetten)</v>
       </c>
@@ -7262,7 +7277,7 @@
       <c r="AA60">
         <v>59</v>
       </c>
-      <c r="AB60" t="str">
+      <c r="AB60" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-Produktklassengruppe</v>
       </c>
@@ -7295,7 +7310,7 @@
       <c r="AA61">
         <v>60</v>
       </c>
-      <c r="AB61" t="str">
+      <c r="AB61" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Kombinationstypen</v>
       </c>
@@ -7328,7 +7343,7 @@
       <c r="AA62">
         <v>61</v>
       </c>
-      <c r="AB62" t="str">
+      <c r="AB62" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Materialgruppen</v>
       </c>
@@ -7361,7 +7376,7 @@
       <c r="AA63">
         <v>62</v>
       </c>
-      <c r="AB63" t="str">
+      <c r="AB63" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Gewichtsklassen</v>
       </c>
@@ -7394,7 +7409,7 @@
       <c r="AA64">
         <v>63</v>
       </c>
-      <c r="AB64" t="str">
+      <c r="AB64" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Objekttypen</v>
       </c>
@@ -7427,7 +7442,7 @@
       <c r="AA65">
         <v>64</v>
       </c>
-      <c r="AB65" t="str">
+      <c r="AB65" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produkt-Produkttypen</v>
       </c>
@@ -7457,7 +7472,7 @@
       <c r="AA66">
         <v>65</v>
       </c>
-      <c r="AB66" t="str">
+      <c r="AB66" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Produktklasse-Mangelbewertungen</v>
       </c>
@@ -7490,7 +7505,7 @@
       <c r="AA67">
         <v>66</v>
       </c>
-      <c r="AB67" t="str">
+      <c r="AB67" s="17" t="str">
         <f t="shared" ref="AB67:AB130" si="1">O67</f>
         <v>Produkt-Statistikgruppe</v>
       </c>
@@ -7520,7 +7535,7 @@
       <c r="AA68">
         <v>67</v>
       </c>
-      <c r="AB68" t="str">
+      <c r="AB68" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Produktklasse-Ergebnisfeld</v>
       </c>
@@ -7553,7 +7568,7 @@
       <c r="AA69">
         <v>68</v>
       </c>
-      <c r="AB69" t="str">
+      <c r="AB69" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kunde-Steuerklasse</v>
       </c>
@@ -7586,7 +7601,7 @@
       <c r="AA70">
         <v>69</v>
       </c>
-      <c r="AB70" t="str">
+      <c r="AB70" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Produkt-Steuercode</v>
       </c>
@@ -7622,7 +7637,7 @@
       <c r="AA71">
         <v>70</v>
       </c>
-      <c r="AB71" t="str">
+      <c r="AB71" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Steuerkombination</v>
       </c>
@@ -7652,7 +7667,7 @@
       <c r="AA72">
         <v>71</v>
       </c>
-      <c r="AB72" t="str">
+      <c r="AB72" s="17" t="str">
         <f t="shared" si="1"/>
         <v>berichtende Stellen</v>
       </c>
@@ -7682,7 +7697,7 @@
       <c r="AA73">
         <v>72</v>
       </c>
-      <c r="AB73" t="str">
+      <c r="AB73" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Produktklasse-Zeiträume</v>
       </c>
@@ -7715,7 +7730,7 @@
       <c r="AA74">
         <v>73</v>
       </c>
-      <c r="AB74" t="str">
+      <c r="AB74" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Mehrwertsteuersatz</v>
       </c>
@@ -7748,7 +7763,7 @@
       <c r="AA75">
         <v>74</v>
       </c>
-      <c r="AB75" t="str">
+      <c r="AB75" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Auszahlungsgrund</v>
       </c>
@@ -7775,7 +7790,7 @@
       <c r="AA76">
         <v>75</v>
       </c>
-      <c r="AB76" t="str">
+      <c r="AB76" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Hintergrundprozess Monitor</v>
       </c>
@@ -7826,7 +7841,7 @@
       <c r="AA77">
         <v>76</v>
       </c>
-      <c r="AB77" t="str">
+      <c r="AB77" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Hintergrundprozess Einstellungen</v>
       </c>
@@ -7862,7 +7877,7 @@
       <c r="AA78">
         <v>77</v>
       </c>
-      <c r="AB78" t="str">
+      <c r="AB78" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Monitor Einstellungen</v>
       </c>
@@ -7913,7 +7928,7 @@
       <c r="AA79">
         <v>78</v>
       </c>
-      <c r="AB79" t="str">
+      <c r="AB79" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Überwachungsnachrichten Einstellungen</v>
       </c>
@@ -7976,7 +7991,7 @@
       <c r="AA80">
         <v>79</v>
       </c>
-      <c r="AB80" t="str">
+      <c r="AB80" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Überwachungsnachrichten</v>
       </c>
@@ -8012,7 +8027,7 @@
       <c r="AA81">
         <v>80</v>
       </c>
-      <c r="AB81" t="str">
+      <c r="AB81" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Überwachungsnachrichten Empfänger</v>
       </c>
@@ -8057,7 +8072,7 @@
       <c r="AA82">
         <v>81</v>
       </c>
-      <c r="AB82" t="str">
+      <c r="AB82" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Berechtigung</v>
       </c>
@@ -8123,7 +8138,7 @@
       <c r="AA83">
         <v>82</v>
       </c>
-      <c r="AB83" t="str">
+      <c r="AB83" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Rolle</v>
       </c>
@@ -8162,7 +8177,7 @@
       <c r="AA84">
         <v>83</v>
       </c>
-      <c r="AB84" t="str">
+      <c r="AB84" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Berechtigung</v>
       </c>
@@ -8189,7 +8204,7 @@
       <c r="AA85">
         <v>84</v>
       </c>
-      <c r="AB85" t="str">
+      <c r="AB85" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Web-Site Monitor</v>
       </c>
@@ -8240,7 +8255,7 @@
       <c r="AA86">
         <v>85</v>
       </c>
-      <c r="AB86" t="str">
+      <c r="AB86" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Web-Site Einstellungen</v>
       </c>
@@ -8288,7 +8303,7 @@
       <c r="AA87">
         <v>86</v>
       </c>
-      <c r="AB87" t="str">
+      <c r="AB87" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Monitor Empfänger</v>
       </c>
@@ -8336,7 +8351,7 @@
       <c r="AA88">
         <v>87</v>
       </c>
-      <c r="AB88" t="str">
+      <c r="AB88" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Benutzer</v>
       </c>
@@ -8363,7 +8378,7 @@
       <c r="AA89">
         <v>88</v>
       </c>
-      <c r="AB89" t="str">
+      <c r="AB89" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Web-Services Monitor</v>
       </c>
@@ -8414,7 +8429,7 @@
       <c r="AA90">
         <v>89</v>
       </c>
-      <c r="AB90" t="str">
+      <c r="AB90" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Web-Services Einstellungen</v>
       </c>
@@ -8441,7 +8456,7 @@
       <c r="AA91">
         <v>90</v>
       </c>
-      <c r="AB91" t="str">
+      <c r="AB91" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Windows Services Monitor</v>
       </c>
@@ -8492,7 +8507,7 @@
       <c r="AA92">
         <v>91</v>
       </c>
-      <c r="AB92" t="str">
+      <c r="AB92" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Windows Services Einstellungen</v>
       </c>
@@ -8525,7 +8540,7 @@
       <c r="AA93">
         <v>92</v>
       </c>
-      <c r="AB93" t="str">
+      <c r="AB93" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Produkt-Arbeitsgebiet</v>
       </c>
@@ -8558,7 +8573,7 @@
       <c r="AA94">
         <v>93</v>
       </c>
-      <c r="AB94" t="str">
+      <c r="AB94" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kunde-Rechnungsintervalle</v>
       </c>
@@ -8591,7 +8606,7 @@
       <c r="AA95">
         <v>94</v>
       </c>
-      <c r="AB95" t="str">
+      <c r="AB95" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kunde-Funktionen Ansprechpartner</v>
       </c>
@@ -8624,7 +8639,7 @@
       <c r="AA96">
         <v>95</v>
       </c>
-      <c r="AB96" t="str">
+      <c r="AB96" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kunde-Informationstyp</v>
       </c>
@@ -8657,7 +8672,7 @@
       <c r="AA97">
         <v>96</v>
       </c>
-      <c r="AB97" t="str">
+      <c r="AB97" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Bundeslandgruppe</v>
       </c>
@@ -8699,7 +8714,7 @@
       <c r="AA98">
         <v>97</v>
       </c>
-      <c r="AB98" t="str">
+      <c r="AB98" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Bundesland</v>
       </c>
@@ -8744,7 +8759,7 @@
       <c r="AA99">
         <v>98</v>
       </c>
-      <c r="AB99" t="str">
+      <c r="AB99" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Zuordnung Bundeslandgruppe zu einem Bundesland</v>
       </c>
@@ -8777,7 +8792,7 @@
       <c r="AA100">
         <v>99</v>
       </c>
-      <c r="AB100" t="str">
+      <c r="AB100" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stornogrund</v>
       </c>
@@ -8810,7 +8825,7 @@
       <c r="AA101">
         <v>100</v>
       </c>
-      <c r="AB101" t="str">
+      <c r="AB101" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kunde-Partnerrollen</v>
       </c>
@@ -8846,7 +8861,7 @@
       <c r="AA102">
         <v>101</v>
       </c>
-      <c r="AB102" t="str">
+      <c r="AB102" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Anerkennung</v>
       </c>
@@ -8891,7 +8906,7 @@
       <c r="AA103">
         <v>102</v>
       </c>
-      <c r="AB103" t="str">
+      <c r="AB103" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Zuordnung Arbeitsgebiet zu Anerkennung</v>
       </c>
@@ -8924,7 +8939,7 @@
       <c r="AA104">
         <v>103</v>
       </c>
-      <c r="AB104" t="str">
+      <c r="AB104" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Produkt-Anerkennungstyp</v>
       </c>
@@ -8957,7 +8972,7 @@
       <c r="AA105">
         <v>104</v>
       </c>
-      <c r="AB105" t="str">
+      <c r="AB105" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Abrechnungsvariante</v>
       </c>
@@ -8996,7 +9011,7 @@
       <c r="AA106">
         <v>105</v>
       </c>
-      <c r="AB106" t="str">
+      <c r="AB106" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Buchungskreis</v>
       </c>
@@ -9029,7 +9044,7 @@
       <c r="AA107">
         <v>106</v>
       </c>
-      <c r="AB107" t="str">
+      <c r="AB107" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Bankverbindung</v>
       </c>
@@ -9065,7 +9080,7 @@
       <c r="AA108">
         <v>107</v>
       </c>
-      <c r="AB108" t="str">
+      <c r="AB108" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Kostenstelle</v>
       </c>
@@ -9110,7 +9125,7 @@
       <c r="AA109">
         <v>108</v>
       </c>
-      <c r="AB109" t="str">
+      <c r="AB109" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Zuordnung Preise zu Kostenstelle</v>
       </c>
@@ -9155,7 +9170,7 @@
       <c r="AA110">
         <v>109</v>
       </c>
-      <c r="AB110" t="str">
+      <c r="AB110" s="17" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Kostenstellenverantwortlicher </v>
       </c>
@@ -9191,7 +9206,7 @@
       <c r="AA111">
         <v>110</v>
       </c>
-      <c r="AB111" t="str">
+      <c r="AB111" s="17" t="str">
         <f t="shared" si="1"/>
         <v>OE-Information</v>
       </c>
@@ -9224,7 +9239,7 @@
       <c r="AA112">
         <v>111</v>
       </c>
-      <c r="AB112" t="str">
+      <c r="AB112" s="17" t="str">
         <f t="shared" si="1"/>
         <v>OE-Prüfmittel</v>
       </c>
@@ -9266,7 +9281,7 @@
       <c r="AA113">
         <v>112</v>
       </c>
-      <c r="AB113" t="str">
+      <c r="AB113" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Organisationseinheit</v>
       </c>
@@ -9299,7 +9314,7 @@
       <c r="AA114">
         <v>113</v>
       </c>
-      <c r="AB114" t="str">
+      <c r="AB114" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Hierarchietyp</v>
       </c>
@@ -9338,7 +9353,7 @@
       <c r="AA115">
         <v>114</v>
       </c>
-      <c r="AB115" t="str">
+      <c r="AB115" s="17" t="str">
         <f t="shared" si="1"/>
         <v>OE-Type</v>
       </c>
@@ -9377,7 +9392,7 @@
       <c r="AA116">
         <v>115</v>
       </c>
-      <c r="AB116" t="str">
+      <c r="AB116" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Spalte</v>
       </c>
@@ -9416,7 +9431,7 @@
       <c r="AA117">
         <v>116</v>
       </c>
-      <c r="AB117" t="str">
+      <c r="AB117" s="17" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Land </v>
       </c>
@@ -9455,7 +9470,7 @@
       <c r="AA118">
         <v>117</v>
       </c>
-      <c r="AB118" t="str">
+      <c r="AB118" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Sprache</v>
       </c>
@@ -9497,7 +9512,7 @@
       <c r="AA119">
         <v>118</v>
       </c>
-      <c r="AB119" t="str">
+      <c r="AB119" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Standortcode</v>
       </c>
@@ -9530,7 +9545,7 @@
       <c r="AA120">
         <v>119</v>
       </c>
-      <c r="AB120" t="str">
+      <c r="AB120" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Postleitzahl</v>
       </c>
@@ -9563,7 +9578,7 @@
       <c r="AA121">
         <v>120</v>
       </c>
-      <c r="AB121" t="str">
+      <c r="AB121" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Systemrolle</v>
       </c>
@@ -9608,7 +9623,7 @@
       <c r="AA122">
         <v>121</v>
       </c>
-      <c r="AB122" t="str">
+      <c r="AB122" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Zuordnung Rechte zu einer Rolle</v>
       </c>
@@ -9662,7 +9677,7 @@
       <c r="AA123">
         <v>122</v>
       </c>
-      <c r="AB123" t="str">
+      <c r="AB123" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Stammdaten Tabelle</v>
       </c>
@@ -9710,7 +9725,7 @@
       <c r="AA124">
         <v>123</v>
       </c>
-      <c r="AB124" t="str">
+      <c r="AB124" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Log-Datei Konfiguration</v>
       </c>
@@ -9737,7 +9752,7 @@
       <c r="AA125">
         <v>124</v>
       </c>
-      <c r="AB125" t="str">
+      <c r="AB125" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Site infos with last result</v>
       </c>
@@ -9764,7 +9779,7 @@
       <c r="AA126">
         <v>125</v>
       </c>
-      <c r="AB126" t="str">
+      <c r="AB126" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Wcf infos with last result</v>
       </c>
@@ -9791,7 +9806,7 @@
       <c r="AA127">
         <v>126</v>
       </c>
-      <c r="AB127" t="str">
+      <c r="AB127" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Win service infos with last result</v>
       </c>
@@ -9818,7 +9833,7 @@
       <c r="AA128">
         <v>127</v>
       </c>
-      <c r="AB128" t="str">
+      <c r="AB128" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Job infos with last result</v>
       </c>
@@ -9845,7 +9860,7 @@
       <c r="AA129">
         <v>128</v>
       </c>
-      <c r="AB129" t="str">
+      <c r="AB129" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Wcf Service Status</v>
       </c>
@@ -9872,7 +9887,7 @@
       <c r="AA130">
         <v>129</v>
       </c>
-      <c r="AB130" t="str">
+      <c r="AB130" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Applikation-Logs</v>
       </c>
@@ -9899,7 +9914,7 @@
       <c r="AA131">
         <v>130</v>
       </c>
-      <c r="AB131" t="str">
+      <c r="AB131" s="17" t="str">
         <f t="shared" ref="AB131:AB133" si="2">O131</f>
         <v>Job Status</v>
       </c>
@@ -9926,7 +9941,7 @@
       <c r="AA132">
         <v>131</v>
       </c>
-      <c r="AB132" t="str">
+      <c r="AB132" s="17" t="str">
         <f t="shared" si="2"/>
         <v>Web Seite Status</v>
       </c>
@@ -9953,7 +9968,7 @@
       <c r="AA133">
         <v>132</v>
       </c>
-      <c r="AB133" t="str">
+      <c r="AB133" s="17" t="str">
         <f t="shared" si="2"/>
         <v>Windows Service Status</v>
       </c>

</xml_diff>